<commit_message>
Updated the status overviews for care and cure
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Project\060.37543 NIVZ\Data\Zorginstellingen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\060.37543 NIVZ\Data\Zorginstellingen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67D50C4-1993-4C57-A2B7-236FE1C417B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB646BB-0787-42E7-8014-C21F65C842B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5970" yWindow="3630" windowWidth="26430" windowHeight="16220" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="6040" yWindow="4770" windowWidth="22430" windowHeight="13500" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,285 +34,423 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="93">
-  <si>
-    <t>voorlopig</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="139">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
   <si>
-    <t>Organisatie</t>
-  </si>
-  <si>
-    <t>AC groep</t>
-  </si>
-  <si>
-    <t>ASVZ</t>
-  </si>
-  <si>
-    <t>Attent Zorg Thuis</t>
-  </si>
-  <si>
-    <t>De Zellingen</t>
-  </si>
-  <si>
-    <t>GGZ Delfland</t>
-  </si>
-  <si>
-    <t>HilverZorg</t>
-  </si>
-  <si>
-    <t>Karakter</t>
-  </si>
-  <si>
-    <t>Land van Horne</t>
-  </si>
-  <si>
-    <t>Magentazorg</t>
-  </si>
-  <si>
-    <t>Noord Ned. Coöp. van Zorgorganisaties U.A.</t>
-  </si>
-  <si>
-    <t>PSW</t>
-  </si>
-  <si>
-    <t>STICHTING WOONZORGGROEP SAMEN</t>
-  </si>
-  <si>
-    <t>SZMH</t>
-  </si>
-  <si>
-    <t>St.GGz Breburg Groep/Regio Breda/Midden-Brab.</t>
-  </si>
-  <si>
-    <t>Stichting 's Heeren Loo Zorggroep</t>
-  </si>
-  <si>
-    <t>Stichting ActiVite</t>
-  </si>
-  <si>
-    <t>Stichting Altrecht</t>
-  </si>
-  <si>
-    <t>Stichting Amarant</t>
-  </si>
-  <si>
-    <t>Stichting Amaris Zorggroep</t>
-  </si>
-  <si>
-    <t>Stichting Archipel</t>
-  </si>
-  <si>
-    <t>Stichting Aveleijn</t>
-  </si>
-  <si>
-    <t>Stichting Azora</t>
-  </si>
-  <si>
-    <t>Stichting Baalderborg Groep</t>
-  </si>
-  <si>
-    <t>Stichting Bethanië</t>
-  </si>
-  <si>
-    <t>Stichting Careyn</t>
-  </si>
-  <si>
-    <t>Stichting Cicero Zorggroep</t>
-  </si>
-  <si>
-    <t>Stichting DSV</t>
-  </si>
-  <si>
-    <t>Stichting De Opbouw</t>
-  </si>
-  <si>
-    <t>Stichting De Wever</t>
-  </si>
-  <si>
-    <t>Stichting Dimence Groep</t>
-  </si>
-  <si>
-    <t>Stichting Driestroom</t>
-  </si>
-  <si>
-    <t>Stichting Elver</t>
-  </si>
-  <si>
-    <t>Stichting GGZ inGeest</t>
-  </si>
-  <si>
-    <t>Stichting GGzE</t>
-  </si>
-  <si>
-    <t>Stichting Gehandicaptenzorg</t>
-  </si>
-  <si>
-    <t>Stichting Novadic-Kentron Groep</t>
-  </si>
-  <si>
-    <t>Stichting Omring</t>
-  </si>
-  <si>
-    <t>Stichting Pameijer</t>
-  </si>
-  <si>
-    <t>Stichting Park Zuiderhout</t>
-  </si>
-  <si>
-    <t>Stichting Pergamijn</t>
-  </si>
-  <si>
-    <t>Stichting Pleyade</t>
-  </si>
-  <si>
-    <t>Stichting Pro Senectute (voor de Ouderdom)</t>
-  </si>
-  <si>
-    <t>Stichting Saffier - De Residentie Groep</t>
-  </si>
-  <si>
-    <t>Stichting Salem</t>
-  </si>
-  <si>
-    <t>Stichting Schakelring</t>
-  </si>
-  <si>
-    <t>Stichting Sint Jacob</t>
-  </si>
-  <si>
-    <t>Stichting Siza</t>
-  </si>
-  <si>
-    <t>Stichting Sovak</t>
-  </si>
-  <si>
-    <t>Stichting Tactus Verslavingszorg</t>
-  </si>
-  <si>
-    <t>Stichting ViVa! Zorggroep</t>
-  </si>
-  <si>
-    <t>Stichting Vincent van Gogh</t>
-  </si>
-  <si>
-    <t>Stichting Vitalis WoonZorg Groep</t>
-  </si>
-  <si>
-    <t>Stichting Wijdezorg</t>
-  </si>
-  <si>
-    <t>Stichting Wonen en Zorg Purmerend</t>
-  </si>
-  <si>
-    <t>Stichting Woon-Zorgcentra De Rijnhoven</t>
-  </si>
-  <si>
-    <t>Stichting ZGR</t>
-  </si>
-  <si>
-    <t>Stichting ZorgAccent</t>
-  </si>
-  <si>
-    <t>Stichting Zorgbalans</t>
-  </si>
-  <si>
-    <t>Stichting Zorggroep Apeldoorn en omstreken</t>
-  </si>
-  <si>
-    <t>Stichting Zorggroep Charim</t>
-  </si>
-  <si>
-    <t>Stichting Zorggroep Ena</t>
-  </si>
-  <si>
-    <t>Stichting Zorggroep Liante</t>
-  </si>
-  <si>
-    <t>Stichting Zorggroep Noorderboog</t>
-  </si>
-  <si>
-    <t>Stichting Zorginstellingen Pieter van Foreest</t>
-  </si>
-  <si>
-    <t>Stichting Zorgspectrum</t>
-  </si>
-  <si>
-    <t>Stichting ZuidOostZorg</t>
-  </si>
-  <si>
-    <t>Stichting de Zorgboog</t>
-  </si>
-  <si>
-    <t>Stichting tanteLouise</t>
-  </si>
-  <si>
-    <t>Trajectum</t>
-  </si>
-  <si>
-    <t>Van Neynsel</t>
-  </si>
-  <si>
-    <t>Zorggroep Reinalda</t>
-  </si>
-  <si>
-    <t>stichting Accolade Zorg</t>
-  </si>
-  <si>
-    <t>stichting Pro Persona Holding</t>
-  </si>
-  <si>
-    <t>Ruitersbos</t>
-  </si>
-  <si>
-    <t>Stichting Interzorg Noord-Nederland</t>
-  </si>
-  <si>
-    <t>Stichting de Vogellanden</t>
-  </si>
-  <si>
-    <t>St. Christelijke Zonnehuisgroep IJssel-Vecht</t>
-  </si>
-  <si>
-    <t>Stichting Atlant Zorggroep</t>
-  </si>
-  <si>
-    <t>Stichting Cardia</t>
-  </si>
-  <si>
-    <t>Stichting De Hoogstraat Revalidatie</t>
-  </si>
-  <si>
-    <t>Stichting De Zijlen</t>
-  </si>
-  <si>
-    <t>Stichting GGNet</t>
-  </si>
-  <si>
-    <t>Stichting Kwadrantgroep</t>
-  </si>
-  <si>
-    <t>Stichting Middin</t>
-  </si>
-  <si>
-    <t>Stichting Reade</t>
-  </si>
-  <si>
-    <t>Stichting Verpleeghuis Bergweide</t>
-  </si>
-  <si>
-    <t>Stichting Zorggroep Amsterdam-Oost</t>
-  </si>
-  <si>
-    <t>Stichting Zorggroep Tangenborgh</t>
-  </si>
-  <si>
-    <t>Stichting Zorggroep Tellus</t>
-  </si>
-  <si>
-    <t>Stichting Zorgspectrum Het Zand</t>
+    <t xml:space="preserve">Organisatie </t>
+  </si>
+  <si>
+    <t>Accolade (Stichting)</t>
+  </si>
+  <si>
+    <t>ActiVite (Stichting)</t>
+  </si>
+  <si>
+    <t>Adelante Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Altrecht (Stichting)</t>
+  </si>
+  <si>
+    <t>Amarant Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Amaris Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Archipel (Stichting)</t>
+  </si>
+  <si>
+    <t>ASVZ (Stichting)</t>
+  </si>
+  <si>
+    <t>Atlant Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Attent</t>
+  </si>
+  <si>
+    <t>Aveleijn (Stichting)</t>
+  </si>
+  <si>
+    <t>AxionContinu Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Azora (Stichting)</t>
+  </si>
+  <si>
+    <t>Baalderborg Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Basalt revalidatie</t>
+  </si>
+  <si>
+    <t>Bethanië (Stichting)</t>
+  </si>
+  <si>
+    <t>Bildt (Zorgcentrum het ... Stichting)</t>
+  </si>
+  <si>
+    <t>Cardia (Stichting)</t>
+  </si>
+  <si>
+    <t>Careyn (Stichting)</t>
+  </si>
+  <si>
+    <t>Carinova (Stichting)</t>
+  </si>
+  <si>
+    <t>Charim (Zorggroep ...)</t>
+  </si>
+  <si>
+    <t>Cicero Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>CIRO+ B.V.</t>
+  </si>
+  <si>
+    <t>Combinatie Jeugdzorg</t>
+  </si>
+  <si>
+    <t>Curamare (Stichting)</t>
+  </si>
+  <si>
+    <t>De Zijlen (Stichting)</t>
+  </si>
+  <si>
+    <t>DFZS De Forensische Zorgspecialisten</t>
+  </si>
+  <si>
+    <t>Dimence Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Driegasthuizengroep</t>
+  </si>
+  <si>
+    <t>Driestroom (Stichting)</t>
+  </si>
+  <si>
+    <t>DSV (Stichting)</t>
+  </si>
+  <si>
+    <t>Elver (Stichting)</t>
+  </si>
+  <si>
+    <t>Espria (stichting ...) (met onderdelen Trans, Meander, Evean, GGZ Drenthe, icare)</t>
+  </si>
+  <si>
+    <t>GGNet (Stichting)</t>
+  </si>
+  <si>
+    <t>GGz Breburg Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>GGZ Delfland - Geestelijke Gezondheidszorg Delfland (Stichting)</t>
+  </si>
+  <si>
+    <t>GGZ inGeest (Stichting)</t>
+  </si>
+  <si>
+    <t>GGzE (Stichting) GGz Eindhoven</t>
+  </si>
+  <si>
+    <t>Heliomare (Stichting)</t>
+  </si>
+  <si>
+    <t>Het Laar (Stichting)</t>
+  </si>
+  <si>
+    <t>HilverZorg (Stichting)</t>
+  </si>
+  <si>
+    <t>Hoogstraat Revalidatie (Stichting)</t>
+  </si>
+  <si>
+    <t>Innoforte (Stichting)</t>
+  </si>
+  <si>
+    <t>Interzorg Noord Nederland (Stichting)</t>
+  </si>
+  <si>
+    <t>Karakter (Stichting)</t>
+  </si>
+  <si>
+    <t>Kennemerhart</t>
+  </si>
+  <si>
+    <t>Klein Geluk</t>
+  </si>
+  <si>
+    <t>Koperhorst (Stichting)</t>
+  </si>
+  <si>
+    <t>KwadrantGroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Land van Horne (Stichting voor Verpleeg-, Verzorgings- en Woonfaciliteiten ...)</t>
+  </si>
+  <si>
+    <t>Lentis</t>
+  </si>
+  <si>
+    <t>Levvel (noord holland)</t>
+  </si>
+  <si>
+    <t>Liante (Stichting)</t>
+  </si>
+  <si>
+    <t>Libra Revalidatie &amp; Audiologie (Stichting)</t>
+  </si>
+  <si>
+    <t>Magenta</t>
+  </si>
+  <si>
+    <t>Marente (Stichting)</t>
+  </si>
+  <si>
+    <t>MET-GGZ (Limburg)</t>
+  </si>
+  <si>
+    <t>Middin (Stichting)</t>
+  </si>
+  <si>
+    <t>Mijzo Schakelring/Eikendonk (Stichting) -&gt; fusie Mijzo (met Riethorst + Volckaert)</t>
+  </si>
+  <si>
+    <t>NNCZ (Noord Nederlandse Coöperatie van Zorgorganisaties)</t>
+  </si>
+  <si>
+    <t>Noorderboog (Stichting)</t>
+  </si>
+  <si>
+    <t>Noorderbreedte</t>
+  </si>
+  <si>
+    <t>Novadic-Kentron (Stichting)</t>
+  </si>
+  <si>
+    <t>Omring (Stichting)</t>
+  </si>
+  <si>
+    <t>Opbouw (Stichting)</t>
+  </si>
+  <si>
+    <t>Pameijer (Stichting)</t>
+  </si>
+  <si>
+    <t>Pantein (Stichting)</t>
+  </si>
+  <si>
+    <t>Park Zuiderhout (Stichting)</t>
+  </si>
+  <si>
+    <t>Pergamijn (Stichting)</t>
+  </si>
+  <si>
+    <t>Pieter van Foreest (Stichting)</t>
+  </si>
+  <si>
+    <t>Pleyade (Stichting)</t>
+  </si>
+  <si>
+    <t>Pluryn Hoenderloo Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Pro Persona Holding (Stichting)</t>
+  </si>
+  <si>
+    <t>Pro Senectute (Stichting)</t>
+  </si>
+  <si>
+    <t>Proteion Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>PSW (Stichting)</t>
+  </si>
+  <si>
+    <t>Reade (Stichting)</t>
+  </si>
+  <si>
+    <t>Reinalda (Stichting Zorggroep)</t>
+  </si>
+  <si>
+    <t>Revalidatie Friesland (Stichting)</t>
+  </si>
+  <si>
+    <t>Revant (Stichting)</t>
+  </si>
+  <si>
+    <t>Rijnhoven (Stichting)</t>
+  </si>
+  <si>
+    <t>Rivierduinen</t>
+  </si>
+  <si>
+    <t>Ruitersbos (Stichting)</t>
+  </si>
+  <si>
+    <t>S&amp;L Zorg (Stichting)</t>
+  </si>
+  <si>
+    <t>Saffier - De Residentie (Stichting Zorginstelling ...))</t>
+  </si>
+  <si>
+    <t>Salem Verpleeghuis (Stichting)</t>
+  </si>
+  <si>
+    <t>SEIN Stichting Epilepsie Instellingen Nederland</t>
+  </si>
+  <si>
+    <t>SGL (Stichting)</t>
+  </si>
+  <si>
+    <t>sHeerenLoo Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Sint Jacob (Stichting)</t>
+  </si>
+  <si>
+    <t>Sirjon</t>
+  </si>
+  <si>
+    <t>Siza (Stichting)</t>
+  </si>
+  <si>
+    <t>SOVAK (Stichting)</t>
+  </si>
+  <si>
+    <t>Sterk Huis (voorheen Kompaan en de Bocht)</t>
+  </si>
+  <si>
+    <t>Surplus (Stichting)</t>
+  </si>
+  <si>
+    <t>SWZP = Stichting Wonen en Zorg Purmerend</t>
+  </si>
+  <si>
+    <t>Tactus Verslavingszorg (Stichting)</t>
+  </si>
+  <si>
+    <t>tanteLouise (Stichting)</t>
+  </si>
+  <si>
+    <t>Terwille verslavingszorg (Stichting)</t>
+  </si>
+  <si>
+    <t>Thebe</t>
+  </si>
+  <si>
+    <t>Zonnehuisgroep IJssel-Vecht (ZGIJV)</t>
+  </si>
+  <si>
+    <t>Topaz (Stichting)</t>
+  </si>
+  <si>
+    <t>Trajectum (Stichting)</t>
+  </si>
+  <si>
+    <t>Treant Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Van Neynselstichting (Stichting)</t>
+  </si>
+  <si>
+    <t>Verpleeghuis Bergweide (Stichting)</t>
+  </si>
+  <si>
+    <t>Viersprong (Netherlands institute for personality disorders)</t>
+  </si>
+  <si>
+    <t>Vincent van Gogh (Stichting)</t>
+  </si>
+  <si>
+    <t>Vitalis</t>
+  </si>
+  <si>
+    <t>ViVa! Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Vogellanden, Centrum voor Revalidatie (Stichting)</t>
+  </si>
+  <si>
+    <t>WelThuis BV</t>
+  </si>
+  <si>
+    <t>Wever (Stichting)</t>
+  </si>
+  <si>
+    <t>WIJdezorg (Stichting)</t>
+  </si>
+  <si>
+    <t>WilgaerdenLeekerweide Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Woon en zorgcentrum de Merwelanden, stichting</t>
+  </si>
+  <si>
+    <t>Woonzorg Samen (Stichting)</t>
+  </si>
+  <si>
+    <t>Wulverhorst (hoort bij St. ouderenzorg Oudewater?)</t>
+  </si>
+  <si>
+    <t>Yulius (Stichting)</t>
+  </si>
+  <si>
+    <t>Zellingen (Stichting Zorgbeheer De ...)</t>
+  </si>
+  <si>
+    <t>ZGR (Zorggroep Raalte (Stichting))</t>
+  </si>
+  <si>
+    <t>Zonnehuisgroep Noord (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorgaccent (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorgbalans</t>
+  </si>
+  <si>
+    <t>Zorgboog (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorggroep Amsterdam Oost (ZGAO) (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorggroep Apeldoorn e.o. (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorggroep Ena (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorggroep Tangenborgh (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorggroep Tellus (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorgpartners Midden-Holland (Stichting)</t>
+  </si>
+  <si>
+    <t>ZorgSpectrum (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorgspectrum Het Zand</t>
+  </si>
+  <si>
+    <t>Zozijn Beheer (Stichting)</t>
+  </si>
+  <si>
+    <t>ZuidOostZorg (Stichting)</t>
+  </si>
+  <si>
+    <t>Voorlopig</t>
+  </si>
+  <si>
+    <t>Vastgesteld</t>
   </si>
 </sst>
 </file>
@@ -673,7 +811,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:B136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -685,178 +823,178 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -864,7 +1002,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -872,7 +1010,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -880,7 +1018,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -888,527 +1026,887 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>0</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>97</v>
+      </c>
+      <c r="B97" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>99</v>
+      </c>
+      <c r="B99" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>103</v>
+      </c>
+      <c r="B103" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>109</v>
+      </c>
+      <c r="B109" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>111</v>
+      </c>
+      <c r="B111" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>112</v>
+      </c>
+      <c r="B112" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>113</v>
+      </c>
+      <c r="B113" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>115</v>
+      </c>
+      <c r="B115" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>117</v>
+      </c>
+      <c r="B117" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>119</v>
+      </c>
+      <c r="B119" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>121</v>
+      </c>
+      <c r="B121" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>122</v>
+      </c>
+      <c r="B122" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>123</v>
+      </c>
+      <c r="B123" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>125</v>
+      </c>
+      <c r="B125" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>126</v>
+      </c>
+      <c r="B126" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>127</v>
+      </c>
+      <c r="B127" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>128</v>
+      </c>
+      <c r="B128" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>129</v>
+      </c>
+      <c r="B129" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>130</v>
+      </c>
+      <c r="B130" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>131</v>
+      </c>
+      <c r="B131" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>132</v>
+      </c>
+      <c r="B132" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>133</v>
+      </c>
+      <c r="B133" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>134</v>
+      </c>
+      <c r="B134" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>135</v>
+      </c>
+      <c r="B135" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>136</v>
+      </c>
+      <c r="B136" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated statuses for care (v13)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\060.37543 NIVZ\Data\Zorginstellingen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB646BB-0787-42E7-8014-C21F65C842B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1C684A-6AE4-468F-8FAE-8F1DA0A0457D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="4770" windowWidth="22430" windowHeight="13500" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="1690" yWindow="900" windowWidth="22820" windowHeight="19260" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="142">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -321,9 +321,6 @@
     <t>SOVAK (Stichting)</t>
   </si>
   <si>
-    <t>Sterk Huis (voorheen Kompaan en de Bocht)</t>
-  </si>
-  <si>
     <t>Surplus (Stichting)</t>
   </si>
   <si>
@@ -342,9 +339,6 @@
     <t>Thebe</t>
   </si>
   <si>
-    <t>Zonnehuisgroep IJssel-Vecht (ZGIJV)</t>
-  </si>
-  <si>
     <t>Topaz (Stichting)</t>
   </si>
   <si>
@@ -451,6 +445,21 @@
   </si>
   <si>
     <t>Vastgesteld</t>
+  </si>
+  <si>
+    <t>Leger des Heils Welzijns- en Gezondheidszorg (Stichting)</t>
+  </si>
+  <si>
+    <t>Vilente (Stichting)</t>
+  </si>
+  <si>
+    <t>Sterk Huis West Brabant (voorheen Juzt)</t>
+  </si>
+  <si>
+    <t>Solis (Stichting)</t>
+  </si>
+  <si>
+    <t>Stichting Sterk Huis</t>
   </si>
 </sst>
 </file>
@@ -811,7 +820,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B136"/>
+  <dimension ref="A1:B139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -834,7 +843,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -842,7 +851,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -850,7 +859,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -858,7 +867,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -866,7 +875,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -874,7 +883,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -882,7 +891,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -890,7 +899,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -898,7 +907,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -906,7 +915,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -914,7 +923,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -922,7 +931,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -930,7 +939,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -938,7 +947,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -946,7 +955,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -954,7 +963,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -962,7 +971,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -970,7 +979,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -978,7 +987,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -986,7 +995,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -994,7 +1003,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -1002,7 +1011,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1010,7 +1019,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -1018,7 +1027,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1026,7 +1035,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -1034,7 +1043,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -1042,7 +1051,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -1050,7 +1059,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -1058,7 +1067,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -1066,7 +1075,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -1074,7 +1083,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -1082,7 +1091,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -1090,7 +1099,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -1098,7 +1107,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -1106,7 +1115,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -1114,7 +1123,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -1122,7 +1131,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -1130,7 +1139,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1138,7 +1147,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -1146,7 +1155,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -1154,7 +1163,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -1162,7 +1171,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -1170,7 +1179,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1178,7 +1187,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -1186,7 +1195,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -1194,7 +1203,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -1202,7 +1211,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -1210,7 +1219,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1218,7 +1227,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -1226,687 +1235,711 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="B95" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="B97" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="B98" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B99" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B100" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B101" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B102" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B103" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B104" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B105" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B106" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B107" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B108" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B109" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B110" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="B111" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B112" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B113" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B114" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B115" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B116" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B117" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B118" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B119" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B120" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B121" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B122" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B123" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B124" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B125" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B126" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B127" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B128" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B129" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B130" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B131" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B132" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B133" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B134" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B135" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B136" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>132</v>
+      </c>
+      <c r="B137" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>133</v>
+      </c>
+      <c r="B138" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>134</v>
+      </c>
+      <c r="B139" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the data for care. v18.
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\060.37543 NIVZ\Data\Zorginstellingen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1C684A-6AE4-468F-8FAE-8F1DA0A0457D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EC31A6-7198-4D99-9CEA-404CA927E255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1690" yWindow="900" windowWidth="22820" windowHeight="19260" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="2660" yWindow="730" windowWidth="18350" windowHeight="19640" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="153">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -460,6 +460,39 @@
   </si>
   <si>
     <t>Stichting Sterk Huis</t>
+  </si>
+  <si>
+    <t>Aafje Thuiszorg Huizen Zorghotels (Stichting)</t>
+  </si>
+  <si>
+    <t>BrabantZorg</t>
+  </si>
+  <si>
+    <t>Fundis (Stichting)</t>
+  </si>
+  <si>
+    <t>GGZ Friesland (Stichting)</t>
+  </si>
+  <si>
+    <t>Philadelphia Zorg (Stichting)</t>
+  </si>
+  <si>
+    <t>Pieter Raat Stichting</t>
+  </si>
+  <si>
+    <t>Residentie Molenwijck</t>
+  </si>
+  <si>
+    <t>Sint Anna (Stichting)</t>
+  </si>
+  <si>
+    <t>St. Anna Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Youke</t>
+  </si>
+  <si>
+    <t>Zonnehuisgroep IJssel-Vecht (ZGIJV)</t>
   </si>
 </sst>
 </file>
@@ -820,9 +853,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B139"/>
+  <dimension ref="A1:B150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -840,7 +875,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
         <v>135</v>
@@ -848,7 +883,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>135</v>
@@ -856,7 +891,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>135</v>
@@ -864,7 +899,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>135</v>
@@ -872,7 +907,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>135</v>
@@ -880,7 +915,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>135</v>
@@ -888,23 +923,23 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>135</v>
@@ -912,7 +947,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>135</v>
@@ -920,7 +955,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>135</v>
@@ -928,23 +963,23 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>135</v>
@@ -952,7 +987,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>135</v>
@@ -960,7 +995,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>135</v>
@@ -968,7 +1003,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>135</v>
@@ -976,31 +1011,31 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="B20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>135</v>
@@ -1008,15 +1043,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>135</v>
@@ -1024,15 +1059,15 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>136</v>
@@ -1040,7 +1075,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>135</v>
@@ -1048,15 +1083,15 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>135</v>
@@ -1064,7 +1099,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>135</v>
@@ -1072,7 +1107,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>135</v>
@@ -1080,15 +1115,15 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>135</v>
@@ -1096,15 +1131,15 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>135</v>
@@ -1112,7 +1147,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>135</v>
@@ -1120,15 +1155,15 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>144</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
         <v>135</v>
@@ -1136,7 +1171,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
         <v>135</v>
@@ -1144,7 +1179,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
         <v>135</v>
@@ -1152,15 +1187,15 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
         <v>135</v>
@@ -1168,7 +1203,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B43" t="s">
         <v>135</v>
@@ -1176,7 +1211,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
         <v>135</v>
@@ -1184,15 +1219,15 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
         <v>135</v>
@@ -1200,7 +1235,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
         <v>135</v>
@@ -1208,7 +1243,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
         <v>135</v>
@@ -1216,23 +1251,23 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
         <v>135</v>
@@ -1240,7 +1275,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>137</v>
+        <v>48</v>
       </c>
       <c r="B52" t="s">
         <v>135</v>
@@ -1248,7 +1283,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B53" t="s">
         <v>135</v>
@@ -1256,7 +1291,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B54" t="s">
         <v>135</v>
@@ -1264,7 +1299,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B55" t="s">
         <v>135</v>
@@ -1272,7 +1307,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>137</v>
       </c>
       <c r="B56" t="s">
         <v>135</v>
@@ -1280,15 +1315,15 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B58" t="s">
         <v>135</v>
@@ -1296,7 +1331,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B59" t="s">
         <v>135</v>
@@ -1304,7 +1339,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B60" t="s">
         <v>135</v>
@@ -1312,7 +1347,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B61" t="s">
         <v>135</v>
@@ -1320,23 +1355,23 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B64" t="s">
         <v>135</v>
@@ -1344,7 +1379,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B65" t="s">
         <v>135</v>
@@ -1352,23 +1387,23 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B68" t="s">
         <v>135</v>
@@ -1376,7 +1411,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B69" t="s">
         <v>135</v>
@@ -1384,15 +1419,15 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B70" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B71" t="s">
         <v>135</v>
@@ -1400,7 +1435,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B72" t="s">
         <v>135</v>
@@ -1408,7 +1443,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B73" t="s">
         <v>135</v>
@@ -1416,7 +1451,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B74" t="s">
         <v>135</v>
@@ -1424,7 +1459,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B75" t="s">
         <v>135</v>
@@ -1432,7 +1467,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>146</v>
       </c>
       <c r="B76" t="s">
         <v>135</v>
@@ -1440,7 +1475,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>147</v>
       </c>
       <c r="B77" t="s">
         <v>136</v>
@@ -1448,7 +1483,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B78" t="s">
         <v>135</v>
@@ -1456,7 +1491,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B79" t="s">
         <v>135</v>
@@ -1464,7 +1499,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B80" t="s">
         <v>135</v>
@@ -1472,7 +1507,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B81" t="s">
         <v>135</v>
@@ -1480,7 +1515,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B82" t="s">
         <v>135</v>
@@ -1488,15 +1523,15 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B84" t="s">
         <v>135</v>
@@ -1504,7 +1539,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B85" t="s">
         <v>135</v>
@@ -1512,7 +1547,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B86" t="s">
         <v>135</v>
@@ -1520,7 +1555,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="B87" t="s">
         <v>135</v>
@@ -1528,23 +1563,23 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B88" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B89" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B90" t="s">
         <v>135</v>
@@ -1552,15 +1587,15 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B91" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B92" t="s">
         <v>135</v>
@@ -1568,15 +1603,15 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B93" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B94" t="s">
         <v>135</v>
@@ -1584,23 +1619,23 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="B95" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B96" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="B97" t="s">
         <v>135</v>
@@ -1608,15 +1643,15 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
       <c r="B98" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="B99" t="s">
         <v>136</v>
@@ -1624,31 +1659,31 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B100" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B101" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B102" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="B103" t="s">
         <v>135</v>
@@ -1656,7 +1691,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B104" t="s">
         <v>135</v>
@@ -1664,15 +1699,15 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>101</v>
+        <v>150</v>
       </c>
       <c r="B105" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
       <c r="B106" t="s">
         <v>135</v>
@@ -1680,7 +1715,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="B107" t="s">
         <v>135</v>
@@ -1688,23 +1723,23 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B108" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B109" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B110" t="s">
         <v>135</v>
@@ -1712,15 +1747,15 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="B111" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B112" t="s">
         <v>135</v>
@@ -1728,7 +1763,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B113" t="s">
         <v>135</v>
@@ -1736,7 +1771,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B114" t="s">
         <v>135</v>
@@ -1744,7 +1779,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B115" t="s">
         <v>135</v>
@@ -1752,7 +1787,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B116" t="s">
         <v>135</v>
@@ -1760,7 +1795,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B117" t="s">
         <v>135</v>
@@ -1768,15 +1803,15 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B118" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B119" t="s">
         <v>135</v>
@@ -1784,23 +1819,23 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="B120" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B121" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B122" t="s">
         <v>135</v>
@@ -1808,7 +1843,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B123" t="s">
         <v>135</v>
@@ -1816,15 +1851,15 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B124" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B125" t="s">
         <v>135</v>
@@ -1832,7 +1867,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B126" t="s">
         <v>135</v>
@@ -1840,15 +1875,15 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B127" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B128" t="s">
         <v>135</v>
@@ -1856,15 +1891,15 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B129" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B130" t="s">
         <v>136</v>
@@ -1872,7 +1907,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B131" t="s">
         <v>135</v>
@@ -1880,7 +1915,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="B132" t="s">
         <v>135</v>
@@ -1888,7 +1923,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B133" t="s">
         <v>135</v>
@@ -1896,7 +1931,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B134" t="s">
         <v>135</v>
@@ -1904,7 +1939,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B135" t="s">
         <v>135</v>
@@ -1912,7 +1947,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="B136" t="s">
         <v>135</v>
@@ -1920,7 +1955,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B137" t="s">
         <v>135</v>
@@ -1928,7 +1963,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B138" t="s">
         <v>135</v>
@@ -1936,9 +1971,97 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
+        <v>123</v>
+      </c>
+      <c r="B139" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>124</v>
+      </c>
+      <c r="B140" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>125</v>
+      </c>
+      <c r="B141" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>126</v>
+      </c>
+      <c r="B142" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>127</v>
+      </c>
+      <c r="B143" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>128</v>
+      </c>
+      <c r="B144" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>129</v>
+      </c>
+      <c r="B145" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>130</v>
+      </c>
+      <c r="B146" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>131</v>
+      </c>
+      <c r="B147" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>132</v>
+      </c>
+      <c r="B148" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>133</v>
+      </c>
+      <c r="B149" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
         <v>134</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B150" t="s">
         <v>135</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the data for care. v19.
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\060.37543 NIVZ\Data\Zorginstellingen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EC31A6-7198-4D99-9CEA-404CA927E255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FD7234-8E88-4FC6-9F01-443CE955BCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="730" windowWidth="18350" windowHeight="19640" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="820" yWindow="2690" windowWidth="14790" windowHeight="16110" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -492,7 +487,7 @@
     <t>Youke</t>
   </si>
   <si>
-    <t>Zonnehuisgroep IJssel-Vecht (ZGIJV)</t>
+    <t>De Hoop ggz (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -855,9 +850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
   <dimension ref="A1:B150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1091,7 +1084,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>152</v>
       </c>
       <c r="B29" t="s">
         <v>135</v>
@@ -1099,7 +1092,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
         <v>135</v>
@@ -1107,7 +1100,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
         <v>135</v>
@@ -1115,7 +1108,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
         <v>135</v>
@@ -1123,7 +1116,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
         <v>135</v>
@@ -1131,23 +1124,23 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
         <v>135</v>
@@ -1155,23 +1148,23 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>144</v>
       </c>
       <c r="B38" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
         <v>135</v>
@@ -1179,7 +1172,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>135</v>
@@ -1187,23 +1180,23 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" t="s">
         <v>135</v>
@@ -1211,7 +1204,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B44" t="s">
         <v>135</v>
@@ -1219,7 +1212,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
         <v>135</v>
@@ -1227,7 +1220,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B46" t="s">
         <v>135</v>
@@ -1235,7 +1228,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
         <v>135</v>
@@ -1243,7 +1236,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" t="s">
         <v>135</v>
@@ -1251,15 +1244,15 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50" t="s">
         <v>136</v>
@@ -1267,15 +1260,15 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B52" t="s">
         <v>135</v>
@@ -1283,7 +1276,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B53" t="s">
         <v>135</v>
@@ -1291,7 +1284,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B54" t="s">
         <v>135</v>
@@ -1299,7 +1292,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55" t="s">
         <v>135</v>
@@ -1307,7 +1300,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="B56" t="s">
         <v>135</v>
@@ -1315,23 +1308,23 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="B57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B58" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B59" t="s">
         <v>135</v>
@@ -1339,7 +1332,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B60" t="s">
         <v>135</v>
@@ -1347,7 +1340,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B61" t="s">
         <v>135</v>
@@ -1355,7 +1348,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B62" t="s">
         <v>135</v>
@@ -1363,7 +1356,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B63" t="s">
         <v>135</v>
@@ -1371,7 +1364,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
         <v>135</v>
@@ -1379,7 +1372,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B65" t="s">
         <v>135</v>
@@ -1387,15 +1380,15 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
         <v>136</v>
@@ -1403,15 +1396,15 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B69" t="s">
         <v>135</v>
@@ -1419,23 +1412,23 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B70" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B71" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B72" t="s">
         <v>135</v>
@@ -1443,7 +1436,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B73" t="s">
         <v>135</v>
@@ -1451,7 +1444,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B74" t="s">
         <v>135</v>
@@ -1459,7 +1452,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B75" t="s">
         <v>135</v>
@@ -1467,7 +1460,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>146</v>
+        <v>70</v>
       </c>
       <c r="B76" t="s">
         <v>135</v>
@@ -1475,23 +1468,23 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B77" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>71</v>
+        <v>147</v>
       </c>
       <c r="B78" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B79" t="s">
         <v>135</v>
@@ -1499,7 +1492,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B80" t="s">
         <v>135</v>
@@ -1507,7 +1500,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B81" t="s">
         <v>135</v>
@@ -1515,7 +1508,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B82" t="s">
         <v>135</v>
@@ -1523,23 +1516,23 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B83" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B84" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B85" t="s">
         <v>135</v>
@@ -1547,7 +1540,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B86" t="s">
         <v>135</v>
@@ -1555,7 +1548,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>148</v>
+        <v>79</v>
       </c>
       <c r="B87" t="s">
         <v>135</v>
@@ -1563,7 +1556,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="B88" t="s">
         <v>135</v>
@@ -1571,23 +1564,23 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B89" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B90" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B91" t="s">
         <v>135</v>
@@ -1595,7 +1588,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B92" t="s">
         <v>135</v>
@@ -1603,7 +1596,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B93" t="s">
         <v>135</v>
@@ -1611,7 +1604,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B94" t="s">
         <v>135</v>
@@ -1619,15 +1612,15 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B95" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B96" t="s">
         <v>136</v>
@@ -1635,23 +1628,23 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B97" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B98" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>149</v>
+        <v>90</v>
       </c>
       <c r="B99" t="s">
         <v>136</v>
@@ -1659,31 +1652,31 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>91</v>
+        <v>149</v>
       </c>
       <c r="B100" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B101" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B102" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="B103" t="s">
         <v>135</v>
@@ -1691,7 +1684,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>94</v>
+        <v>140</v>
       </c>
       <c r="B104" t="s">
         <v>135</v>
@@ -1699,23 +1692,23 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="B105" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="B106" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B107" t="s">
         <v>135</v>
@@ -1723,15 +1716,15 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="B108" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B109" t="s">
         <v>136</v>
@@ -1739,31 +1732,31 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B110" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B111" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B112" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B113" t="s">
         <v>135</v>
@@ -1771,7 +1764,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B114" t="s">
         <v>135</v>
@@ -1779,7 +1772,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B115" t="s">
         <v>135</v>
@@ -1787,7 +1780,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B116" t="s">
         <v>135</v>
@@ -1795,7 +1788,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B117" t="s">
         <v>135</v>
@@ -1803,7 +1796,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B118" t="s">
         <v>135</v>
@@ -1811,7 +1804,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B119" t="s">
         <v>135</v>
@@ -1819,7 +1812,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="B120" t="s">
         <v>135</v>
@@ -1827,7 +1820,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="B121" t="s">
         <v>135</v>
@@ -1835,7 +1828,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B122" t="s">
         <v>135</v>
@@ -1843,7 +1836,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B123" t="s">
         <v>135</v>
@@ -1851,23 +1844,23 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B124" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B125" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B126" t="s">
         <v>135</v>
@@ -1875,31 +1868,31 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B127" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B128" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B129" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B130" t="s">
         <v>136</v>
@@ -1907,15 +1900,15 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B131" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="B132" t="s">
         <v>135</v>
@@ -1923,7 +1916,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="B133" t="s">
         <v>135</v>
@@ -1931,7 +1924,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B134" t="s">
         <v>135</v>
@@ -1939,7 +1932,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B135" t="s">
         <v>135</v>
@@ -1947,7 +1940,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="B136" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
Updated the data for care (v20)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FD7234-8E88-4FC6-9F01-443CE955BCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAA869F-6453-45A3-BF72-4FC5504C9B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="2690" windowWidth="14790" windowHeight="16110" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="15710" yWindow="2450" windowWidth="14950" windowHeight="15590" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="159">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Cicero Zorggroep (Stichting)</t>
   </si>
   <si>
-    <t>CIRO+ B.V.</t>
-  </si>
-  <si>
     <t>Combinatie Jeugdzorg</t>
   </si>
   <si>
@@ -265,15 +262,9 @@
     <t>PSW (Stichting)</t>
   </si>
   <si>
-    <t>Reade (Stichting)</t>
-  </si>
-  <si>
     <t>Reinalda (Stichting Zorggroep)</t>
   </si>
   <si>
-    <t>Revalidatie Friesland (Stichting)</t>
-  </si>
-  <si>
     <t>Revant (Stichting)</t>
   </si>
   <si>
@@ -481,13 +472,40 @@
     <t>Sint Anna (Stichting)</t>
   </si>
   <si>
-    <t>St. Anna Zorggroep (Stichting)</t>
-  </si>
-  <si>
     <t>Youke</t>
   </si>
   <si>
     <t>De Hoop ggz (Stichting)</t>
+  </si>
+  <si>
+    <t>Dichterbij (Stichting)</t>
+  </si>
+  <si>
+    <t>GGz Centraal (Stichting)</t>
+  </si>
+  <si>
+    <t>Mediant, Stichting voor Geestelijke Gezondheidszorg Oost- en Midden Twente</t>
+  </si>
+  <si>
+    <t>Mondriaan (Stichting)</t>
+  </si>
+  <si>
+    <t>QuaRijn (Stichting)</t>
+  </si>
+  <si>
+    <t>R.K. Zorgcentrum Roomburgh (Stichting)</t>
+  </si>
+  <si>
+    <t>Savant, Organisatie voor Zorg (Stichting)</t>
+  </si>
+  <si>
+    <t>Severinusstichting</t>
+  </si>
+  <si>
+    <t>Woonzorgcentrum Raffy (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorgfederatie Oldenzaal (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -848,7 +866,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B150"/>
+  <dimension ref="A1:B156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -868,10 +886,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -879,7 +897,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -887,7 +905,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -895,7 +913,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -903,7 +921,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -911,7 +929,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -919,7 +937,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -927,7 +945,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -935,7 +953,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -943,7 +961,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -951,7 +969,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -959,7 +977,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -967,7 +985,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -975,7 +993,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -983,7 +1001,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -991,7 +1009,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -999,7 +1017,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -1007,15 +1025,15 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -1023,7 +1041,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -1031,7 +1049,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -1039,7 +1057,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1047,7 +1065,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -1055,7 +1073,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1063,7 +1081,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -1071,23 +1089,23 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>148</v>
       </c>
       <c r="B28" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -1095,967 +1113,1015 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>149</v>
       </c>
       <c r="B31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B38" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>150</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>142</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B53" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B54" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B56" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>137</v>
+        <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B59" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B60" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B61" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B62" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="B65" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>152</v>
       </c>
       <c r="B69" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B70" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B71" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B72" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B73" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B74" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B75" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B76" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>146</v>
+        <v>67</v>
       </c>
       <c r="B77" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>68</v>
       </c>
       <c r="B78" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B79" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="B80" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>73</v>
+        <v>144</v>
       </c>
       <c r="B81" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B82" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B83" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B84" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B85" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B86" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B87" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>148</v>
+        <v>76</v>
       </c>
       <c r="B88" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>80</v>
+        <v>153</v>
       </c>
       <c r="B89" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="B90" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B91" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>83</v>
+        <v>145</v>
       </c>
       <c r="B92" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B93" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B94" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B95" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B96" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B97" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B98" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B99" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B100" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B101" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="B102" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B103" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="B104" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="B105" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>150</v>
+        <v>88</v>
       </c>
       <c r="B106" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="B107" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
       <c r="B108" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="B109" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B110" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
       <c r="B111" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="B112" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B113" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B114" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B115" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B116" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B117" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B118" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B119" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B120" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="B121" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B122" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B123" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B124" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="B125" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B126" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B127" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B128" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B129" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B130" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B131" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B132" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="B133" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B134" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B135" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="B136" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B137" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="B138" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B139" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B140" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B141" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B142" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B143" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B144" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B145" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="B146" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B147" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B148" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B149" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B150" t="s">
-        <v>135</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>126</v>
+      </c>
+      <c r="B151" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>127</v>
+      </c>
+      <c r="B152" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>128</v>
+      </c>
+      <c r="B153" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>129</v>
+      </c>
+      <c r="B154" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>130</v>
+      </c>
+      <c r="B155" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>131</v>
+      </c>
+      <c r="B156" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data for care (v22)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CE6A23-243D-4BD0-B5F9-99C4BC7EB186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A830D3EA-8A22-4C26-A790-0C31DBEDFEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="255" windowWidth="20580" windowHeight="14340" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="1780" yWindow="3060" windowWidth="16500" windowHeight="14900" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="163">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -448,9 +448,6 @@
     <t>BrabantZorg</t>
   </si>
   <si>
-    <t>Fundis (Stichting)</t>
-  </si>
-  <si>
     <t>GGZ Friesland (Stichting)</t>
   </si>
   <si>
@@ -515,6 +512,12 @@
   </si>
   <si>
     <t>Wulverhorst</t>
+  </si>
+  <si>
+    <t>Fundis (Stichting) (onderdeel van Welthuis)</t>
+  </si>
+  <si>
+    <t>sHeerenLoo Zorggroep (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -879,13 +882,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -893,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -901,15 +904,15 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -917,7 +920,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -925,7 +928,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -933,15 +936,15 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -949,23 +952,23 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -973,7 +976,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -981,7 +984,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -989,31 +992,31 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1021,7 +1024,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1029,31 +1032,31 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>138</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1061,15 +1064,15 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1085,79 +1088,79 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B28" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1165,7 +1168,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1173,23 +1176,23 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1197,23 +1200,23 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -1221,15 +1224,15 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B43" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -1237,23 +1240,23 @@
         <v>130</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>38</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -1269,7 +1272,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>40</v>
       </c>
@@ -1277,7 +1280,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>41</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -1301,15 +1304,15 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>44</v>
       </c>
       <c r="B53" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>45</v>
       </c>
@@ -1317,15 +1320,15 @@
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>46</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -1333,7 +1336,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>49</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>50</v>
       </c>
@@ -1357,7 +1360,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>132</v>
       </c>
@@ -1365,23 +1368,23 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>51</v>
       </c>
       <c r="B61" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>52</v>
       </c>
       <c r="B62" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>53</v>
       </c>
@@ -1389,7 +1392,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>54</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -1405,7 +1408,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>56</v>
       </c>
@@ -1413,15 +1416,15 @@
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B67" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>57</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>58</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>59</v>
       </c>
@@ -1445,15 +1448,15 @@
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B71" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>60</v>
       </c>
@@ -1461,7 +1464,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>61</v>
       </c>
@@ -1469,15 +1472,15 @@
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>62</v>
       </c>
       <c r="B74" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>63</v>
       </c>
@@ -1485,23 +1488,23 @@
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>64</v>
       </c>
       <c r="B76" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>65</v>
       </c>
       <c r="B77" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>66</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>67</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>68</v>
       </c>
@@ -1525,7 +1528,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>69</v>
       </c>
@@ -1533,31 +1536,31 @@
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>140</v>
+      </c>
+      <c r="B82" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>141</v>
       </c>
-      <c r="B82" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>142</v>
-      </c>
       <c r="B83" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>70</v>
       </c>
       <c r="B84" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>71</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>72</v>
       </c>
@@ -1573,7 +1576,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>73</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>74</v>
       </c>
@@ -1589,39 +1592,39 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>75</v>
       </c>
       <c r="B89" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>76</v>
       </c>
       <c r="B90" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
+        <v>150</v>
+      </c>
+      <c r="B91" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>151</v>
       </c>
-      <c r="B91" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>152</v>
-      </c>
       <c r="B92" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>77</v>
       </c>
@@ -1629,39 +1632,39 @@
         <v>130</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B94" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B95" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>78</v>
       </c>
       <c r="B96" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>79</v>
       </c>
       <c r="B97" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>80</v>
       </c>
@@ -1669,7 +1672,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>81</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>82</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>83</v>
       </c>
@@ -1693,23 +1696,23 @@
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>84</v>
       </c>
       <c r="B102" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B103" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>85</v>
       </c>
@@ -1717,15 +1720,15 @@
         <v>131</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B105" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>86</v>
       </c>
@@ -1733,431 +1736,434 @@
         <v>130</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
+        <v>162</v>
+      </c>
+      <c r="B107" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>143</v>
+      </c>
+      <c r="B108" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>87</v>
+      </c>
+      <c r="B109" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>88</v>
+      </c>
+      <c r="B110" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>89</v>
+      </c>
+      <c r="B111" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>135</v>
+      </c>
+      <c r="B112" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>90</v>
+      </c>
+      <c r="B113" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>134</v>
+      </c>
+      <c r="B114" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>136</v>
+      </c>
+      <c r="B115" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>91</v>
+      </c>
+      <c r="B116" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>92</v>
+      </c>
+      <c r="B117" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>93</v>
+      </c>
+      <c r="B118" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>94</v>
+      </c>
+      <c r="B119" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>95</v>
+      </c>
+      <c r="B120" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>96</v>
+      </c>
+      <c r="B121" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>97</v>
+      </c>
+      <c r="B122" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>98</v>
+      </c>
+      <c r="B123" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>99</v>
+      </c>
+      <c r="B124" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>100</v>
+      </c>
+      <c r="B125" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>101</v>
+      </c>
+      <c r="B126" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>102</v>
+      </c>
+      <c r="B127" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>133</v>
+      </c>
+      <c r="B128" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>103</v>
+      </c>
+      <c r="B129" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>104</v>
+      </c>
+      <c r="B130" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>105</v>
+      </c>
+      <c r="B131" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>106</v>
+      </c>
+      <c r="B132" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>107</v>
+      </c>
+      <c r="B133" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>159</v>
+      </c>
+      <c r="B134" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>108</v>
+      </c>
+      <c r="B135" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>109</v>
+      </c>
+      <c r="B136" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>110</v>
+      </c>
+      <c r="B137" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>111</v>
+      </c>
+      <c r="B138" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>112</v>
+      </c>
+      <c r="B139" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>154</v>
+      </c>
+      <c r="B140" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>160</v>
+      </c>
+      <c r="B141" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>144</v>
       </c>
-      <c r="B107" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>87</v>
-      </c>
-      <c r="B108" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>88</v>
-      </c>
-      <c r="B109" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>89</v>
-      </c>
-      <c r="B110" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>135</v>
-      </c>
-      <c r="B111" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>90</v>
-      </c>
-      <c r="B112" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>134</v>
-      </c>
-      <c r="B113" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>136</v>
-      </c>
-      <c r="B114" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>91</v>
-      </c>
-      <c r="B115" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>92</v>
-      </c>
-      <c r="B116" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>93</v>
-      </c>
-      <c r="B117" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>94</v>
-      </c>
-      <c r="B118" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>95</v>
-      </c>
-      <c r="B119" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>96</v>
-      </c>
-      <c r="B120" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>97</v>
-      </c>
-      <c r="B121" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>98</v>
-      </c>
-      <c r="B122" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>99</v>
-      </c>
-      <c r="B123" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>100</v>
-      </c>
-      <c r="B124" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>101</v>
-      </c>
-      <c r="B125" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>102</v>
-      </c>
-      <c r="B126" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>133</v>
-      </c>
-      <c r="B127" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>103</v>
-      </c>
-      <c r="B128" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>104</v>
-      </c>
-      <c r="B129" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>105</v>
-      </c>
-      <c r="B130" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>106</v>
-      </c>
-      <c r="B131" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>107</v>
-      </c>
-      <c r="B132" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>160</v>
-      </c>
-      <c r="B133" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>108</v>
-      </c>
-      <c r="B134" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>109</v>
-      </c>
-      <c r="B135" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>110</v>
-      </c>
-      <c r="B136" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>111</v>
-      </c>
-      <c r="B137" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>112</v>
-      </c>
-      <c r="B138" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="B142" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>113</v>
+      </c>
+      <c r="B143" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>114</v>
+      </c>
+      <c r="B144" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>115</v>
+      </c>
+      <c r="B145" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>116</v>
+      </c>
+      <c r="B146" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>117</v>
+      </c>
+      <c r="B147" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>118</v>
+      </c>
+      <c r="B148" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>119</v>
+      </c>
+      <c r="B149" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
         <v>155</v>
       </c>
-      <c r="B139" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>161</v>
-      </c>
-      <c r="B140" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>145</v>
-      </c>
-      <c r="B141" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>113</v>
-      </c>
-      <c r="B142" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>114</v>
-      </c>
-      <c r="B143" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>115</v>
-      </c>
-      <c r="B144" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>116</v>
-      </c>
-      <c r="B145" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>117</v>
-      </c>
-      <c r="B146" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>118</v>
-      </c>
-      <c r="B147" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>119</v>
-      </c>
-      <c r="B148" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>156</v>
-      </c>
-      <c r="B149" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="B150" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
         <v>120</v>
       </c>
-      <c r="B150" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="B151" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
         <v>121</v>
       </c>
-      <c r="B151" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="B152" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
         <v>122</v>
       </c>
-      <c r="B152" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="B153" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
         <v>123</v>
       </c>
-      <c r="B153" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+      <c r="B154" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
         <v>124</v>
       </c>
-      <c r="B154" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+      <c r="B155" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
         <v>125</v>
       </c>
-      <c r="B155" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+      <c r="B156" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
         <v>126</v>
       </c>
-      <c r="B156" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+      <c r="B157" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
         <v>127</v>
       </c>
-      <c r="B157" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+      <c r="B158" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
         <v>128</v>
       </c>
-      <c r="B158" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="B159" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
         <v>129</v>
       </c>
-      <c r="B159" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>130</v>
       </c>

</xml_diff>

<commit_message>
Updated data for care (v24)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A830D3EA-8A22-4C26-A790-0C31DBEDFEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C97E7F-647F-4B86-AD99-460FD16F68FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="3060" windowWidth="16500" windowHeight="14900" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="3210" yWindow="4040" windowWidth="18890" windowHeight="15290" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="166">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -250,9 +250,6 @@
     <t>Pluryn Hoenderloo Groep (Stichting)</t>
   </si>
   <si>
-    <t>Pro Persona Holding (Stichting)</t>
-  </si>
-  <si>
     <t>Pro Senectute (Stichting)</t>
   </si>
   <si>
@@ -448,9 +445,6 @@
     <t>BrabantZorg</t>
   </si>
   <si>
-    <t>GGZ Friesland (Stichting)</t>
-  </si>
-  <si>
     <t>Philadelphia Zorg (Stichting)</t>
   </si>
   <si>
@@ -460,9 +454,6 @@
     <t>Residentie Molenwijck</t>
   </si>
   <si>
-    <t>Sint Anna (Stichting)</t>
-  </si>
-  <si>
     <t>Youke</t>
   </si>
   <si>
@@ -518,6 +509,24 @@
   </si>
   <si>
     <t>sHeerenLoo Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Arkin (Stichting)</t>
+  </si>
+  <si>
+    <t>Cordaan Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>GGZ Friesland</t>
+  </si>
+  <si>
+    <t>Het Gasthuis (Sint Jan De Deo) (Stichting)</t>
+  </si>
+  <si>
+    <t>Sint Anna Boxmeer (Stichting)</t>
+  </si>
+  <si>
+    <t>Vecht &amp; Ijssel (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -878,7 +887,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B160"/>
+  <dimension ref="A1:B163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -898,10 +907,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -909,7 +918,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -917,7 +926,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -925,7 +934,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -933,7 +942,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -941,7 +950,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -949,7 +958,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -957,60 +966,60 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>160</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
         <v>130</v>
@@ -1018,31 +1027,31 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>130</v>
@@ -1050,23 +1059,23 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
         <v>130</v>
@@ -1074,31 +1083,31 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
         <v>130</v>
@@ -1106,55 +1115,55 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>146</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
         <v>130</v>
@@ -1162,7 +1171,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
         <v>130</v>
@@ -1170,31 +1179,31 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
         <v>130</v>
@@ -1202,23 +1211,23 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>161</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>158</v>
       </c>
       <c r="B42" t="s">
         <v>130</v>
@@ -1226,15 +1235,15 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>147</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B44" t="s">
         <v>130</v>
@@ -1242,23 +1251,23 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="B47" t="s">
         <v>130</v>
@@ -1266,71 +1275,71 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>163</v>
       </c>
       <c r="B51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B54" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B56" t="s">
         <v>130</v>
@@ -1338,7 +1347,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B57" t="s">
         <v>130</v>
@@ -1346,55 +1355,55 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>132</v>
+        <v>48</v>
       </c>
       <c r="B60" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B62" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>53</v>
+        <v>131</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B64" t="s">
         <v>130</v>
@@ -1402,79 +1411,79 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B65" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B66" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="B67" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B68" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>59</v>
+        <v>145</v>
       </c>
       <c r="B70" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>149</v>
+        <v>57</v>
       </c>
       <c r="B71" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B72" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B73" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
       <c r="B74" t="s">
         <v>130</v>
@@ -1482,7 +1491,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B75" t="s">
         <v>130</v>
@@ -1490,31 +1499,31 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B76" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B78" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B79" t="s">
         <v>130</v>
@@ -1522,55 +1531,55 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B80" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B81" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
       <c r="B82" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>141</v>
+        <v>68</v>
       </c>
       <c r="B83" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B84" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="B85" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="B86" t="s">
         <v>130</v>
@@ -1578,39 +1587,39 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B87" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B88" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B89" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B90" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>150</v>
+        <v>74</v>
       </c>
       <c r="B91" t="s">
         <v>130</v>
@@ -1618,23 +1627,23 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>151</v>
+        <v>75</v>
       </c>
       <c r="B92" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="B93" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B94" t="s">
         <v>130</v>
@@ -1642,31 +1651,31 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>158</v>
+        <v>76</v>
       </c>
       <c r="B95" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="B96" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>79</v>
+        <v>155</v>
       </c>
       <c r="B97" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B98" t="s">
         <v>130</v>
@@ -1674,55 +1683,55 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B99" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B100" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B101" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B102" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
       <c r="B103" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B104" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B105" t="s">
         <v>130</v>
@@ -1730,7 +1739,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B106" t="s">
         <v>130</v>
@@ -1738,23 +1747,23 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B107" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="B108" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>87</v>
+        <v>159</v>
       </c>
       <c r="B109" t="s">
         <v>130</v>
@@ -1762,23 +1771,23 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>88</v>
+        <v>164</v>
       </c>
       <c r="B110" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B111" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="B112" t="s">
         <v>130</v>
@@ -1786,10 +1795,10 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B113" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
@@ -1797,12 +1806,12 @@
         <v>134</v>
       </c>
       <c r="B114" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
       <c r="B115" t="s">
         <v>130</v>
@@ -1810,23 +1819,23 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>91</v>
+        <v>133</v>
       </c>
       <c r="B116" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="B117" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B118" t="s">
         <v>130</v>
@@ -1834,23 +1843,23 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B119" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B120" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B121" t="s">
         <v>130</v>
@@ -1858,79 +1867,79 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B122" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B123" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B124" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B125" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B126" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B127" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="B128" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B129" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B130" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="B131" t="s">
         <v>130</v>
@@ -1938,31 +1947,31 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B132" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B133" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>159</v>
+        <v>104</v>
       </c>
       <c r="B134" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B135" t="s">
         <v>130</v>
@@ -1970,47 +1979,47 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B136" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>110</v>
+        <v>156</v>
       </c>
       <c r="B137" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B138" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B139" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>154</v>
+        <v>109</v>
       </c>
       <c r="B140" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="B141" t="s">
         <v>130</v>
@@ -2018,7 +2027,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="B142" t="s">
         <v>130</v>
@@ -2026,79 +2035,79 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="B143" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>114</v>
+        <v>157</v>
       </c>
       <c r="B144" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="B145" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B146" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B147" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B148" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B149" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="B150" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B151" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B152" t="s">
         <v>130</v>
@@ -2106,7 +2115,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="B153" t="s">
         <v>130</v>
@@ -2114,7 +2123,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B154" t="s">
         <v>130</v>
@@ -2122,50 +2131,74 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B155" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B156" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B157" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B158" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B159" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B160" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>126</v>
+      </c>
+      <c r="B161" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>127</v>
+      </c>
+      <c r="B162" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>128</v>
+      </c>
+      <c r="B163" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated care data (v25)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C97E7F-647F-4B86-AD99-460FD16F68FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC568BFB-7DE6-433B-8024-153AC6034BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="4040" windowWidth="18890" windowHeight="15290" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="18070" yWindow="810" windowWidth="16120" windowHeight="18880" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,9 +505,6 @@
     <t>Wulverhorst</t>
   </si>
   <si>
-    <t>Fundis (Stichting) (onderdeel van Welthuis)</t>
-  </si>
-  <si>
     <t>sHeerenLoo Zorggroep (Stichting)</t>
   </si>
   <si>
@@ -527,6 +524,9 @@
   </si>
   <si>
     <t>Vecht &amp; Ijssel (Stichting)</t>
+  </si>
+  <si>
+    <t>Beweging 3.0 (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -971,7 +971,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s">
         <v>129</v>
@@ -1059,23 +1059,23 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="B23" t="s">
         <v>130</v>
@@ -1083,15 +1083,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
         <v>129</v>
@@ -1099,7 +1099,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>129</v>
@@ -1107,23 +1107,23 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
         <v>129</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B30" t="s">
         <v>129</v>
@@ -1139,31 +1139,31 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>154</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>142</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>142</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
         <v>130</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>143</v>
+        <v>27</v>
       </c>
       <c r="B35" t="s">
         <v>130</v>
@@ -1179,15 +1179,15 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
         <v>129</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
         <v>129</v>
@@ -1203,23 +1203,23 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B41" t="s">
         <v>129</v>
@@ -1227,10 +1227,10 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>158</v>
+        <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -1262,12 +1262,12 @@
         <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B47" t="s">
         <v>130</v>
@@ -1299,10 +1299,10 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B51" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -1398,7 +1398,7 @@
         <v>131</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -1763,7 +1763,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B109" t="s">
         <v>130</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B110" t="s">
         <v>130</v>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B128" t="s">
         <v>129</v>
@@ -1982,7 +1982,7 @@
         <v>106</v>
       </c>
       <c r="B136" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated care data (v26)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC568BFB-7DE6-433B-8024-153AC6034BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31430F84-B594-4D40-98CD-B6B76A94FAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18070" yWindow="810" windowWidth="16120" windowHeight="18880" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="10580" yWindow="3220" windowWidth="26240" windowHeight="17500" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="174">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -259,9 +259,6 @@
     <t>PSW (Stichting)</t>
   </si>
   <si>
-    <t>Reinalda (Stichting Zorggroep)</t>
-  </si>
-  <si>
     <t>Revant (Stichting)</t>
   </si>
   <si>
@@ -271,9 +268,6 @@
     <t>Rivierduinen</t>
   </si>
   <si>
-    <t>Ruitersbos (Stichting)</t>
-  </si>
-  <si>
     <t>S&amp;L Zorg (Stichting)</t>
   </si>
   <si>
@@ -325,9 +319,6 @@
     <t>Trajectum (Stichting)</t>
   </si>
   <si>
-    <t>Treant Zorggroep (Stichting)</t>
-  </si>
-  <si>
     <t>Van Neynselstichting (Stichting)</t>
   </si>
   <si>
@@ -508,9 +499,6 @@
     <t>sHeerenLoo Zorggroep (Stichting)</t>
   </si>
   <si>
-    <t>Arkin (Stichting)</t>
-  </si>
-  <si>
     <t>Cordaan Groep (Stichting)</t>
   </si>
   <si>
@@ -527,6 +515,42 @@
   </si>
   <si>
     <t>Beweging 3.0 (Stichting)</t>
+  </si>
+  <si>
+    <t>Amaliazorg (Stichting)</t>
+  </si>
+  <si>
+    <t>Kalorama (Stichting)</t>
+  </si>
+  <si>
+    <t>Lister (Stichting)</t>
+  </si>
+  <si>
+    <t>Parnassia Groep B.V. afdeling Vastgoed en Facilitair</t>
+  </si>
+  <si>
+    <t>Pento (Stichting)</t>
+  </si>
+  <si>
+    <t>Pro Persona</t>
+  </si>
+  <si>
+    <t>Reade</t>
+  </si>
+  <si>
+    <t>Reinalda (Stichting Zorggroep, nu onder Kennemerhart)</t>
+  </si>
+  <si>
+    <t>Revalidatie Friesland</t>
+  </si>
+  <si>
+    <t>Ruitersbos (Stichting, valt nu onder Thebe)</t>
+  </si>
+  <si>
+    <t>Warande (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorggroep Groningen (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -887,7 +911,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B163"/>
+  <dimension ref="A1:B171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -907,10 +931,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -918,7 +942,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -926,7 +950,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -934,7 +958,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -942,39 +966,39 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>162</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -982,7 +1006,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -990,7 +1014,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -998,7 +1022,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -1006,15 +1030,15 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -1022,7 +1046,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1030,7 +1054,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -1038,7 +1062,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -1046,7 +1070,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1054,15 +1078,15 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -1070,15 +1094,15 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1086,7 +1110,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -1094,7 +1118,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1102,7 +1126,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -1110,7 +1134,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -1118,7 +1142,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -1126,23 +1150,23 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B31" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -1150,15 +1174,15 @@
         <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -1166,7 +1190,7 @@
         <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -1174,15 +1198,15 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B36" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -1190,7 +1214,7 @@
         <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -1198,7 +1222,7 @@
         <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -1206,7 +1230,7 @@
         <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1214,7 +1238,7 @@
         <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -1222,7 +1246,7 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -1230,7 +1254,7 @@
         <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -1238,7 +1262,7 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -1246,15 +1270,15 @@
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -1262,15 +1286,15 @@
         <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B47" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -1278,7 +1302,7 @@
         <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -1286,7 +1310,7 @@
         <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1294,15 +1318,15 @@
         <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B51" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -1310,7 +1334,7 @@
         <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -1318,7 +1342,7 @@
         <v>41</v>
       </c>
       <c r="B53" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -1326,7 +1350,7 @@
         <v>42</v>
       </c>
       <c r="B54" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -1334,7 +1358,7 @@
         <v>43</v>
       </c>
       <c r="B55" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -1342,863 +1366,927 @@
         <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="B57" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B58" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B59" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B60" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B61" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>131</v>
+        <v>50</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B66" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B67" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>56</v>
+        <v>164</v>
       </c>
       <c r="B69" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="B70" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B71" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>58</v>
+        <v>142</v>
       </c>
       <c r="B72" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B73" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>146</v>
+        <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B75" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>61</v>
+        <v>143</v>
       </c>
       <c r="B76" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B77" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B78" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B79" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B80" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B81" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B82" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B83" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B84" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="B85" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="B86" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>70</v>
+        <v>166</v>
       </c>
       <c r="B87" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B88" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="B89" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
       <c r="B90" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B91" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B92" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>147</v>
+        <v>72</v>
       </c>
       <c r="B93" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="B94" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B95" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>140</v>
+        <v>74</v>
       </c>
       <c r="B96" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>155</v>
+        <v>75</v>
       </c>
       <c r="B97" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
       <c r="B98" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="B99" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>79</v>
+        <v>168</v>
       </c>
       <c r="B100" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>80</v>
+        <v>169</v>
       </c>
       <c r="B101" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="B102" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="B103" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
       <c r="B104" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>149</v>
+        <v>76</v>
       </c>
       <c r="B105" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B106" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>150</v>
+        <v>78</v>
       </c>
       <c r="B107" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>85</v>
+        <v>171</v>
       </c>
       <c r="B108" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>158</v>
+        <v>79</v>
       </c>
       <c r="B109" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>163</v>
+        <v>80</v>
       </c>
       <c r="B110" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B111" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="B112" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B113" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="B114" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B115" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="B116" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="B117" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B118" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B119" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B120" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="B121" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B122" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="B123" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="B124" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B125" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B126" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B127" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>164</v>
+        <v>91</v>
       </c>
       <c r="B128" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B129" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B130" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="B131" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B132" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B133" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>104</v>
+        <v>160</v>
       </c>
       <c r="B134" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B135" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B136" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="B137" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B138" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B139" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B140" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B141" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>111</v>
+        <v>172</v>
       </c>
       <c r="B142" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="B143" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B144" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="B145" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B146" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B147" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B148" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B149" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="B151" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="B152" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="B153" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B154" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B155" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B156" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B157" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B158" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B159" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="B160" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B161" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B162" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B163" t="s">
-        <v>129</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>173</v>
+      </c>
+      <c r="B164" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>119</v>
+      </c>
+      <c r="B165" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>120</v>
+      </c>
+      <c r="B166" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>121</v>
+      </c>
+      <c r="B167" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>122</v>
+      </c>
+      <c r="B168" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>123</v>
+      </c>
+      <c r="B169" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>124</v>
+      </c>
+      <c r="B170" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>125</v>
+      </c>
+      <c r="B171" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated care data (v27)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31430F84-B594-4D40-98CD-B6B76A94FAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C87B87-0F70-4C03-9FF1-A113DC8AB122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10580" yWindow="3220" windowWidth="26240" windowHeight="17500" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="16000" yWindow="2030" windowWidth="18380" windowHeight="13930" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="194">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Bethanië (Stichting)</t>
   </si>
   <si>
-    <t>Bildt (Zorgcentrum het ... Stichting)</t>
-  </si>
-  <si>
     <t>Cardia (Stichting)</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>Carinova (Stichting)</t>
   </si>
   <si>
-    <t>Charim (Zorggroep ...)</t>
-  </si>
-  <si>
     <t>Cicero Zorggroep (Stichting)</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>Curamare (Stichting)</t>
   </si>
   <si>
-    <t>De Zijlen (Stichting)</t>
-  </si>
-  <si>
     <t>DFZS De Forensische Zorgspecialisten</t>
   </si>
   <si>
@@ -184,9 +175,6 @@
     <t>Land van Horne (Stichting voor Verpleeg-, Verzorgings- en Woonfaciliteiten ...)</t>
   </si>
   <si>
-    <t>Lentis</t>
-  </si>
-  <si>
     <t>Levvel (noord holland)</t>
   </si>
   <si>
@@ -226,9 +214,6 @@
     <t>Omring (Stichting)</t>
   </si>
   <si>
-    <t>Opbouw (Stichting)</t>
-  </si>
-  <si>
     <t>Pameijer (Stichting)</t>
   </si>
   <si>
@@ -286,21 +271,12 @@
     <t>Sint Jacob (Stichting)</t>
   </si>
   <si>
-    <t>Sirjon</t>
-  </si>
-  <si>
     <t>Siza (Stichting)</t>
   </si>
   <si>
     <t>SOVAK (Stichting)</t>
   </si>
   <si>
-    <t>Surplus (Stichting)</t>
-  </si>
-  <si>
-    <t>SWZP = Stichting Wonen en Zorg Purmerend</t>
-  </si>
-  <si>
     <t>Tactus Verslavingszorg (Stichting)</t>
   </si>
   <si>
@@ -310,9 +286,6 @@
     <t>Terwille verslavingszorg (Stichting)</t>
   </si>
   <si>
-    <t>Thebe</t>
-  </si>
-  <si>
     <t>Topaz (Stichting)</t>
   </si>
   <si>
@@ -382,9 +355,6 @@
     <t>Zorggroep Amsterdam Oost (ZGAO) (Stichting)</t>
   </si>
   <si>
-    <t>Zorggroep Apeldoorn e.o. (Stichting)</t>
-  </si>
-  <si>
     <t>Zorggroep Ena (Stichting)</t>
   </si>
   <si>
@@ -421,15 +391,9 @@
     <t>Vilente (Stichting)</t>
   </si>
   <si>
-    <t>Sterk Huis West Brabant (voorheen Juzt)</t>
-  </si>
-  <si>
     <t>Solis (Stichting)</t>
   </si>
   <si>
-    <t>Stichting Sterk Huis</t>
-  </si>
-  <si>
     <t>Aafje Thuiszorg Huizen Zorghotels (Stichting)</t>
   </si>
   <si>
@@ -475,9 +439,6 @@
     <t>Severinusstichting</t>
   </si>
   <si>
-    <t>Woonzorgcentrum Raffy (Stichting)</t>
-  </si>
-  <si>
     <t>Zorgfederatie Oldenzaal (Stichting)</t>
   </si>
   <si>
@@ -490,12 +451,6 @@
     <t>Respect Zorggroep (Stichting)</t>
   </si>
   <si>
-    <t>Werkt voor Ouderen (Stichting)</t>
-  </si>
-  <si>
-    <t>Wulverhorst</t>
-  </si>
-  <si>
     <t>sHeerenLoo Zorggroep (Stichting)</t>
   </si>
   <si>
@@ -505,9 +460,6 @@
     <t>GGZ Friesland</t>
   </si>
   <si>
-    <t>Het Gasthuis (Sint Jan De Deo) (Stichting)</t>
-  </si>
-  <si>
     <t>Sint Anna Boxmeer (Stichting)</t>
   </si>
   <si>
@@ -526,12 +478,6 @@
     <t>Lister (Stichting)</t>
   </si>
   <si>
-    <t>Parnassia Groep B.V. afdeling Vastgoed en Facilitair</t>
-  </si>
-  <si>
-    <t>Pento (Stichting)</t>
-  </si>
-  <si>
     <t>Pro Persona</t>
   </si>
   <si>
@@ -544,13 +490,127 @@
     <t>Revalidatie Friesland</t>
   </si>
   <si>
-    <t>Ruitersbos (Stichting, valt nu onder Thebe)</t>
-  </si>
-  <si>
     <t>Warande (Stichting)</t>
   </si>
   <si>
     <t>Zorggroep Groningen (Stichting)</t>
+  </si>
+  <si>
+    <t>Amerpoort (Stichting)</t>
+  </si>
+  <si>
+    <t>Argos Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Bartholomeus Gasthuis (Stichting)</t>
+  </si>
+  <si>
+    <t>Carint-Reggeland Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Charim (Zorggroep)</t>
+  </si>
+  <si>
+    <t>De Zijlen (Stichting) (Ilmarinen)</t>
+  </si>
+  <si>
+    <t>Dienstencentrum Oud Burgeren Gasthuis (OBG) (Stichting)</t>
+  </si>
+  <si>
+    <t>DZN B.V. (directe zorg nijmegen)</t>
+  </si>
+  <si>
+    <t>Fier Fryslan (Stichting)</t>
+  </si>
+  <si>
+    <t>GGZ Westelijk Noord-Brabant / GGZ-WNB (Stichting)</t>
+  </si>
+  <si>
+    <t>Het Gasthuis Millingen aan de Rijn (Sint Jan De Deo) (Stichting)</t>
+  </si>
+  <si>
+    <t>Het Parkhuis (Stichting)</t>
+  </si>
+  <si>
+    <t>Ipse de Bruggen (Stichting)</t>
+  </si>
+  <si>
+    <t>Klimmendaal (Stichting)</t>
+  </si>
+  <si>
+    <t>Koninklijke Visio, expertisecentrum voor slechtziende en blinde mensen (Stichting)</t>
+  </si>
+  <si>
+    <t>Lelie Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Lentis incl. Dignis</t>
+  </si>
+  <si>
+    <t>Odion (Stichting)</t>
+  </si>
+  <si>
+    <t>Omega (Groep, Zwolle!)</t>
+  </si>
+  <si>
+    <t>Opbouw (Stichting) incl. Prinsenstichting</t>
+  </si>
+  <si>
+    <t>Ouderenzorg Oudewater, De Wulverhorst</t>
+  </si>
+  <si>
+    <t>Parnassia Groep B.V. Incl. Parnassia haaglanden en noord holland, Antes, Brijder, Youz, etc.</t>
+  </si>
+  <si>
+    <t>Prisma (Stichting)</t>
+  </si>
+  <si>
+    <t>Raffy-Leystroom</t>
+  </si>
+  <si>
+    <t>Robert Coppes Stichting</t>
+  </si>
+  <si>
+    <t>Schärwachter B.V.</t>
+  </si>
+  <si>
+    <t>Sterk Huis (Stichting) (West Brabant was voorheen Juzt)</t>
+  </si>
+  <si>
+    <t>Surplus (Stichting en surplus zorg)</t>
+  </si>
+  <si>
+    <t>SVRZ (Stichting Voor Regionale Zorgverlening)</t>
+  </si>
+  <si>
+    <t>Thebe (Zorggroep west en midden Brabant, incl. Ruitersbos)</t>
+  </si>
+  <si>
+    <t>Treant Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Valkenhof (Stichting)</t>
+  </si>
+  <si>
+    <t>Werkt voor Ouderen (Stichting) (WVO Zorg)</t>
+  </si>
+  <si>
+    <t>Wonen en Zorg Purmerend (Stichting) (SWZP)</t>
+  </si>
+  <si>
+    <t>Zorgcentrum het Bildt (Beukelaar) (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorggroep Apeldoorn en omstreken (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorggroep Elde Maasduinen (Maasduinen Zorg =&gt; gefuseerd uit GD HvB gestapt)</t>
+  </si>
+  <si>
+    <t>Zorggroep Sirjon</t>
+  </si>
+  <si>
+    <t>ZZG Zorggroep (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -911,9 +971,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B171"/>
+  <dimension ref="A1:B191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -931,10 +993,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -942,7 +1004,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -950,7 +1012,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -958,7 +1020,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -966,15 +1028,15 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -982,7 +1044,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -990,1303 +1052,1463 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>155</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>137</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>145</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>122</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B30" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B36" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="B37" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B38" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>161</v>
       </c>
       <c r="B40" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B42" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B45" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>157</v>
+        <v>30</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>163</v>
       </c>
       <c r="B48" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B49" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="B51" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B54" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>164</v>
       </c>
       <c r="B55" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>163</v>
+        <v>36</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="B58" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B59" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>47</v>
+        <v>166</v>
       </c>
       <c r="B60" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B61" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B63" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>52</v>
+        <v>147</v>
       </c>
       <c r="B66" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>164</v>
+        <v>44</v>
       </c>
       <c r="B69" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>55</v>
+        <v>168</v>
       </c>
       <c r="B70" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>56</v>
+        <v>169</v>
       </c>
       <c r="B71" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>45</v>
       </c>
       <c r="B72" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B73" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B74" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="B75" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="B76" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>171</v>
       </c>
       <c r="B77" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B78" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B79" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B80" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>64</v>
+        <v>148</v>
       </c>
       <c r="B81" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B82" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B83" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>67</v>
+        <v>130</v>
       </c>
       <c r="B84" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B85" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>165</v>
+        <v>54</v>
       </c>
       <c r="B86" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>166</v>
+        <v>55</v>
       </c>
       <c r="B87" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>69</v>
+        <v>131</v>
       </c>
       <c r="B88" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>135</v>
+        <v>56</v>
       </c>
       <c r="B89" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="B90" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B91" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B92" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="B93" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B94" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B95" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>74</v>
+        <v>174</v>
       </c>
       <c r="B96" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>144</v>
+        <v>61</v>
       </c>
       <c r="B98" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>145</v>
+        <v>62</v>
       </c>
       <c r="B99" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>168</v>
+        <v>63</v>
       </c>
       <c r="B100" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B101" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>137</v>
+        <v>64</v>
       </c>
       <c r="B102" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="B103" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>170</v>
+        <v>124</v>
       </c>
       <c r="B104" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B105" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B106" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B107" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B108" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>79</v>
+        <v>149</v>
       </c>
       <c r="B109" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B110" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B111" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>146</v>
+        <v>70</v>
       </c>
       <c r="B112" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>82</v>
+        <v>132</v>
       </c>
       <c r="B113" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B114" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>83</v>
+        <v>178</v>
       </c>
       <c r="B115" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B116" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B117" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="B118" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="B119" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="B120" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="B121" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B122" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="B123" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="B124" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B125" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B126" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B127" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="B128" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="B129" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B130" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="B131" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B132" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="B133" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="B134" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B135" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="B136" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B137" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B138" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>100</v>
+        <v>181</v>
       </c>
       <c r="B139" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>101</v>
+        <v>182</v>
       </c>
       <c r="B140" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>102</v>
+        <v>183</v>
       </c>
       <c r="B141" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>172</v>
+        <v>82</v>
       </c>
       <c r="B142" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B143" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>153</v>
+        <v>84</v>
       </c>
       <c r="B144" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>104</v>
+        <v>184</v>
       </c>
       <c r="B145" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B146" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="B147" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>107</v>
+        <v>185</v>
       </c>
       <c r="B148" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>108</v>
+        <v>186</v>
       </c>
       <c r="B149" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="B150" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B151" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="B152" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B153" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B154" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="B155" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="B156" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="B157" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="B158" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="B159" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>149</v>
+        <v>94</v>
       </c>
       <c r="B160" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>116</v>
+        <v>187</v>
       </c>
       <c r="B161" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="B162" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="B163" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>173</v>
+        <v>97</v>
       </c>
       <c r="B164" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>119</v>
+        <v>188</v>
       </c>
       <c r="B165" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="B166" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="B167" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B168" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="B169" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="B170" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="B171" t="s">
-        <v>126</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>103</v>
+      </c>
+      <c r="B172" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>104</v>
+      </c>
+      <c r="B173" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>105</v>
+      </c>
+      <c r="B174" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>106</v>
+      </c>
+      <c r="B175" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>189</v>
+      </c>
+      <c r="B176" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>136</v>
+      </c>
+      <c r="B177" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>107</v>
+      </c>
+      <c r="B178" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>190</v>
+      </c>
+      <c r="B179" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>191</v>
+      </c>
+      <c r="B180" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>108</v>
+      </c>
+      <c r="B181" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>154</v>
+      </c>
+      <c r="B182" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>192</v>
+      </c>
+      <c r="B183" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>109</v>
+      </c>
+      <c r="B184" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>110</v>
+      </c>
+      <c r="B185" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>111</v>
+      </c>
+      <c r="B186" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>112</v>
+      </c>
+      <c r="B187" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>113</v>
+      </c>
+      <c r="B188" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>114</v>
+      </c>
+      <c r="B189" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>115</v>
+      </c>
+      <c r="B190" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>193</v>
+      </c>
+      <c r="B191" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated care data (v28)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C87B87-0F70-4C03-9FF1-A113DC8AB122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387D8EEB-C172-4A60-926A-7D4EEABFAC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16000" yWindow="2030" windowWidth="18380" windowHeight="13930" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="1780" yWindow="1020" windowWidth="22810" windowHeight="18890" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="195">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -484,9 +484,6 @@
     <t>Reade</t>
   </si>
   <si>
-    <t>Reinalda (Stichting Zorggroep, nu onder Kennemerhart)</t>
-  </si>
-  <si>
     <t>Revalidatie Friesland</t>
   </si>
   <si>
@@ -611,6 +608,12 @@
   </si>
   <si>
     <t>ZZG Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Emergis (Stichting)</t>
+  </si>
+  <si>
+    <t>Waardeburgh (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -971,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B191"/>
+  <dimension ref="A1:B192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1020,7 +1023,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1057,7 +1060,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
         <v>116</v>
@@ -1073,7 +1076,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
         <v>116</v>
@@ -1145,7 +1148,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B21" t="s">
         <v>116</v>
@@ -1209,15 +1212,15 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
         <v>116</v>
@@ -1273,7 +1276,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B37" t="s">
         <v>117</v>
@@ -1297,7 +1300,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B40" t="s">
         <v>116</v>
@@ -1337,7 +1340,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B45" t="s">
         <v>117</v>
@@ -1353,55 +1356,55 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>30</v>
+        <v>193</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>163</v>
+        <v>30</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>32</v>
       </c>
       <c r="B51" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="B52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
       <c r="B53" t="s">
         <v>117</v>
@@ -1409,15 +1412,15 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
       <c r="B55" t="s">
         <v>116</v>
@@ -1425,7 +1428,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>163</v>
       </c>
       <c r="B56" t="s">
         <v>116</v>
@@ -1433,7 +1436,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B57" t="s">
         <v>116</v>
@@ -1441,23 +1444,23 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>165</v>
+        <v>36</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>164</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
       <c r="B60" t="s">
         <v>116</v>
@@ -1465,7 +1468,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>38</v>
+        <v>165</v>
       </c>
       <c r="B61" t="s">
         <v>116</v>
@@ -1473,7 +1476,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B62" t="s">
         <v>116</v>
@@ -1481,7 +1484,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B63" t="s">
         <v>116</v>
@@ -1489,15 +1492,15 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B64" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>167</v>
+        <v>41</v>
       </c>
       <c r="B65" t="s">
         <v>117</v>
@@ -1505,31 +1508,31 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="B66" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
       <c r="B67" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B69" t="s">
         <v>116</v>
@@ -1537,7 +1540,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>168</v>
+        <v>44</v>
       </c>
       <c r="B70" t="s">
         <v>116</v>
@@ -1545,7 +1548,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B71" t="s">
         <v>116</v>
@@ -1553,7 +1556,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>45</v>
+        <v>168</v>
       </c>
       <c r="B72" t="s">
         <v>116</v>
@@ -1561,7 +1564,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B73" t="s">
         <v>116</v>
@@ -1569,7 +1572,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B74" t="s">
         <v>116</v>
@@ -1577,39 +1580,39 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="B76" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>48</v>
+        <v>170</v>
       </c>
       <c r="B78" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B79" t="s">
         <v>116</v>
@@ -1617,7 +1620,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B80" t="s">
         <v>116</v>
@@ -1625,7 +1628,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>148</v>
+        <v>50</v>
       </c>
       <c r="B81" t="s">
         <v>116</v>
@@ -1633,7 +1636,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="B82" t="s">
         <v>116</v>
@@ -1641,7 +1644,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B83" t="s">
         <v>116</v>
@@ -1649,7 +1652,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>130</v>
+        <v>52</v>
       </c>
       <c r="B84" t="s">
         <v>116</v>
@@ -1657,7 +1660,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="B85" t="s">
         <v>116</v>
@@ -1665,7 +1668,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B86" t="s">
         <v>116</v>
@@ -1673,7 +1676,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B87" t="s">
         <v>116</v>
@@ -1681,15 +1684,15 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="B88" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>56</v>
+        <v>131</v>
       </c>
       <c r="B89" t="s">
         <v>117</v>
@@ -1697,7 +1700,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B90" t="s">
         <v>117</v>
@@ -1705,15 +1708,15 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B91" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B92" t="s">
         <v>116</v>
@@ -1721,7 +1724,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>172</v>
+        <v>59</v>
       </c>
       <c r="B93" t="s">
         <v>116</v>
@@ -1729,7 +1732,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B94" t="s">
         <v>116</v>
@@ -1737,23 +1740,23 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>60</v>
+        <v>172</v>
       </c>
       <c r="B95" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>174</v>
+        <v>60</v>
       </c>
       <c r="B96" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B97" t="s">
         <v>116</v>
@@ -1761,7 +1764,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>61</v>
+        <v>174</v>
       </c>
       <c r="B98" t="s">
         <v>116</v>
@@ -1769,7 +1772,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B99" t="s">
         <v>116</v>
@@ -1777,23 +1780,23 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B100" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>176</v>
+        <v>63</v>
       </c>
       <c r="B101" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>64</v>
+        <v>175</v>
       </c>
       <c r="B102" t="s">
         <v>116</v>
@@ -1801,7 +1804,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>123</v>
+        <v>64</v>
       </c>
       <c r="B103" t="s">
         <v>116</v>
@@ -1809,23 +1812,23 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B104" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="B105" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B106" t="s">
         <v>116</v>
@@ -1833,7 +1836,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B107" t="s">
         <v>116</v>
@@ -1841,7 +1844,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>177</v>
+        <v>67</v>
       </c>
       <c r="B108" t="s">
         <v>116</v>
@@ -1849,7 +1852,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="B109" t="s">
         <v>116</v>
@@ -1857,7 +1860,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="B110" t="s">
         <v>116</v>
@@ -1865,23 +1868,23 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B111" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B112" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="B113" t="s">
         <v>116</v>
@@ -1889,23 +1892,23 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B114" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>178</v>
+        <v>133</v>
       </c>
       <c r="B115" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="B116" t="s">
         <v>116</v>
@@ -1913,7 +1916,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B117" t="s">
         <v>116</v>
@@ -1937,7 +1940,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B120" t="s">
         <v>116</v>
@@ -1969,7 +1972,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B124" t="s">
         <v>117</v>
@@ -2009,7 +2012,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B129" t="s">
         <v>117</v>
@@ -2089,7 +2092,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B139" t="s">
         <v>116</v>
@@ -2097,7 +2100,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B140" t="s">
         <v>117</v>
@@ -2105,7 +2108,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B141" t="s">
         <v>116</v>
@@ -2137,7 +2140,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B145" t="s">
         <v>116</v>
@@ -2161,7 +2164,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B148" t="s">
         <v>116</v>
@@ -2169,7 +2172,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B149" t="s">
         <v>116</v>
@@ -2249,7 +2252,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
       <c r="B159" t="s">
         <v>116</v>
@@ -2257,23 +2260,23 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>94</v>
+        <v>152</v>
       </c>
       <c r="B160" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>187</v>
+        <v>94</v>
       </c>
       <c r="B161" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>95</v>
+        <v>186</v>
       </c>
       <c r="B162" t="s">
         <v>116</v>
@@ -2281,31 +2284,31 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B163" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B164" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>188</v>
+        <v>97</v>
       </c>
       <c r="B165" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>98</v>
+        <v>187</v>
       </c>
       <c r="B166" t="s">
         <v>117</v>
@@ -2313,7 +2316,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B167" t="s">
         <v>117</v>
@@ -2321,15 +2324,15 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="B168" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="B169" t="s">
         <v>116</v>
@@ -2337,7 +2340,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B170" t="s">
         <v>116</v>
@@ -2345,7 +2348,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B171" t="s">
         <v>116</v>
@@ -2353,7 +2356,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B172" t="s">
         <v>116</v>
@@ -2361,7 +2364,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B173" t="s">
         <v>116</v>
@@ -2369,7 +2372,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B174" t="s">
         <v>116</v>
@@ -2377,31 +2380,31 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B175" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>189</v>
+        <v>106</v>
       </c>
       <c r="B176" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>136</v>
+        <v>188</v>
       </c>
       <c r="B177" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="B178" t="s">
         <v>117</v>
@@ -2409,15 +2412,15 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>190</v>
+        <v>107</v>
       </c>
       <c r="B179" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B180" t="s">
         <v>116</v>
@@ -2425,7 +2428,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>108</v>
+        <v>190</v>
       </c>
       <c r="B181" t="s">
         <v>116</v>
@@ -2433,15 +2436,15 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
       <c r="B182" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="B183" t="s">
         <v>117</v>
@@ -2449,15 +2452,15 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>109</v>
+        <v>191</v>
       </c>
       <c r="B184" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B185" t="s">
         <v>116</v>
@@ -2465,7 +2468,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B186" t="s">
         <v>116</v>
@@ -2473,41 +2476,49 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B187" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B188" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B189" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B190" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>193</v>
+        <v>115</v>
       </c>
       <c r="B191" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>192</v>
+      </c>
+      <c r="B192" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated care data (v29)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387D8EEB-C172-4A60-926A-7D4EEABFAC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3997688B-2B06-4E64-B3A9-43B8F3977ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1020" windowWidth="22810" windowHeight="18890" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="8550" yWindow="2230" windowWidth="22900" windowHeight="18330" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="200">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -614,6 +614,21 @@
   </si>
   <si>
     <t>Waardeburgh (Stichting)</t>
+  </si>
+  <si>
+    <t>Alkcare (Stichting)</t>
+  </si>
+  <si>
+    <t>Fundis (Stichting) (beheren meerdere zorginstellingen, zoals Welthuis)</t>
+  </si>
+  <si>
+    <t>Hartekamp Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Liemerije (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorggroep Sint Maarten (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -974,11 +989,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B192"/>
+  <dimension ref="A1:B197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1028,7 +1041,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
         <v>116</v>
@@ -1036,7 +1049,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>116</v>
@@ -1044,23 +1057,23 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>116</v>
@@ -1068,23 +1081,23 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
         <v>116</v>
@@ -1092,7 +1105,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>116</v>
@@ -1100,7 +1113,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>116</v>
@@ -1108,7 +1121,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>116</v>
@@ -1116,7 +1129,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>116</v>
@@ -1124,23 +1137,23 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>137</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>116</v>
@@ -1148,7 +1161,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>116</v>
@@ -1156,7 +1169,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
       <c r="B22" t="s">
         <v>116</v>
@@ -1164,15 +1177,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
         <v>117</v>
@@ -1180,7 +1193,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="B25" t="s">
         <v>117</v>
@@ -1188,7 +1201,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="B26" t="s">
         <v>117</v>
@@ -1196,15 +1209,15 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
         <v>116</v>
@@ -1212,39 +1225,39 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>157</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>141</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
         <v>116</v>
@@ -1252,7 +1265,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B34" t="s">
         <v>116</v>
@@ -1260,31 +1273,31 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>138</v>
       </c>
       <c r="B35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>159</v>
       </c>
       <c r="B38" t="s">
         <v>117</v>
@@ -1292,7 +1305,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>24</v>
       </c>
       <c r="B39" t="s">
         <v>117</v>
@@ -1300,15 +1313,15 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="B40" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>160</v>
       </c>
       <c r="B41" t="s">
         <v>116</v>
@@ -1316,7 +1329,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B42" t="s">
         <v>116</v>
@@ -1324,7 +1337,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B43" t="s">
         <v>116</v>
@@ -1332,15 +1345,15 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="B45" t="s">
         <v>117</v>
@@ -1348,47 +1361,47 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>161</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>193</v>
+        <v>29</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>30</v>
+        <v>193</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="B49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="B50" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>196</v>
       </c>
       <c r="B51" t="s">
         <v>117</v>
@@ -1396,7 +1409,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>129</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
         <v>116</v>
@@ -1404,7 +1417,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B53" t="s">
         <v>117</v>
@@ -1412,31 +1425,31 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B55" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B56" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B57" t="s">
         <v>116</v>
@@ -1444,7 +1457,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>163</v>
       </c>
       <c r="B58" t="s">
         <v>116</v>
@@ -1452,23 +1465,23 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>164</v>
+        <v>35</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>197</v>
       </c>
       <c r="B60" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>165</v>
+        <v>36</v>
       </c>
       <c r="B61" t="s">
         <v>116</v>
@@ -1476,15 +1489,15 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>38</v>
+        <v>164</v>
       </c>
       <c r="B62" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B63" t="s">
         <v>116</v>
@@ -1492,7 +1505,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="B64" t="s">
         <v>116</v>
@@ -1500,23 +1513,23 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>166</v>
+        <v>39</v>
       </c>
       <c r="B66" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>147</v>
+        <v>40</v>
       </c>
       <c r="B67" t="s">
         <v>116</v>
@@ -1524,7 +1537,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B68" t="s">
         <v>117</v>
@@ -1532,15 +1545,15 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>43</v>
+        <v>166</v>
       </c>
       <c r="B69" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="B70" t="s">
         <v>116</v>
@@ -1548,15 +1561,15 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>167</v>
+        <v>42</v>
       </c>
       <c r="B71" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>168</v>
+        <v>43</v>
       </c>
       <c r="B72" t="s">
         <v>116</v>
@@ -1564,7 +1577,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" t="s">
         <v>116</v>
@@ -1572,7 +1585,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="B74" t="s">
         <v>116</v>
@@ -1580,7 +1593,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>47</v>
+        <v>168</v>
       </c>
       <c r="B75" t="s">
         <v>116</v>
@@ -1588,15 +1601,15 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B76" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>169</v>
+        <v>46</v>
       </c>
       <c r="B77" t="s">
         <v>116</v>
@@ -1604,7 +1617,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>170</v>
+        <v>47</v>
       </c>
       <c r="B78" t="s">
         <v>117</v>
@@ -1612,15 +1625,15 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="B79" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>49</v>
+        <v>169</v>
       </c>
       <c r="B80" t="s">
         <v>116</v>
@@ -1628,15 +1641,15 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>50</v>
+        <v>170</v>
       </c>
       <c r="B81" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>148</v>
+        <v>48</v>
       </c>
       <c r="B82" t="s">
         <v>116</v>
@@ -1644,7 +1657,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B83" t="s">
         <v>116</v>
@@ -1652,7 +1665,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B84" t="s">
         <v>116</v>
@@ -1660,15 +1673,15 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>130</v>
+        <v>198</v>
       </c>
       <c r="B85" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>53</v>
+        <v>148</v>
       </c>
       <c r="B86" t="s">
         <v>116</v>
@@ -1676,15 +1689,15 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B87" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B88" t="s">
         <v>116</v>
@@ -1692,31 +1705,31 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B89" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B90" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B91" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B92" t="s">
         <v>116</v>
@@ -1724,39 +1737,39 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
       <c r="B93" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>171</v>
+        <v>56</v>
       </c>
       <c r="B94" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>172</v>
+        <v>57</v>
       </c>
       <c r="B95" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B96" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>173</v>
+        <v>59</v>
       </c>
       <c r="B97" t="s">
         <v>116</v>
@@ -1764,7 +1777,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B98" t="s">
         <v>116</v>
@@ -1772,7 +1785,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>61</v>
+        <v>172</v>
       </c>
       <c r="B99" t="s">
         <v>116</v>
@@ -1780,23 +1793,23 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B100" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>63</v>
+        <v>173</v>
       </c>
       <c r="B101" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B102" t="s">
         <v>116</v>
@@ -1804,7 +1817,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B103" t="s">
         <v>116</v>
@@ -1812,7 +1825,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>123</v>
+        <v>62</v>
       </c>
       <c r="B104" t="s">
         <v>116</v>
@@ -1820,7 +1833,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="B105" t="s">
         <v>117</v>
@@ -1828,7 +1841,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>65</v>
+        <v>175</v>
       </c>
       <c r="B106" t="s">
         <v>116</v>
@@ -1836,7 +1849,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B107" t="s">
         <v>116</v>
@@ -1844,7 +1857,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="B108" t="s">
         <v>116</v>
@@ -1852,15 +1865,15 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>176</v>
+        <v>124</v>
       </c>
       <c r="B109" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="B110" t="s">
         <v>116</v>
@@ -1868,7 +1881,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B111" t="s">
         <v>116</v>
@@ -1876,15 +1889,15 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B112" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>70</v>
+        <v>176</v>
       </c>
       <c r="B113" t="s">
         <v>116</v>
@@ -1892,7 +1905,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="B114" t="s">
         <v>116</v>
@@ -1900,23 +1913,23 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="B115" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>177</v>
+        <v>69</v>
       </c>
       <c r="B116" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>150</v>
+        <v>70</v>
       </c>
       <c r="B117" t="s">
         <v>116</v>
@@ -1924,7 +1937,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B118" t="s">
         <v>116</v>
@@ -1932,15 +1945,15 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B119" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="B120" t="s">
         <v>116</v>
@@ -1948,15 +1961,15 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="B121" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>72</v>
+        <v>125</v>
       </c>
       <c r="B122" t="s">
         <v>116</v>
@@ -1964,7 +1977,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>73</v>
+        <v>139</v>
       </c>
       <c r="B123" t="s">
         <v>116</v>
@@ -1972,23 +1985,23 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="B124" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B125" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B126" t="s">
         <v>116</v>
@@ -1996,7 +2009,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B127" t="s">
         <v>117</v>
@@ -2004,7 +2017,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>134</v>
+        <v>178</v>
       </c>
       <c r="B128" t="s">
         <v>117</v>
@@ -2012,31 +2025,31 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>179</v>
+        <v>74</v>
       </c>
       <c r="B129" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B130" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>135</v>
+        <v>76</v>
       </c>
       <c r="B131" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="B132" t="s">
         <v>117</v>
@@ -2044,7 +2057,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="B133" t="s">
         <v>117</v>
@@ -2052,7 +2065,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>143</v>
+        <v>77</v>
       </c>
       <c r="B134" t="s">
         <v>117</v>
@@ -2060,7 +2073,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>79</v>
+        <v>135</v>
       </c>
       <c r="B135" t="s">
         <v>116</v>
@@ -2068,23 +2081,23 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B136" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="B137" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="B138" t="s">
         <v>117</v>
@@ -2092,7 +2105,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
       <c r="B139" t="s">
         <v>116</v>
@@ -2100,15 +2113,15 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>181</v>
+        <v>80</v>
       </c>
       <c r="B140" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>182</v>
+        <v>120</v>
       </c>
       <c r="B141" t="s">
         <v>116</v>
@@ -2116,31 +2129,31 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B142" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>83</v>
+        <v>180</v>
       </c>
       <c r="B143" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>84</v>
+        <v>181</v>
       </c>
       <c r="B144" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B145" t="s">
         <v>116</v>
@@ -2148,7 +2161,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B146" t="s">
         <v>116</v>
@@ -2156,15 +2169,15 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B147" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>184</v>
+        <v>84</v>
       </c>
       <c r="B148" t="s">
         <v>116</v>
@@ -2172,7 +2185,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B149" t="s">
         <v>116</v>
@@ -2180,7 +2193,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B150" t="s">
         <v>116</v>
@@ -2188,7 +2201,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>144</v>
+        <v>86</v>
       </c>
       <c r="B151" t="s">
         <v>116</v>
@@ -2196,7 +2209,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>88</v>
+        <v>184</v>
       </c>
       <c r="B152" t="s">
         <v>116</v>
@@ -2204,7 +2217,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>89</v>
+        <v>185</v>
       </c>
       <c r="B153" t="s">
         <v>116</v>
@@ -2212,15 +2225,15 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="B154" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="B155" t="s">
         <v>116</v>
@@ -2228,7 +2241,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B156" t="s">
         <v>116</v>
@@ -2236,7 +2249,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B157" t="s">
         <v>116</v>
@@ -2244,7 +2257,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B158" t="s">
         <v>117</v>
@@ -2252,7 +2265,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>194</v>
+        <v>90</v>
       </c>
       <c r="B159" t="s">
         <v>116</v>
@@ -2260,7 +2273,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="B160" t="s">
         <v>116</v>
@@ -2268,23 +2281,23 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B161" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>186</v>
+        <v>93</v>
       </c>
       <c r="B162" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>95</v>
+        <v>194</v>
       </c>
       <c r="B163" t="s">
         <v>116</v>
@@ -2292,39 +2305,39 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>96</v>
+        <v>152</v>
       </c>
       <c r="B164" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B165" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B166" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B167" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B168" t="s">
         <v>117</v>
@@ -2332,7 +2345,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="B169" t="s">
         <v>116</v>
@@ -2340,31 +2353,31 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>100</v>
+        <v>187</v>
       </c>
       <c r="B170" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B171" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B172" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="B173" t="s">
         <v>116</v>
@@ -2372,7 +2385,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B174" t="s">
         <v>116</v>
@@ -2380,7 +2393,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B175" t="s">
         <v>116</v>
@@ -2388,15 +2401,15 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B176" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>188</v>
+        <v>103</v>
       </c>
       <c r="B177" t="s">
         <v>116</v>
@@ -2404,31 +2417,31 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="B178" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B179" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>189</v>
+        <v>106</v>
       </c>
       <c r="B180" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B181" t="s">
         <v>116</v>
@@ -2436,15 +2449,15 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="B182" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="B183" t="s">
         <v>117</v>
@@ -2452,15 +2465,15 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B184" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="B185" t="s">
         <v>116</v>
@@ -2468,7 +2481,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B186" t="s">
         <v>116</v>
@@ -2476,39 +2489,39 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="B187" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>112</v>
+        <v>199</v>
       </c>
       <c r="B188" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>113</v>
+        <v>191</v>
       </c>
       <c r="B189" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B190" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B191" t="s">
         <v>116</v>
@@ -2516,9 +2529,49 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
+        <v>111</v>
+      </c>
+      <c r="B192" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>112</v>
+      </c>
+      <c r="B193" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>113</v>
+      </c>
+      <c r="B194" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>114</v>
+      </c>
+      <c r="B195" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>115</v>
+      </c>
+      <c r="B196" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
         <v>192</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B197" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated care data (v30)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3997688B-2B06-4E64-B3A9-43B8F3977ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465A5C9C-2DBA-4A7E-980E-1943D89DDC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8550" yWindow="2230" windowWidth="22900" windowHeight="18330" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="12640" yWindow="1030" windowWidth="24390" windowHeight="18970" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="205">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -313,9 +313,6 @@
     <t>Vogellanden, Centrum voor Revalidatie (Stichting)</t>
   </si>
   <si>
-    <t>WelThuis BV</t>
-  </si>
-  <si>
     <t>Wever (Stichting)</t>
   </si>
   <si>
@@ -629,6 +626,24 @@
   </si>
   <si>
     <t>Zorggroep Sint Maarten (Stichting)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alliade </t>
+  </si>
+  <si>
+    <t>Ambiq (Stichting)</t>
+  </si>
+  <si>
+    <t>Breederzorg Thuiszorg (Stichting)</t>
+  </si>
+  <si>
+    <t>Huize Winterdijk (Stichting tot Oprichting en Instandhouding van Bejaardenoorden en Verzorgingstehuizen, uitgaande v.d. Gereformeerde Gemeente in Nederland)</t>
+  </si>
+  <si>
+    <t>Korian Zorg B.V.</t>
+  </si>
+  <si>
+    <t>Zorgcentrum Beek en Bos (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -989,7 +1004,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B197"/>
+  <dimension ref="A1:B202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1009,10 +1024,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1020,7 +1035,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1028,7 +1043,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1036,12 +1051,12 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B6" t="s">
         <v>116</v>
@@ -1049,7 +1064,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="B7" t="s">
         <v>116</v>
@@ -1057,23 +1072,23 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>116</v>
@@ -1081,31 +1096,31 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>200</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
         <v>116</v>
@@ -1113,55 +1128,55 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>154</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
         <v>116</v>
@@ -1169,55 +1184,55 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>156</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>155</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>144</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="B28" t="s">
         <v>116</v>
@@ -1225,7 +1240,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>201</v>
       </c>
       <c r="B29" t="s">
         <v>116</v>
@@ -1233,31 +1248,31 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="B33" t="s">
         <v>116</v>
@@ -1265,15 +1280,15 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
         <v>116</v>
@@ -1281,47 +1296,47 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="B38" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B41" t="s">
         <v>116</v>
@@ -1329,7 +1344,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
         <v>116</v>
@@ -1337,7 +1352,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s">
         <v>116</v>
@@ -1345,47 +1360,47 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="B44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>161</v>
+        <v>26</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>193</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>30</v>
+        <v>160</v>
       </c>
       <c r="B49" t="s">
         <v>116</v>
@@ -1393,39 +1408,39 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>162</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>161</v>
       </c>
       <c r="B53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>129</v>
+        <v>195</v>
       </c>
       <c r="B54" t="s">
         <v>116</v>
@@ -1433,31 +1448,31 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>142</v>
+        <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
       <c r="B57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>163</v>
+        <v>33</v>
       </c>
       <c r="B58" t="s">
         <v>116</v>
@@ -1465,7 +1480,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>141</v>
       </c>
       <c r="B59" t="s">
         <v>116</v>
@@ -1473,31 +1488,31 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>197</v>
+        <v>34</v>
       </c>
       <c r="B60" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="B61" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>164</v>
+        <v>35</v>
       </c>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>37</v>
+        <v>196</v>
       </c>
       <c r="B63" t="s">
         <v>116</v>
@@ -1505,15 +1520,15 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>165</v>
+        <v>36</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>38</v>
+        <v>163</v>
       </c>
       <c r="B65" t="s">
         <v>116</v>
@@ -1521,39 +1536,39 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B66" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>40</v>
+        <v>164</v>
       </c>
       <c r="B67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B68" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>166</v>
+        <v>39</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>147</v>
+        <v>202</v>
       </c>
       <c r="B70" t="s">
         <v>116</v>
@@ -1561,15 +1576,15 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B71" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B72" t="s">
         <v>116</v>
@@ -1577,7 +1592,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>44</v>
+        <v>165</v>
       </c>
       <c r="B73" t="s">
         <v>116</v>
@@ -1585,15 +1600,15 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="B74" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>168</v>
+        <v>42</v>
       </c>
       <c r="B75" t="s">
         <v>116</v>
@@ -1601,63 +1616,63 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>47</v>
+        <v>166</v>
       </c>
       <c r="B78" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>118</v>
+        <v>167</v>
       </c>
       <c r="B79" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>169</v>
+        <v>45</v>
       </c>
       <c r="B80" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>170</v>
+        <v>203</v>
       </c>
       <c r="B81" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B82" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B83" t="s">
         <v>116</v>
@@ -1665,7 +1680,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="B84" t="s">
         <v>116</v>
@@ -1673,15 +1688,15 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="B85" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="B86" t="s">
         <v>116</v>
@@ -1689,31 +1704,31 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B87" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B88" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="B89" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>53</v>
+        <v>197</v>
       </c>
       <c r="B90" t="s">
         <v>116</v>
@@ -1721,63 +1736,63 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>54</v>
+        <v>147</v>
       </c>
       <c r="B91" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B92" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="B93" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>56</v>
+        <v>129</v>
       </c>
       <c r="B94" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B95" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B96" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B97" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="B98" t="s">
         <v>116</v>
@@ -1785,7 +1800,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>172</v>
+        <v>56</v>
       </c>
       <c r="B99" t="s">
         <v>116</v>
@@ -1793,87 +1808,87 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B100" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>173</v>
+        <v>58</v>
       </c>
       <c r="B101" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>174</v>
+        <v>59</v>
       </c>
       <c r="B102" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>61</v>
+        <v>170</v>
       </c>
       <c r="B103" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B105" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B106" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="B107" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="B108" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
       <c r="B109" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B110" t="s">
         <v>116</v>
@@ -1881,31 +1896,31 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>66</v>
+        <v>174</v>
       </c>
       <c r="B111" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B112" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>176</v>
+        <v>122</v>
       </c>
       <c r="B113" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="B114" t="s">
         <v>116</v>
@@ -1913,55 +1928,55 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B115" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B116" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>132</v>
+        <v>175</v>
       </c>
       <c r="B118" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="B119" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>177</v>
+        <v>68</v>
       </c>
       <c r="B120" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>150</v>
+        <v>69</v>
       </c>
       <c r="B121" t="s">
         <v>116</v>
@@ -1969,23 +1984,23 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>125</v>
+        <v>70</v>
       </c>
       <c r="B122" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B123" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="B124" t="s">
         <v>116</v>
@@ -1993,47 +2008,47 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>71</v>
+        <v>176</v>
       </c>
       <c r="B125" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>72</v>
+        <v>149</v>
       </c>
       <c r="B126" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="B127" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="B128" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>74</v>
+        <v>150</v>
       </c>
       <c r="B129" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B130" t="s">
         <v>116</v>
@@ -2041,71 +2056,71 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B131" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>134</v>
+        <v>73</v>
       </c>
       <c r="B132" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B133" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B134" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="B135" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B136" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B137" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="B138" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B139" t="s">
         <v>116</v>
@@ -2113,15 +2128,15 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="B140" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="B141" t="s">
         <v>116</v>
@@ -2129,15 +2144,15 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="B142" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="B143" t="s">
         <v>116</v>
@@ -2145,47 +2160,47 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>181</v>
+        <v>79</v>
       </c>
       <c r="B144" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>182</v>
+        <v>80</v>
       </c>
       <c r="B145" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="B146" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B147" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>84</v>
+        <v>179</v>
       </c>
       <c r="B148" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B149" t="s">
         <v>116</v>
@@ -2193,23 +2208,23 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="B150" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B151" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B152" t="s">
         <v>116</v>
@@ -2217,87 +2232,87 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>185</v>
+        <v>84</v>
       </c>
       <c r="B153" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>87</v>
+        <v>182</v>
       </c>
       <c r="B154" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>144</v>
+        <v>85</v>
       </c>
       <c r="B155" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B156" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>89</v>
+        <v>183</v>
       </c>
       <c r="B157" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>119</v>
+        <v>184</v>
       </c>
       <c r="B158" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B159" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="B160" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B161" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B162" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>194</v>
+        <v>118</v>
       </c>
       <c r="B163" t="s">
         <v>116</v>
@@ -2305,31 +2320,31 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>152</v>
+        <v>90</v>
       </c>
       <c r="B164" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B165" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>186</v>
+        <v>92</v>
       </c>
       <c r="B166" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B167" t="s">
         <v>116</v>
@@ -2337,55 +2352,55 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>96</v>
+        <v>193</v>
       </c>
       <c r="B168" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="B169" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B170" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B171" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B172" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="B173" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>100</v>
+        <v>186</v>
       </c>
       <c r="B174" t="s">
         <v>116</v>
@@ -2393,7 +2408,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B175" t="s">
         <v>116</v>
@@ -2401,7 +2416,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B176" t="s">
         <v>116</v>
@@ -2409,63 +2424,63 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="B177" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B178" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B179" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B180" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>188</v>
+        <v>102</v>
       </c>
       <c r="B181" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="B182" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B183" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>189</v>
+        <v>105</v>
       </c>
       <c r="B184" t="s">
         <v>116</v>
@@ -2473,7 +2488,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="B185" t="s">
         <v>116</v>
@@ -2481,23 +2496,23 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>108</v>
+        <v>187</v>
       </c>
       <c r="B186" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="B187" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>199</v>
+        <v>106</v>
       </c>
       <c r="B188" t="s">
         <v>116</v>
@@ -2505,31 +2520,31 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>109</v>
+        <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B191" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>111</v>
+        <v>152</v>
       </c>
       <c r="B192" t="s">
         <v>116</v>
@@ -2537,15 +2552,15 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>112</v>
+        <v>198</v>
       </c>
       <c r="B193" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>113</v>
+        <v>190</v>
       </c>
       <c r="B194" t="s">
         <v>116</v>
@@ -2553,26 +2568,66 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B195" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B196" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>192</v>
+        <v>110</v>
       </c>
       <c r="B197" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>111</v>
+      </c>
+      <c r="B198" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>112</v>
+      </c>
+      <c r="B199" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>113</v>
+      </c>
+      <c r="B200" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>114</v>
+      </c>
+      <c r="B201" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>191</v>
+      </c>
+      <c r="B202" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated care data (v31)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465A5C9C-2DBA-4A7E-980E-1943D89DDC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFB62D4-DBE0-4600-B34B-918592926499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12640" yWindow="1030" windowWidth="24390" windowHeight="18970" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="4940" yWindow="2400" windowWidth="24320" windowHeight="19200" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="208">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -644,6 +644,15 @@
   </si>
   <si>
     <t>Zorgcentrum Beek en Bos (Stichting)</t>
+  </si>
+  <si>
+    <t>Dagelijks Leven Zorg (B.V).</t>
+  </si>
+  <si>
+    <t>De Blije Borgh / Protestants Interkerkelijke Stichting Zorgverlening Hendrik-Ido-Ambacht</t>
+  </si>
+  <si>
+    <t>Swinhove Groep (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1013,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B202"/>
+  <dimension ref="A1:B205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1328,15 +1337,15 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>205</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>158</v>
+        <v>206</v>
       </c>
       <c r="B41" t="s">
         <v>116</v>
@@ -1344,15 +1353,15 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="B43" t="s">
         <v>116</v>
@@ -1360,23 +1369,23 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>159</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>159</v>
       </c>
       <c r="B46" t="s">
         <v>115</v>
@@ -1384,7 +1393,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B47" t="s">
         <v>115</v>
@@ -1392,31 +1401,31 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>160</v>
+        <v>27</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="B51" t="s">
         <v>116</v>
@@ -1424,7 +1433,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B52" t="s">
         <v>115</v>
@@ -1432,7 +1441,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
       <c r="B53" t="s">
         <v>116</v>
@@ -1440,23 +1449,23 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>195</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>161</v>
       </c>
       <c r="B55" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>195</v>
       </c>
       <c r="B56" t="s">
         <v>116</v>
@@ -1464,7 +1473,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="B57" t="s">
         <v>115</v>
@@ -1472,7 +1481,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B58" t="s">
         <v>116</v>
@@ -1480,7 +1489,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B59" t="s">
         <v>116</v>
@@ -1488,7 +1497,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B60" t="s">
         <v>115</v>
@@ -1496,7 +1505,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="B61" t="s">
         <v>115</v>
@@ -1504,7 +1513,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B62" t="s">
         <v>115</v>
@@ -1512,7 +1521,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="B63" t="s">
         <v>116</v>
@@ -1520,7 +1529,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
         <v>115</v>
@@ -1528,7 +1537,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="B65" t="s">
         <v>116</v>
@@ -1536,7 +1545,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B66" t="s">
         <v>115</v>
@@ -1544,7 +1553,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B67" t="s">
         <v>115</v>
@@ -1552,7 +1561,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B68" t="s">
         <v>115</v>
@@ -1560,7 +1569,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>39</v>
+        <v>164</v>
       </c>
       <c r="B69" t="s">
         <v>115</v>
@@ -1568,7 +1577,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>202</v>
+        <v>38</v>
       </c>
       <c r="B70" t="s">
         <v>116</v>
@@ -1576,7 +1585,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B71" t="s">
         <v>115</v>
@@ -1584,7 +1593,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>41</v>
+        <v>202</v>
       </c>
       <c r="B72" t="s">
         <v>116</v>
@@ -1592,7 +1601,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="B73" t="s">
         <v>116</v>
@@ -1600,7 +1609,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>146</v>
+        <v>41</v>
       </c>
       <c r="B74" t="s">
         <v>115</v>
@@ -1608,7 +1617,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>42</v>
+        <v>165</v>
       </c>
       <c r="B75" t="s">
         <v>116</v>
@@ -1616,7 +1625,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="B76" t="s">
         <v>115</v>
@@ -1624,7 +1633,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B77" t="s">
         <v>115</v>
@@ -1632,7 +1641,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="B78" t="s">
         <v>115</v>
@@ -1640,7 +1649,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>167</v>
+        <v>44</v>
       </c>
       <c r="B79" t="s">
         <v>115</v>
@@ -1648,7 +1657,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>45</v>
+        <v>166</v>
       </c>
       <c r="B80" t="s">
         <v>115</v>
@@ -1656,7 +1665,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="B81" t="s">
         <v>115</v>
@@ -1664,7 +1673,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B82" t="s">
         <v>115</v>
@@ -1672,7 +1681,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>47</v>
+        <v>203</v>
       </c>
       <c r="B83" t="s">
         <v>116</v>
@@ -1680,7 +1689,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>117</v>
+        <v>46</v>
       </c>
       <c r="B84" t="s">
         <v>116</v>
@@ -1688,7 +1697,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>168</v>
+        <v>47</v>
       </c>
       <c r="B85" t="s">
         <v>115</v>
@@ -1696,7 +1705,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>169</v>
+        <v>117</v>
       </c>
       <c r="B86" t="s">
         <v>116</v>
@@ -1704,7 +1713,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>48</v>
+        <v>168</v>
       </c>
       <c r="B87" t="s">
         <v>115</v>
@@ -1712,7 +1721,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>49</v>
+        <v>169</v>
       </c>
       <c r="B88" t="s">
         <v>115</v>
@@ -1720,7 +1729,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B89" t="s">
         <v>115</v>
@@ -1728,7 +1737,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>197</v>
+        <v>49</v>
       </c>
       <c r="B90" t="s">
         <v>116</v>
@@ -1736,7 +1745,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>147</v>
+        <v>50</v>
       </c>
       <c r="B91" t="s">
         <v>115</v>
@@ -1744,7 +1753,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>51</v>
+        <v>197</v>
       </c>
       <c r="B92" t="s">
         <v>115</v>
@@ -1752,7 +1761,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>52</v>
+        <v>147</v>
       </c>
       <c r="B93" t="s">
         <v>115</v>
@@ -1760,7 +1769,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>129</v>
+        <v>51</v>
       </c>
       <c r="B94" t="s">
         <v>115</v>
@@ -1768,7 +1777,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B95" t="s">
         <v>115</v>
@@ -1776,7 +1785,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="B96" t="s">
         <v>115</v>
@@ -1784,7 +1793,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B97" t="s">
         <v>115</v>
@@ -1792,7 +1801,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="B98" t="s">
         <v>116</v>
@@ -1800,7 +1809,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B99" t="s">
         <v>116</v>
@@ -1808,7 +1817,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>57</v>
+        <v>130</v>
       </c>
       <c r="B100" t="s">
         <v>116</v>
@@ -1816,7 +1825,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B101" t="s">
         <v>115</v>
@@ -1824,7 +1833,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B102" t="s">
         <v>115</v>
@@ -1832,7 +1841,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>170</v>
+        <v>58</v>
       </c>
       <c r="B103" t="s">
         <v>115</v>
@@ -1840,7 +1849,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="B104" t="s">
         <v>115</v>
@@ -1848,7 +1857,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>60</v>
+        <v>170</v>
       </c>
       <c r="B105" t="s">
         <v>116</v>
@@ -1856,7 +1865,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B106" t="s">
         <v>115</v>
@@ -1864,7 +1873,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>173</v>
+        <v>60</v>
       </c>
       <c r="B107" t="s">
         <v>115</v>
@@ -1872,7 +1881,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>61</v>
+        <v>172</v>
       </c>
       <c r="B108" t="s">
         <v>115</v>
@@ -1880,7 +1889,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>62</v>
+        <v>173</v>
       </c>
       <c r="B109" t="s">
         <v>115</v>
@@ -1888,7 +1897,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B110" t="s">
         <v>116</v>
@@ -1896,7 +1905,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>174</v>
+        <v>62</v>
       </c>
       <c r="B111" t="s">
         <v>115</v>
@@ -1904,7 +1913,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B112" t="s">
         <v>115</v>
@@ -1912,7 +1921,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>122</v>
+        <v>174</v>
       </c>
       <c r="B113" t="s">
         <v>115</v>
@@ -1920,7 +1929,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>123</v>
+        <v>64</v>
       </c>
       <c r="B114" t="s">
         <v>116</v>
@@ -1928,7 +1937,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>65</v>
+        <v>122</v>
       </c>
       <c r="B115" t="s">
         <v>115</v>
@@ -1936,7 +1945,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="B116" t="s">
         <v>115</v>
@@ -1944,7 +1953,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B117" t="s">
         <v>115</v>
@@ -1952,7 +1961,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>175</v>
+        <v>66</v>
       </c>
       <c r="B118" t="s">
         <v>115</v>
@@ -1960,7 +1969,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="B119" t="s">
         <v>115</v>
@@ -1968,7 +1977,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>68</v>
+        <v>175</v>
       </c>
       <c r="B120" t="s">
         <v>115</v>
@@ -1976,7 +1985,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>69</v>
+        <v>148</v>
       </c>
       <c r="B121" t="s">
         <v>116</v>
@@ -1984,7 +1993,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B122" t="s">
         <v>115</v>
@@ -1992,7 +2001,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>131</v>
+        <v>69</v>
       </c>
       <c r="B123" t="s">
         <v>115</v>
@@ -2000,7 +2009,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="B124" t="s">
         <v>116</v>
@@ -2008,7 +2017,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>176</v>
+        <v>131</v>
       </c>
       <c r="B125" t="s">
         <v>115</v>
@@ -2016,7 +2025,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="B126" t="s">
         <v>115</v>
@@ -2024,7 +2033,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>124</v>
+        <v>176</v>
       </c>
       <c r="B127" t="s">
         <v>115</v>
@@ -2032,7 +2041,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="B128" t="s">
         <v>115</v>
@@ -2040,7 +2049,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="B129" t="s">
         <v>115</v>
@@ -2048,7 +2057,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="B130" t="s">
         <v>116</v>
@@ -2056,7 +2065,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="B131" t="s">
         <v>115</v>
@@ -2064,7 +2073,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B132" t="s">
         <v>116</v>
@@ -2072,7 +2081,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>177</v>
+        <v>72</v>
       </c>
       <c r="B133" t="s">
         <v>116</v>
@@ -2080,7 +2089,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B134" t="s">
         <v>115</v>
@@ -2088,7 +2097,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
       <c r="B135" t="s">
         <v>115</v>
@@ -2096,7 +2105,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B136" t="s">
         <v>116</v>
@@ -2104,7 +2113,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>133</v>
+        <v>75</v>
       </c>
       <c r="B137" t="s">
         <v>116</v>
@@ -2112,7 +2121,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>178</v>
+        <v>76</v>
       </c>
       <c r="B138" t="s">
         <v>116</v>
@@ -2120,7 +2129,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="B139" t="s">
         <v>116</v>
@@ -2128,7 +2137,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>134</v>
+        <v>178</v>
       </c>
       <c r="B140" t="s">
         <v>115</v>
@@ -2136,7 +2145,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B141" t="s">
         <v>116</v>
@@ -2144,7 +2153,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B142" t="s">
         <v>116</v>
@@ -2152,7 +2161,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="B143" t="s">
         <v>116</v>
@@ -2160,7 +2169,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>79</v>
+        <v>139</v>
       </c>
       <c r="B144" t="s">
         <v>115</v>
@@ -2168,7 +2177,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="B145" t="s">
         <v>115</v>
@@ -2176,7 +2185,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="B146" t="s">
         <v>115</v>
@@ -2184,7 +2193,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B147" t="s">
         <v>116</v>
@@ -2192,7 +2201,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>179</v>
+        <v>119</v>
       </c>
       <c r="B148" t="s">
         <v>115</v>
@@ -2200,7 +2209,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>180</v>
+        <v>81</v>
       </c>
       <c r="B149" t="s">
         <v>116</v>
@@ -2208,7 +2217,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B150" t="s">
         <v>115</v>
@@ -2216,7 +2225,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="B151" t="s">
         <v>115</v>
@@ -2224,7 +2233,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>83</v>
+        <v>181</v>
       </c>
       <c r="B152" t="s">
         <v>116</v>
@@ -2232,7 +2241,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>84</v>
+        <v>207</v>
       </c>
       <c r="B153" t="s">
         <v>115</v>
@@ -2240,7 +2249,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>182</v>
+        <v>82</v>
       </c>
       <c r="B154" t="s">
         <v>115</v>
@@ -2248,7 +2257,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B155" t="s">
         <v>115</v>
@@ -2256,7 +2265,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B156" t="s">
         <v>115</v>
@@ -2264,7 +2273,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B157" t="s">
         <v>115</v>
@@ -2272,7 +2281,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>184</v>
+        <v>85</v>
       </c>
       <c r="B158" t="s">
         <v>115</v>
@@ -2280,7 +2289,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B159" t="s">
         <v>115</v>
@@ -2288,7 +2297,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="B160" t="s">
         <v>115</v>
@@ -2296,7 +2305,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>88</v>
+        <v>184</v>
       </c>
       <c r="B161" t="s">
         <v>115</v>
@@ -2304,7 +2313,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B162" t="s">
         <v>115</v>
@@ -2312,7 +2321,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="B163" t="s">
         <v>116</v>
@@ -2320,7 +2329,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B164" t="s">
         <v>115</v>
@@ -2328,7 +2337,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B165" t="s">
         <v>115</v>
@@ -2336,7 +2345,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="B166" t="s">
         <v>115</v>
@@ -2344,7 +2353,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B167" t="s">
         <v>116</v>
@@ -2352,7 +2361,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>193</v>
+        <v>91</v>
       </c>
       <c r="B168" t="s">
         <v>115</v>
@@ -2360,7 +2369,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>151</v>
+        <v>92</v>
       </c>
       <c r="B169" t="s">
         <v>115</v>
@@ -2368,7 +2377,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>185</v>
+        <v>93</v>
       </c>
       <c r="B170" t="s">
         <v>115</v>
@@ -2376,7 +2385,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>94</v>
+        <v>193</v>
       </c>
       <c r="B171" t="s">
         <v>115</v>
@@ -2384,7 +2393,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="B172" t="s">
         <v>116</v>
@@ -2392,7 +2401,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>96</v>
+        <v>185</v>
       </c>
       <c r="B173" t="s">
         <v>115</v>
@@ -2400,7 +2409,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>186</v>
+        <v>94</v>
       </c>
       <c r="B174" t="s">
         <v>116</v>
@@ -2408,7 +2417,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B175" t="s">
         <v>116</v>
@@ -2416,7 +2425,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B176" t="s">
         <v>116</v>
@@ -2424,7 +2433,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="B177" t="s">
         <v>115</v>
@@ -2432,7 +2441,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B178" t="s">
         <v>115</v>
@@ -2440,7 +2449,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B179" t="s">
         <v>115</v>
@@ -2448,7 +2457,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="B180" t="s">
         <v>115</v>
@@ -2456,7 +2465,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B181" t="s">
         <v>115</v>
@@ -2464,7 +2473,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B182" t="s">
         <v>115</v>
@@ -2472,7 +2481,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B183" t="s">
         <v>115</v>
@@ -2480,7 +2489,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B184" t="s">
         <v>116</v>
@@ -2488,7 +2497,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>204</v>
+        <v>103</v>
       </c>
       <c r="B185" t="s">
         <v>116</v>
@@ -2496,7 +2505,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>187</v>
+        <v>104</v>
       </c>
       <c r="B186" t="s">
         <v>115</v>
@@ -2504,7 +2513,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="B187" t="s">
         <v>116</v>
@@ -2512,7 +2521,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>106</v>
+        <v>204</v>
       </c>
       <c r="B188" t="s">
         <v>116</v>
@@ -2520,7 +2529,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B189" t="s">
         <v>115</v>
@@ -2528,7 +2537,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="B190" t="s">
         <v>115</v>
@@ -2536,7 +2545,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B191" t="s">
         <v>115</v>
@@ -2544,7 +2553,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="B192" t="s">
         <v>116</v>
@@ -2552,7 +2561,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B193" t="s">
         <v>115</v>
@@ -2560,7 +2569,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>190</v>
+        <v>107</v>
       </c>
       <c r="B194" t="s">
         <v>116</v>
@@ -2568,7 +2577,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>108</v>
+        <v>152</v>
       </c>
       <c r="B195" t="s">
         <v>115</v>
@@ -2576,7 +2585,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>109</v>
+        <v>198</v>
       </c>
       <c r="B196" t="s">
         <v>115</v>
@@ -2584,7 +2593,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>110</v>
+        <v>190</v>
       </c>
       <c r="B197" t="s">
         <v>115</v>
@@ -2592,7 +2601,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B198" t="s">
         <v>116</v>
@@ -2600,7 +2609,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B199" t="s">
         <v>115</v>
@@ -2608,7 +2617,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B200" t="s">
         <v>116</v>
@@ -2616,7 +2625,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B201" t="s">
         <v>115</v>
@@ -2624,10 +2633,25 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
+        <v>112</v>
+      </c>
+      <c r="B202" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
         <v>191</v>
-      </c>
-      <c r="B202" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated care data (v32)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFB62D4-DBE0-4600-B34B-918592926499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26348C41-8478-4D31-89AC-3C9E43347EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="2400" windowWidth="24320" windowHeight="19200" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="7240" yWindow="560" windowWidth="24540" windowHeight="14300" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="210">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -565,9 +565,6 @@
     <t>Robert Coppes Stichting</t>
   </si>
   <si>
-    <t>Schärwachter B.V.</t>
-  </si>
-  <si>
     <t>Sterk Huis (Stichting) (West Brabant was voorheen Juzt)</t>
   </si>
   <si>
@@ -653,6 +650,15 @@
   </si>
   <si>
     <t>Swinhove Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Amstelring Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Teamzorg B.V.</t>
+  </si>
+  <si>
+    <t>Zorggroep Florence (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1019,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B205"/>
+  <dimension ref="A1:B207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1065,7 +1071,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" t="s">
         <v>116</v>
@@ -1073,7 +1079,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B7" t="s">
         <v>116</v>
@@ -1113,7 +1119,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B12" t="s">
         <v>115</v>
@@ -1129,23 +1135,23 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>207</v>
       </c>
       <c r="B14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>154</v>
       </c>
       <c r="B16" t="s">
         <v>115</v>
@@ -1153,7 +1159,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
         <v>115</v>
@@ -1161,7 +1167,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
         <v>115</v>
@@ -1169,7 +1175,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>115</v>
@@ -1177,7 +1183,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
         <v>115</v>
@@ -1185,23 +1191,23 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
         <v>115</v>
@@ -1209,7 +1215,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
         <v>115</v>
@@ -1217,7 +1223,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="B25" t="s">
         <v>115</v>
@@ -1225,15 +1231,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>144</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
         <v>116</v>
@@ -1241,7 +1247,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="B28" t="s">
         <v>116</v>
@@ -1249,7 +1255,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>201</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
         <v>116</v>
@@ -1257,7 +1263,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>200</v>
       </c>
       <c r="B30" t="s">
         <v>116</v>
@@ -1265,15 +1271,15 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
         <v>115</v>
@@ -1281,39 +1287,39 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B34" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>157</v>
       </c>
       <c r="B35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>140</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
         <v>115</v>
@@ -1321,7 +1327,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B38" t="s">
         <v>115</v>
@@ -1329,15 +1335,15 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
       <c r="B39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>205</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
         <v>116</v>
@@ -1345,7 +1351,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B41" t="s">
         <v>116</v>
@@ -1353,23 +1359,23 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>126</v>
+        <v>205</v>
       </c>
       <c r="B42" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>158</v>
       </c>
       <c r="B44" t="s">
         <v>116</v>
@@ -1377,7 +1383,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>127</v>
+        <v>24</v>
       </c>
       <c r="B45" t="s">
         <v>116</v>
@@ -1385,15 +1391,15 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>159</v>
       </c>
       <c r="B47" t="s">
         <v>115</v>
@@ -1401,7 +1407,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B48" t="s">
         <v>115</v>
@@ -1409,7 +1415,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B49" t="s">
         <v>115</v>
@@ -1417,15 +1423,15 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>160</v>
+        <v>28</v>
       </c>
       <c r="B51" t="s">
         <v>116</v>
@@ -1433,39 +1439,39 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>29</v>
+        <v>160</v>
       </c>
       <c r="B52" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>192</v>
+        <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
       <c r="B54" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>161</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="B56" t="s">
         <v>116</v>
@@ -1473,23 +1479,23 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>31</v>
+        <v>194</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="B59" t="s">
         <v>116</v>
@@ -1497,7 +1503,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B60" t="s">
         <v>115</v>
@@ -1505,31 +1511,31 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>141</v>
+        <v>33</v>
       </c>
       <c r="B61" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>34</v>
+        <v>141</v>
       </c>
       <c r="B62" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>162</v>
+        <v>34</v>
       </c>
       <c r="B63" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>162</v>
       </c>
       <c r="B64" t="s">
         <v>115</v>
@@ -1537,23 +1543,23 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>196</v>
+        <v>35</v>
       </c>
       <c r="B65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>36</v>
+        <v>195</v>
       </c>
       <c r="B66" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>163</v>
+        <v>36</v>
       </c>
       <c r="B67" t="s">
         <v>115</v>
@@ -1561,15 +1567,15 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>37</v>
+        <v>163</v>
       </c>
       <c r="B68" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>164</v>
+        <v>37</v>
       </c>
       <c r="B69" t="s">
         <v>115</v>
@@ -1577,15 +1583,15 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>38</v>
+        <v>164</v>
       </c>
       <c r="B70" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B71" t="s">
         <v>115</v>
@@ -1593,15 +1599,15 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>202</v>
+        <v>39</v>
       </c>
       <c r="B72" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>40</v>
+        <v>201</v>
       </c>
       <c r="B73" t="s">
         <v>116</v>
@@ -1609,7 +1615,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B74" t="s">
         <v>115</v>
@@ -1617,7 +1623,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>165</v>
+        <v>41</v>
       </c>
       <c r="B75" t="s">
         <v>116</v>
@@ -1625,15 +1631,15 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="B76" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>42</v>
+        <v>146</v>
       </c>
       <c r="B77" t="s">
         <v>115</v>
@@ -1641,15 +1647,15 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B78" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B79" t="s">
         <v>115</v>
@@ -1657,7 +1663,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>166</v>
+        <v>44</v>
       </c>
       <c r="B80" t="s">
         <v>115</v>
@@ -1665,7 +1671,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B81" t="s">
         <v>115</v>
@@ -1673,7 +1679,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>45</v>
+        <v>167</v>
       </c>
       <c r="B82" t="s">
         <v>115</v>
@@ -1681,23 +1687,23 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>203</v>
+        <v>45</v>
       </c>
       <c r="B83" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>46</v>
+        <v>202</v>
       </c>
       <c r="B84" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B85" t="s">
         <v>115</v>
@@ -1705,7 +1711,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="B86" t="s">
         <v>116</v>
@@ -1713,15 +1719,15 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="B87" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B88" t="s">
         <v>115</v>
@@ -1729,23 +1735,23 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>48</v>
+        <v>169</v>
       </c>
       <c r="B89" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B90" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B91" t="s">
         <v>115</v>
@@ -1753,7 +1759,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>197</v>
+        <v>50</v>
       </c>
       <c r="B92" t="s">
         <v>115</v>
@@ -1761,15 +1767,15 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>147</v>
+        <v>196</v>
       </c>
       <c r="B93" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="B94" t="s">
         <v>115</v>
@@ -1777,7 +1783,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B95" t="s">
         <v>115</v>
@@ -1785,7 +1791,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="B96" t="s">
         <v>115</v>
@@ -1793,7 +1799,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="B97" t="s">
         <v>115</v>
@@ -1801,55 +1807,55 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B98" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B99" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>130</v>
+        <v>55</v>
       </c>
       <c r="B100" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="B101" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B102" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B103" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B104" t="s">
         <v>115</v>
@@ -1857,15 +1863,15 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>170</v>
+        <v>59</v>
       </c>
       <c r="B105" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B106" t="s">
         <v>115</v>
@@ -1873,7 +1879,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>60</v>
+        <v>171</v>
       </c>
       <c r="B107" t="s">
         <v>115</v>
@@ -1881,15 +1887,15 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>172</v>
+        <v>60</v>
       </c>
       <c r="B108" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B109" t="s">
         <v>115</v>
@@ -1897,15 +1903,15 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>61</v>
+        <v>173</v>
       </c>
       <c r="B110" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B111" t="s">
         <v>115</v>
@@ -1913,7 +1919,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B112" t="s">
         <v>115</v>
@@ -1921,23 +1927,23 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>174</v>
+        <v>63</v>
       </c>
       <c r="B113" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="B114" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>122</v>
+        <v>64</v>
       </c>
       <c r="B115" t="s">
         <v>115</v>
@@ -1945,7 +1951,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B116" t="s">
         <v>115</v>
@@ -1953,15 +1959,15 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="B117" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B118" t="s">
         <v>115</v>
@@ -1969,7 +1975,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B119" t="s">
         <v>115</v>
@@ -1977,7 +1983,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>175</v>
+        <v>67</v>
       </c>
       <c r="B120" t="s">
         <v>115</v>
@@ -1985,15 +1991,15 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="B121" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="B122" t="s">
         <v>115</v>
@@ -2001,7 +2007,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B123" t="s">
         <v>115</v>
@@ -2009,7 +2015,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B124" t="s">
         <v>116</v>
@@ -2017,7 +2023,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
       <c r="B125" t="s">
         <v>115</v>
@@ -2025,7 +2031,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B126" t="s">
         <v>115</v>
@@ -2033,15 +2039,15 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>176</v>
+        <v>132</v>
       </c>
       <c r="B127" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="B128" t="s">
         <v>115</v>
@@ -2049,7 +2055,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="B129" t="s">
         <v>115</v>
@@ -2057,15 +2063,15 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B130" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B131" t="s">
         <v>115</v>
@@ -2073,15 +2079,15 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="B132" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B133" t="s">
         <v>116</v>
@@ -2089,7 +2095,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B134" t="s">
         <v>115</v>
@@ -2097,15 +2103,15 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>177</v>
+        <v>73</v>
       </c>
       <c r="B135" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="B136" t="s">
         <v>116</v>
@@ -2113,23 +2119,23 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B137" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B138" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="B139" t="s">
         <v>116</v>
@@ -2137,10 +2143,10 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>178</v>
+        <v>133</v>
       </c>
       <c r="B140" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
@@ -2156,7 +2162,7 @@
         <v>134</v>
       </c>
       <c r="B142" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
@@ -2172,7 +2178,7 @@
         <v>139</v>
       </c>
       <c r="B144" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -2180,7 +2186,7 @@
         <v>142</v>
       </c>
       <c r="B145" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
@@ -2196,7 +2202,7 @@
         <v>80</v>
       </c>
       <c r="B147" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -2217,7 +2223,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B150" t="s">
         <v>115</v>
@@ -2225,26 +2231,26 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B151" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B152" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B153" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
@@ -2260,12 +2266,12 @@
         <v>83</v>
       </c>
       <c r="B155" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>84</v>
+        <v>208</v>
       </c>
       <c r="B156" t="s">
         <v>115</v>
@@ -2273,7 +2279,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>182</v>
+        <v>84</v>
       </c>
       <c r="B157" t="s">
         <v>115</v>
@@ -2281,7 +2287,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="B158" t="s">
         <v>115</v>
@@ -2289,7 +2295,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B159" t="s">
         <v>115</v>
@@ -2297,7 +2303,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>183</v>
+        <v>86</v>
       </c>
       <c r="B160" t="s">
         <v>115</v>
@@ -2305,7 +2311,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B161" t="s">
         <v>115</v>
@@ -2313,7 +2319,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>87</v>
+        <v>183</v>
       </c>
       <c r="B162" t="s">
         <v>115</v>
@@ -2321,15 +2327,15 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>143</v>
+        <v>87</v>
       </c>
       <c r="B163" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="B164" t="s">
         <v>115</v>
@@ -2337,7 +2343,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B165" t="s">
         <v>115</v>
@@ -2345,7 +2351,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="B166" t="s">
         <v>115</v>
@@ -2353,7 +2359,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="B167" t="s">
         <v>116</v>
@@ -2361,7 +2367,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B168" t="s">
         <v>115</v>
@@ -2369,7 +2375,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B169" t="s">
         <v>115</v>
@@ -2377,7 +2383,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B170" t="s">
         <v>115</v>
@@ -2385,23 +2391,23 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>193</v>
+        <v>93</v>
       </c>
       <c r="B171" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="B172" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="B173" t="s">
         <v>115</v>
@@ -2409,23 +2415,23 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="B174" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B175" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B176" t="s">
         <v>116</v>
@@ -2433,7 +2439,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>186</v>
+        <v>96</v>
       </c>
       <c r="B177" t="s">
         <v>115</v>
@@ -2441,31 +2447,31 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>97</v>
+        <v>185</v>
       </c>
       <c r="B178" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B179" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="B180" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="B181" t="s">
         <v>115</v>
@@ -2473,7 +2479,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B182" t="s">
         <v>115</v>
@@ -2481,7 +2487,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B183" t="s">
         <v>115</v>
@@ -2489,23 +2495,23 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B184" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B185" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B186" t="s">
         <v>115</v>
@@ -2513,15 +2519,15 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B187" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>204</v>
+        <v>105</v>
       </c>
       <c r="B188" t="s">
         <v>116</v>
@@ -2529,15 +2535,15 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="B189" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>135</v>
+        <v>186</v>
       </c>
       <c r="B190" t="s">
         <v>115</v>
@@ -2545,15 +2551,15 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="B191" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>188</v>
+        <v>106</v>
       </c>
       <c r="B192" t="s">
         <v>116</v>
@@ -2561,7 +2567,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B193" t="s">
         <v>115</v>
@@ -2569,15 +2575,15 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>107</v>
+        <v>188</v>
       </c>
       <c r="B194" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>152</v>
+        <v>107</v>
       </c>
       <c r="B195" t="s">
         <v>115</v>
@@ -2585,7 +2591,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="B196" t="s">
         <v>115</v>
@@ -2593,39 +2599,39 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
       <c r="B197" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>108</v>
+        <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>109</v>
+        <v>189</v>
       </c>
       <c r="B199" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B200" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B201" t="s">
         <v>115</v>
@@ -2633,25 +2639,50 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B202" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="B203" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>114</v>
+        <v>112</v>
+      </c>
+      <c r="B204" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>191</v>
+        <v>113</v>
+      </c>
+      <c r="B205" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>114</v>
+      </c>
+      <c r="B206" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>190</v>
+      </c>
+      <c r="B207" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated care data (v33)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26348C41-8478-4D31-89AC-3C9E43347EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E90C03-BAF9-4E43-991D-E1FAC16A402E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="560" windowWidth="24540" windowHeight="14300" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="22560" windowHeight="20660" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="212">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -659,6 +659,12 @@
   </si>
   <si>
     <t>Zorggroep Florence (Stichting)</t>
+  </si>
+  <si>
+    <t>Mariënstede (Stichting) (incl. Vughterstede)</t>
+  </si>
+  <si>
+    <t>Schärwachter B.V.</t>
   </si>
 </sst>
 </file>
@@ -1019,9 +1025,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B207"/>
+  <dimension ref="A1:B209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1799,15 +1807,15 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>129</v>
+        <v>210</v>
       </c>
       <c r="B97" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="B98" t="s">
         <v>115</v>
@@ -1815,7 +1823,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B99" t="s">
         <v>115</v>
@@ -1823,7 +1831,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B100" t="s">
         <v>115</v>
@@ -1831,15 +1839,15 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>130</v>
+        <v>55</v>
       </c>
       <c r="B101" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="B102" t="s">
         <v>116</v>
@@ -1847,7 +1855,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B103" t="s">
         <v>116</v>
@@ -1855,15 +1863,15 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B104" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B105" t="s">
         <v>115</v>
@@ -1871,7 +1879,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>170</v>
+        <v>59</v>
       </c>
       <c r="B106" t="s">
         <v>115</v>
@@ -1879,7 +1887,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B107" t="s">
         <v>115</v>
@@ -1887,23 +1895,23 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>60</v>
+        <v>171</v>
       </c>
       <c r="B108" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>172</v>
+        <v>60</v>
       </c>
       <c r="B109" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B110" t="s">
         <v>115</v>
@@ -1911,7 +1919,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>61</v>
+        <v>173</v>
       </c>
       <c r="B111" t="s">
         <v>115</v>
@@ -1919,7 +1927,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B112" t="s">
         <v>115</v>
@@ -1927,23 +1935,23 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B113" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>174</v>
+        <v>63</v>
       </c>
       <c r="B114" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="B115" t="s">
         <v>115</v>
@@ -1951,7 +1959,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>122</v>
+        <v>64</v>
       </c>
       <c r="B116" t="s">
         <v>115</v>
@@ -1959,23 +1967,23 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="B118" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B119" t="s">
         <v>115</v>
@@ -1983,7 +1991,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B120" t="s">
         <v>115</v>
@@ -1991,7 +1999,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>175</v>
+        <v>67</v>
       </c>
       <c r="B121" t="s">
         <v>115</v>
@@ -1999,7 +2007,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="B122" t="s">
         <v>115</v>
@@ -2007,7 +2015,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="B123" t="s">
         <v>115</v>
@@ -2015,23 +2023,23 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B124" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B125" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
       <c r="B126" t="s">
         <v>115</v>
@@ -2039,23 +2047,23 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B127" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>176</v>
+        <v>132</v>
       </c>
       <c r="B128" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="B129" t="s">
         <v>115</v>
@@ -2063,7 +2071,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="B130" t="s">
         <v>115</v>
@@ -2071,7 +2079,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B131" t="s">
         <v>115</v>
@@ -2079,7 +2087,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B132" t="s">
         <v>115</v>
@@ -2087,31 +2095,31 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="B133" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B134" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B135" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>177</v>
+        <v>73</v>
       </c>
       <c r="B136" t="s">
         <v>116</v>
@@ -2119,15 +2127,15 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="B137" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B138" t="s">
         <v>115</v>
@@ -2135,15 +2143,15 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B139" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="B140" t="s">
         <v>116</v>
@@ -2151,7 +2159,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="B141" t="s">
         <v>116</v>
@@ -2159,15 +2167,15 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>134</v>
+        <v>211</v>
       </c>
       <c r="B142" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B143" t="s">
         <v>116</v>
@@ -2175,15 +2183,15 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B144" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="B145" t="s">
         <v>116</v>
@@ -2191,23 +2199,23 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>79</v>
+        <v>139</v>
       </c>
       <c r="B146" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="B147" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="B148" t="s">
         <v>115</v>
@@ -2215,15 +2223,15 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B149" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="B150" t="s">
         <v>115</v>
@@ -2231,7 +2239,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>179</v>
+        <v>81</v>
       </c>
       <c r="B151" t="s">
         <v>116</v>
@@ -2239,7 +2247,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B152" t="s">
         <v>115</v>
@@ -2247,7 +2255,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="B153" t="s">
         <v>116</v>
@@ -2255,7 +2263,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="B154" t="s">
         <v>115</v>
@@ -2263,7 +2271,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>83</v>
+        <v>206</v>
       </c>
       <c r="B155" t="s">
         <v>116</v>
@@ -2271,7 +2279,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>208</v>
+        <v>82</v>
       </c>
       <c r="B156" t="s">
         <v>115</v>
@@ -2279,15 +2287,15 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B157" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>181</v>
+        <v>208</v>
       </c>
       <c r="B158" t="s">
         <v>115</v>
@@ -2295,7 +2303,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B159" t="s">
         <v>115</v>
@@ -2303,7 +2311,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>86</v>
+        <v>181</v>
       </c>
       <c r="B160" t="s">
         <v>115</v>
@@ -2311,7 +2319,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>182</v>
+        <v>85</v>
       </c>
       <c r="B161" t="s">
         <v>115</v>
@@ -2319,7 +2327,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>183</v>
+        <v>86</v>
       </c>
       <c r="B162" t="s">
         <v>115</v>
@@ -2327,7 +2335,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>87</v>
+        <v>182</v>
       </c>
       <c r="B163" t="s">
         <v>115</v>
@@ -2335,7 +2343,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="B164" t="s">
         <v>115</v>
@@ -2343,7 +2351,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B165" t="s">
         <v>115</v>
@@ -2351,7 +2359,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
       <c r="B166" t="s">
         <v>115</v>
@@ -2359,15 +2367,15 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="B167" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B168" t="s">
         <v>115</v>
@@ -2375,15 +2383,15 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="B169" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B170" t="s">
         <v>115</v>
@@ -2391,15 +2399,15 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B171" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>192</v>
+        <v>92</v>
       </c>
       <c r="B172" t="s">
         <v>115</v>
@@ -2407,15 +2415,15 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>151</v>
+        <v>93</v>
       </c>
       <c r="B173" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B174" t="s">
         <v>115</v>
@@ -2423,7 +2431,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="B175" t="s">
         <v>115</v>
@@ -2431,15 +2439,15 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>95</v>
+        <v>184</v>
       </c>
       <c r="B176" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B177" t="s">
         <v>115</v>
@@ -2447,7 +2455,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>185</v>
+        <v>95</v>
       </c>
       <c r="B178" t="s">
         <v>116</v>
@@ -2455,15 +2463,15 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B179" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>98</v>
+        <v>185</v>
       </c>
       <c r="B180" t="s">
         <v>116</v>
@@ -2471,23 +2479,23 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="B181" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B182" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="B183" t="s">
         <v>115</v>
@@ -2495,7 +2503,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B184" t="s">
         <v>115</v>
@@ -2503,7 +2511,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B185" t="s">
         <v>115</v>
@@ -2511,7 +2519,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B186" t="s">
         <v>115</v>
@@ -2519,7 +2527,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B187" t="s">
         <v>115</v>
@@ -2527,31 +2535,31 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B188" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="B189" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>186</v>
+        <v>105</v>
       </c>
       <c r="B190" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>135</v>
+        <v>203</v>
       </c>
       <c r="B191" t="s">
         <v>116</v>
@@ -2559,31 +2567,31 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>106</v>
+        <v>186</v>
       </c>
       <c r="B192" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>187</v>
+        <v>135</v>
       </c>
       <c r="B193" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>188</v>
+        <v>106</v>
       </c>
       <c r="B194" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>107</v>
+        <v>187</v>
       </c>
       <c r="B195" t="s">
         <v>115</v>
@@ -2591,7 +2599,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="B196" t="s">
         <v>115</v>
@@ -2599,15 +2607,15 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>152</v>
+        <v>107</v>
       </c>
       <c r="B197" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="B198" t="s">
         <v>115</v>
@@ -2615,7 +2623,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="B199" t="s">
         <v>116</v>
@@ -2623,7 +2631,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>108</v>
+        <v>197</v>
       </c>
       <c r="B200" t="s">
         <v>115</v>
@@ -2631,39 +2639,39 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>109</v>
+        <v>189</v>
       </c>
       <c r="B201" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B202" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B203" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B204" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B205" t="s">
         <v>116</v>
@@ -2671,7 +2679,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B206" t="s">
         <v>115</v>
@@ -2679,9 +2687,25 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
+        <v>113</v>
+      </c>
+      <c r="B207" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>114</v>
+      </c>
+      <c r="B208" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
         <v>190</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B209" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update care data (v34).
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E90C03-BAF9-4E43-991D-E1FAC16A402E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222957A1-D206-4D7C-83D7-9F5D09533BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="22560" windowHeight="20660" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="2800" yWindow="1480" windowWidth="20920" windowHeight="18800" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="211">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -322,9 +322,6 @@
     <t>WilgaerdenLeekerweide Groep (Stichting)</t>
   </si>
   <si>
-    <t>Woon en zorgcentrum de Merwelanden, stichting</t>
-  </si>
-  <si>
     <t>Woonzorg Samen (Stichting)</t>
   </si>
   <si>
@@ -661,10 +658,10 @@
     <t>Zorggroep Florence (Stichting)</t>
   </si>
   <si>
-    <t>Mariënstede (Stichting) (incl. Vughterstede)</t>
-  </si>
-  <si>
     <t>Schärwachter B.V.</t>
+  </si>
+  <si>
+    <t>Kwintes (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1022,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B209"/>
+  <dimension ref="A1:B208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1047,10 +1044,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1058,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1066,7 +1063,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1074,23 +1071,23 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1098,15 +1095,15 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1114,7 +1111,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1122,31 +1119,31 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -1154,15 +1151,15 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1170,7 +1167,7 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -1178,7 +1175,7 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -1186,7 +1183,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1194,15 +1191,15 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -1210,7 +1207,7 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -1218,7 +1215,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1226,15 +1223,15 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1242,7 +1239,7 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -1250,31 +1247,31 @@
         <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -1282,7 +1279,7 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -1290,7 +1287,7 @@
         <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -1298,23 +1295,23 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -1322,7 +1319,7 @@
         <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -1330,23 +1327,23 @@
         <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1354,39 +1351,39 @@
         <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1394,23 +1391,23 @@
         <v>24</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -1418,7 +1415,7 @@
         <v>25</v>
       </c>
       <c r="B48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -1426,7 +1423,7 @@
         <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1434,7 +1431,7 @@
         <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -1442,15 +1439,15 @@
         <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -1458,15 +1455,15 @@
         <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -1474,23 +1471,23 @@
         <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B56" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -1498,7 +1495,7 @@
         <v>31</v>
       </c>
       <c r="B58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -1506,15 +1503,15 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -1522,15 +1519,15 @@
         <v>33</v>
       </c>
       <c r="B61" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B62" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -1538,15 +1535,15 @@
         <v>34</v>
       </c>
       <c r="B63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B64" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
@@ -1554,15 +1551,15 @@
         <v>35</v>
       </c>
       <c r="B65" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B66" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
@@ -1570,15 +1567,15 @@
         <v>36</v>
       </c>
       <c r="B67" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
@@ -1586,15 +1583,15 @@
         <v>37</v>
       </c>
       <c r="B69" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B70" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
@@ -1602,7 +1599,7 @@
         <v>38</v>
       </c>
       <c r="B71" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -1610,15 +1607,15 @@
         <v>39</v>
       </c>
       <c r="B72" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B73" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -1626,7 +1623,7 @@
         <v>40</v>
       </c>
       <c r="B74" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -1634,23 +1631,23 @@
         <v>41</v>
       </c>
       <c r="B75" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B77" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
@@ -1658,7 +1655,7 @@
         <v>42</v>
       </c>
       <c r="B78" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -1666,7 +1663,7 @@
         <v>43</v>
       </c>
       <c r="B79" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
@@ -1674,23 +1671,23 @@
         <v>44</v>
       </c>
       <c r="B80" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B82" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -1698,15 +1695,15 @@
         <v>45</v>
       </c>
       <c r="B83" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B84" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -1714,28 +1711,28 @@
         <v>46</v>
       </c>
       <c r="B85" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>47</v>
+        <v>210</v>
       </c>
       <c r="B86" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="B87" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="B88" t="s">
         <v>115</v>
@@ -1743,15 +1740,15 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B89" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>48</v>
+        <v>168</v>
       </c>
       <c r="B90" t="s">
         <v>115</v>
@@ -1759,31 +1756,31 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B91" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B92" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>196</v>
+        <v>50</v>
       </c>
       <c r="B93" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>147</v>
+        <v>195</v>
       </c>
       <c r="B94" t="s">
         <v>115</v>
@@ -1791,34 +1788,34 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="B95" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B96" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>210</v>
+        <v>52</v>
       </c>
       <c r="B97" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B98" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -1826,7 +1823,7 @@
         <v>53</v>
       </c>
       <c r="B99" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -1834,7 +1831,7 @@
         <v>54</v>
       </c>
       <c r="B100" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
@@ -1842,15 +1839,15 @@
         <v>55</v>
       </c>
       <c r="B101" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B102" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -1858,7 +1855,7 @@
         <v>56</v>
       </c>
       <c r="B103" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
@@ -1866,7 +1863,7 @@
         <v>57</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
@@ -1874,7 +1871,7 @@
         <v>58</v>
       </c>
       <c r="B105" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
@@ -1882,23 +1879,23 @@
         <v>59</v>
       </c>
       <c r="B106" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B107" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B108" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -1906,23 +1903,23 @@
         <v>60</v>
       </c>
       <c r="B109" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B110" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B111" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -1930,7 +1927,7 @@
         <v>61</v>
       </c>
       <c r="B112" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -1938,7 +1935,7 @@
         <v>62</v>
       </c>
       <c r="B113" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
@@ -1946,15 +1943,15 @@
         <v>63</v>
       </c>
       <c r="B114" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B115" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -1962,23 +1959,23 @@
         <v>64</v>
       </c>
       <c r="B116" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B117" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B118" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
@@ -1986,7 +1983,7 @@
         <v>65</v>
       </c>
       <c r="B119" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
@@ -1994,7 +1991,7 @@
         <v>66</v>
       </c>
       <c r="B120" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -2002,23 +1999,23 @@
         <v>67</v>
       </c>
       <c r="B121" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B122" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B123" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -2026,7 +2023,7 @@
         <v>68</v>
       </c>
       <c r="B124" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -2034,7 +2031,7 @@
         <v>69</v>
       </c>
       <c r="B125" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
@@ -2042,63 +2039,63 @@
         <v>70</v>
       </c>
       <c r="B126" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B127" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B128" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B129" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B130" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B131" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B132" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B133" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
@@ -2106,7 +2103,7 @@
         <v>71</v>
       </c>
       <c r="B134" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
@@ -2114,7 +2111,7 @@
         <v>72</v>
       </c>
       <c r="B135" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -2122,15 +2119,15 @@
         <v>73</v>
       </c>
       <c r="B136" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B137" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
@@ -2138,7 +2135,7 @@
         <v>74</v>
       </c>
       <c r="B138" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
@@ -2146,7 +2143,7 @@
         <v>75</v>
       </c>
       <c r="B139" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
@@ -2154,23 +2151,23 @@
         <v>76</v>
       </c>
       <c r="B140" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B141" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B142" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
@@ -2178,15 +2175,15 @@
         <v>77</v>
       </c>
       <c r="B143" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B144" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -2194,23 +2191,23 @@
         <v>78</v>
       </c>
       <c r="B145" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B146" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B147" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -2218,7 +2215,7 @@
         <v>79</v>
       </c>
       <c r="B148" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
@@ -2226,15 +2223,15 @@
         <v>80</v>
       </c>
       <c r="B149" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B150" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
@@ -2242,39 +2239,39 @@
         <v>81</v>
       </c>
       <c r="B151" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B152" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B153" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B154" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B155" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
@@ -2282,7 +2279,7 @@
         <v>82</v>
       </c>
       <c r="B156" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
@@ -2290,15 +2287,15 @@
         <v>83</v>
       </c>
       <c r="B157" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B158" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
@@ -2306,15 +2303,15 @@
         <v>84</v>
       </c>
       <c r="B159" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B160" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
@@ -2322,7 +2319,7 @@
         <v>85</v>
       </c>
       <c r="B161" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
@@ -2330,23 +2327,23 @@
         <v>86</v>
       </c>
       <c r="B162" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B163" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B164" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
@@ -2354,15 +2351,15 @@
         <v>87</v>
       </c>
       <c r="B165" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B166" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
@@ -2370,7 +2367,7 @@
         <v>88</v>
       </c>
       <c r="B167" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
@@ -2378,15 +2375,15 @@
         <v>89</v>
       </c>
       <c r="B168" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B169" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
@@ -2394,7 +2391,7 @@
         <v>90</v>
       </c>
       <c r="B170" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
@@ -2402,7 +2399,7 @@
         <v>91</v>
       </c>
       <c r="B171" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -2410,7 +2407,7 @@
         <v>92</v>
       </c>
       <c r="B172" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
@@ -2418,31 +2415,31 @@
         <v>93</v>
       </c>
       <c r="B173" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B174" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B175" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B176" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
@@ -2450,7 +2447,7 @@
         <v>94</v>
       </c>
       <c r="B177" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -2458,7 +2455,7 @@
         <v>95</v>
       </c>
       <c r="B178" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
@@ -2466,15 +2463,15 @@
         <v>96</v>
       </c>
       <c r="B179" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B180" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
@@ -2482,23 +2479,23 @@
         <v>97</v>
       </c>
       <c r="B181" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="B182" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="B183" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -2506,7 +2503,7 @@
         <v>99</v>
       </c>
       <c r="B184" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
@@ -2514,7 +2511,7 @@
         <v>100</v>
       </c>
       <c r="B185" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
@@ -2522,7 +2519,7 @@
         <v>101</v>
       </c>
       <c r="B186" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
@@ -2530,7 +2527,7 @@
         <v>102</v>
       </c>
       <c r="B187" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
@@ -2538,7 +2535,7 @@
         <v>103</v>
       </c>
       <c r="B188" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
@@ -2551,23 +2548,23 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>105</v>
+        <v>202</v>
       </c>
       <c r="B190" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="B191" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>186</v>
+        <v>134</v>
       </c>
       <c r="B192" t="s">
         <v>115</v>
@@ -2575,18 +2572,18 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="B193" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>106</v>
+        <v>186</v>
       </c>
       <c r="B194" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
@@ -2594,28 +2591,28 @@
         <v>187</v>
       </c>
       <c r="B195" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>188</v>
+        <v>106</v>
       </c>
       <c r="B196" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>107</v>
+        <v>208</v>
       </c>
       <c r="B197" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>209</v>
+        <v>151</v>
       </c>
       <c r="B198" t="s">
         <v>115</v>
@@ -2623,15 +2620,15 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>152</v>
+        <v>196</v>
       </c>
       <c r="B199" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B200" t="s">
         <v>115</v>
@@ -2639,10 +2636,10 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>189</v>
+        <v>107</v>
       </c>
       <c r="B201" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
@@ -2650,7 +2647,7 @@
         <v>108</v>
       </c>
       <c r="B202" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
@@ -2666,7 +2663,7 @@
         <v>110</v>
       </c>
       <c r="B204" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
@@ -2674,7 +2671,7 @@
         <v>111</v>
       </c>
       <c r="B205" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
@@ -2690,23 +2687,15 @@
         <v>113</v>
       </c>
       <c r="B207" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>114</v>
+        <v>189</v>
       </c>
       <c r="B208" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A209" t="s">
-        <v>190</v>
-      </c>
-      <c r="B209" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data, for v36
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222957A1-D206-4D7C-83D7-9F5D09533BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D653E80-102D-481C-915B-E8064EDD2DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="1480" windowWidth="20920" windowHeight="18800" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="17930" yWindow="2410" windowWidth="20040" windowHeight="18180" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="225">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -662,6 +662,48 @@
   </si>
   <si>
     <t>Kwintes (Stichting)</t>
+  </si>
+  <si>
+    <t>Careander (Stichting)</t>
+  </si>
+  <si>
+    <t>Cedrah (Stichting)</t>
+  </si>
+  <si>
+    <t>De Wijngaerd (Stichting)</t>
+  </si>
+  <si>
+    <t>Het Gastenhuis B.V.</t>
+  </si>
+  <si>
+    <t>Landelijke Stichting Vredenoord</t>
+  </si>
+  <si>
+    <t>Mariënstede (Stichting) (incl. Vughterstede)</t>
+  </si>
+  <si>
+    <t>Profila Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Rivas Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>RST Zorgverleners, RST Zorgverleners Waardenland, RST Zorgverleners (Zwolle) (Stichting)</t>
+  </si>
+  <si>
+    <t>Vanboeijen</t>
+  </si>
+  <si>
+    <t>Woon en zorgcentrum de Merwelanden, stichting</t>
+  </si>
+  <si>
+    <t>Woon- en Zorgcentrum Humanitas (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorggroep Triade B.V. (incl. Vitree)</t>
+  </si>
+  <si>
+    <t>Zuyderland Zorg (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -1022,11 +1064,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B208"/>
+  <dimension ref="A1:B222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1087,7 +1127,7 @@
         <v>197</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1095,7 +1135,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1247,7 +1287,7 @@
         <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -1284,7 +1324,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>211</v>
       </c>
       <c r="B32" t="s">
         <v>114</v>
@@ -1292,7 +1332,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" t="s">
         <v>114</v>
@@ -1300,31 +1340,31 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>212</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="B37" t="s">
         <v>114</v>
@@ -1332,15 +1372,15 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>139</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>136</v>
+        <v>22</v>
       </c>
       <c r="B39" t="s">
         <v>114</v>
@@ -1348,39 +1388,39 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>203</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>204</v>
+        <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>125</v>
+        <v>203</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>157</v>
+        <v>204</v>
       </c>
       <c r="B44" t="s">
         <v>115</v>
@@ -1388,15 +1428,15 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>126</v>
+        <v>213</v>
       </c>
       <c r="B46" t="s">
         <v>115</v>
@@ -1404,7 +1444,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B47" t="s">
         <v>114</v>
@@ -1412,15 +1452,15 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="B49" t="s">
         <v>114</v>
@@ -1428,7 +1468,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="B50" t="s">
         <v>114</v>
@@ -1436,23 +1476,23 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>26</v>
       </c>
       <c r="B52" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
         <v>114</v>
@@ -1460,7 +1500,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>190</v>
+        <v>28</v>
       </c>
       <c r="B54" t="s">
         <v>115</v>
@@ -1468,23 +1508,23 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>30</v>
+        <v>159</v>
       </c>
       <c r="B55" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>160</v>
+        <v>29</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B57" t="s">
         <v>115</v>
@@ -1492,15 +1532,15 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>32</v>
+        <v>160</v>
       </c>
       <c r="B59" t="s">
         <v>115</v>
@@ -1508,23 +1548,23 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
       <c r="B60" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B61" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>140</v>
+        <v>32</v>
       </c>
       <c r="B62" t="s">
         <v>115</v>
@@ -1532,7 +1572,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="B63" t="s">
         <v>114</v>
@@ -1540,7 +1580,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>161</v>
+        <v>33</v>
       </c>
       <c r="B64" t="s">
         <v>114</v>
@@ -1548,15 +1588,15 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="B65" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>194</v>
+        <v>34</v>
       </c>
       <c r="B66" t="s">
         <v>115</v>
@@ -1564,7 +1604,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>36</v>
+        <v>161</v>
       </c>
       <c r="B67" t="s">
         <v>114</v>
@@ -1572,23 +1612,23 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>162</v>
+        <v>35</v>
       </c>
       <c r="B68" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>37</v>
+        <v>194</v>
       </c>
       <c r="B69" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>163</v>
+        <v>36</v>
       </c>
       <c r="B70" t="s">
         <v>114</v>
@@ -1596,23 +1636,23 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>38</v>
+        <v>214</v>
       </c>
       <c r="B71" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>39</v>
+        <v>162</v>
       </c>
       <c r="B72" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>200</v>
+        <v>37</v>
       </c>
       <c r="B73" t="s">
         <v>115</v>
@@ -1620,7 +1660,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>40</v>
+        <v>163</v>
       </c>
       <c r="B74" t="s">
         <v>114</v>
@@ -1628,55 +1668,55 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>164</v>
+        <v>39</v>
       </c>
       <c r="B76" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>145</v>
+        <v>200</v>
       </c>
       <c r="B77" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B78" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B79" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>44</v>
+        <v>164</v>
       </c>
       <c r="B80" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="B81" t="s">
         <v>114</v>
@@ -1684,15 +1724,15 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>166</v>
+        <v>42</v>
       </c>
       <c r="B82" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B83" t="s">
         <v>114</v>
@@ -1700,7 +1740,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>201</v>
+        <v>44</v>
       </c>
       <c r="B84" t="s">
         <v>114</v>
@@ -1708,7 +1748,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>46</v>
+        <v>165</v>
       </c>
       <c r="B85" t="s">
         <v>114</v>
@@ -1716,7 +1756,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>210</v>
+        <v>166</v>
       </c>
       <c r="B86" t="s">
         <v>114</v>
@@ -1724,15 +1764,15 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B87" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>116</v>
+        <v>201</v>
       </c>
       <c r="B88" t="s">
         <v>115</v>
@@ -1740,7 +1780,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>167</v>
+        <v>46</v>
       </c>
       <c r="B89" t="s">
         <v>114</v>
@@ -1748,23 +1788,23 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="B90" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B91" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>49</v>
+        <v>215</v>
       </c>
       <c r="B92" t="s">
         <v>114</v>
@@ -1772,23 +1812,23 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="B93" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="B94" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="B95" t="s">
         <v>114</v>
@@ -1796,7 +1836,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B96" t="s">
         <v>114</v>
@@ -1804,7 +1844,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B97" t="s">
         <v>114</v>
@@ -1812,7 +1852,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>128</v>
+        <v>50</v>
       </c>
       <c r="B98" t="s">
         <v>114</v>
@@ -1820,15 +1860,15 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>53</v>
+        <v>195</v>
       </c>
       <c r="B99" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>54</v>
+        <v>146</v>
       </c>
       <c r="B100" t="s">
         <v>114</v>
@@ -1836,7 +1876,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B101" t="s">
         <v>114</v>
@@ -1844,15 +1884,15 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="B102" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>56</v>
+        <v>216</v>
       </c>
       <c r="B103" t="s">
         <v>115</v>
@@ -1860,15 +1900,15 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="B104" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B105" t="s">
         <v>114</v>
@@ -1876,7 +1916,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B106" t="s">
         <v>114</v>
@@ -1884,7 +1924,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>169</v>
+        <v>55</v>
       </c>
       <c r="B107" t="s">
         <v>114</v>
@@ -1892,15 +1932,15 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>170</v>
+        <v>129</v>
       </c>
       <c r="B108" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B109" t="s">
         <v>115</v>
@@ -1908,15 +1948,15 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>171</v>
+        <v>57</v>
       </c>
       <c r="B110" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>172</v>
+        <v>58</v>
       </c>
       <c r="B111" t="s">
         <v>114</v>
@@ -1924,7 +1964,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B112" t="s">
         <v>114</v>
@@ -1932,7 +1972,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>62</v>
+        <v>169</v>
       </c>
       <c r="B113" t="s">
         <v>114</v>
@@ -1940,23 +1980,23 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>63</v>
+        <v>170</v>
       </c>
       <c r="B114" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>173</v>
+        <v>60</v>
       </c>
       <c r="B115" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="B116" t="s">
         <v>114</v>
@@ -1964,15 +2004,15 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>121</v>
+        <v>172</v>
       </c>
       <c r="B117" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>122</v>
+        <v>61</v>
       </c>
       <c r="B118" t="s">
         <v>115</v>
@@ -1980,7 +2020,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B119" t="s">
         <v>114</v>
@@ -1988,15 +2028,15 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B120" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="B121" t="s">
         <v>114</v>
@@ -2004,7 +2044,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>174</v>
+        <v>64</v>
       </c>
       <c r="B122" t="s">
         <v>114</v>
@@ -2012,7 +2052,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="B123" t="s">
         <v>114</v>
@@ -2020,23 +2060,23 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B125" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B126" t="s">
         <v>114</v>
@@ -2044,7 +2084,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>130</v>
+        <v>67</v>
       </c>
       <c r="B127" t="s">
         <v>114</v>
@@ -2052,15 +2092,15 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="B128" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="B129" t="s">
         <v>114</v>
@@ -2068,7 +2108,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
       <c r="B130" t="s">
         <v>114</v>
@@ -2076,23 +2116,23 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>123</v>
+        <v>217</v>
       </c>
       <c r="B131" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>137</v>
+        <v>69</v>
       </c>
       <c r="B132" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>149</v>
+        <v>70</v>
       </c>
       <c r="B133" t="s">
         <v>114</v>
@@ -2100,39 +2140,39 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="B134" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="B135" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
       <c r="B136" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="B137" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="B138" t="s">
         <v>114</v>
@@ -2140,7 +2180,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
       <c r="B139" t="s">
         <v>114</v>
@@ -2148,15 +2188,15 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>76</v>
+        <v>149</v>
       </c>
       <c r="B140" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>132</v>
+        <v>71</v>
       </c>
       <c r="B141" t="s">
         <v>115</v>
@@ -2164,15 +2204,15 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>209</v>
+        <v>72</v>
       </c>
       <c r="B142" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>77</v>
+        <v>218</v>
       </c>
       <c r="B143" t="s">
         <v>115</v>
@@ -2180,15 +2220,15 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>133</v>
+        <v>73</v>
       </c>
       <c r="B144" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>78</v>
+        <v>176</v>
       </c>
       <c r="B145" t="s">
         <v>115</v>
@@ -2196,7 +2236,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>138</v>
+        <v>219</v>
       </c>
       <c r="B146" t="s">
         <v>115</v>
@@ -2204,15 +2244,15 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>141</v>
+        <v>74</v>
       </c>
       <c r="B147" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B148" t="s">
         <v>114</v>
@@ -2220,23 +2260,23 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B149" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="B150" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>81</v>
+        <v>209</v>
       </c>
       <c r="B151" t="s">
         <v>115</v>
@@ -2244,31 +2284,31 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>177</v>
+        <v>77</v>
       </c>
       <c r="B152" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>178</v>
+        <v>133</v>
       </c>
       <c r="B153" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>179</v>
+        <v>78</v>
       </c>
       <c r="B154" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="B155" t="s">
         <v>115</v>
@@ -2276,23 +2316,23 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="B156" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B157" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>207</v>
+        <v>80</v>
       </c>
       <c r="B158" t="s">
         <v>114</v>
@@ -2300,7 +2340,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="B159" t="s">
         <v>114</v>
@@ -2308,15 +2348,15 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>180</v>
+        <v>81</v>
       </c>
       <c r="B160" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>85</v>
+        <v>177</v>
       </c>
       <c r="B161" t="s">
         <v>114</v>
@@ -2324,15 +2364,15 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>86</v>
+        <v>178</v>
       </c>
       <c r="B162" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B163" t="s">
         <v>114</v>
@@ -2340,15 +2380,15 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="B164" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B165" t="s">
         <v>114</v>
@@ -2356,15 +2396,15 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>142</v>
+        <v>83</v>
       </c>
       <c r="B166" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>88</v>
+        <v>207</v>
       </c>
       <c r="B167" t="s">
         <v>114</v>
@@ -2372,7 +2412,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B168" t="s">
         <v>114</v>
@@ -2380,15 +2420,15 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>117</v>
+        <v>180</v>
       </c>
       <c r="B169" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B170" t="s">
         <v>114</v>
@@ -2396,7 +2436,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B171" t="s">
         <v>114</v>
@@ -2404,7 +2444,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>92</v>
+        <v>181</v>
       </c>
       <c r="B172" t="s">
         <v>114</v>
@@ -2412,15 +2452,15 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>93</v>
+        <v>182</v>
       </c>
       <c r="B173" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>191</v>
+        <v>87</v>
       </c>
       <c r="B174" t="s">
         <v>114</v>
@@ -2428,15 +2468,15 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="B175" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="B176" t="s">
         <v>114</v>
@@ -2444,7 +2484,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B177" t="s">
         <v>114</v>
@@ -2452,39 +2492,39 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B178" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="B179" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>184</v>
+        <v>90</v>
       </c>
       <c r="B180" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B181" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="B182" t="s">
         <v>114</v>
@@ -2492,15 +2532,15 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B183" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>99</v>
+        <v>191</v>
       </c>
       <c r="B184" t="s">
         <v>114</v>
@@ -2508,15 +2548,15 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="B185" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>101</v>
+        <v>183</v>
       </c>
       <c r="B186" t="s">
         <v>114</v>
@@ -2524,7 +2564,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B187" t="s">
         <v>114</v>
@@ -2532,7 +2572,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B188" t="s">
         <v>114</v>
@@ -2540,31 +2580,31 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B189" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="B190" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
       <c r="B191" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>134</v>
+        <v>222</v>
       </c>
       <c r="B192" t="s">
         <v>115</v>
@@ -2572,7 +2612,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B193" t="s">
         <v>115</v>
@@ -2580,7 +2620,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>186</v>
+        <v>124</v>
       </c>
       <c r="B194" t="s">
         <v>114</v>
@@ -2588,15 +2628,15 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>187</v>
+        <v>98</v>
       </c>
       <c r="B195" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B196" t="s">
         <v>114</v>
@@ -2604,7 +2644,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>208</v>
+        <v>100</v>
       </c>
       <c r="B197" t="s">
         <v>114</v>
@@ -2612,15 +2652,15 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="B198" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>196</v>
+        <v>102</v>
       </c>
       <c r="B199" t="s">
         <v>114</v>
@@ -2628,39 +2668,39 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>188</v>
+        <v>103</v>
       </c>
       <c r="B200" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B201" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>108</v>
+        <v>202</v>
       </c>
       <c r="B202" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>109</v>
+        <v>185</v>
       </c>
       <c r="B203" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="B204" t="s">
         <v>115</v>
@@ -2668,23 +2708,23 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B205" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>112</v>
+        <v>186</v>
       </c>
       <c r="B206" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>113</v>
+        <v>187</v>
       </c>
       <c r="B207" t="s">
         <v>114</v>
@@ -2692,9 +2732,121 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
+        <v>106</v>
+      </c>
+      <c r="B208" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>208</v>
+      </c>
+      <c r="B209" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>151</v>
+      </c>
+      <c r="B210" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>196</v>
+      </c>
+      <c r="B211" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>188</v>
+      </c>
+      <c r="B212" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>107</v>
+      </c>
+      <c r="B213" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
+        <v>108</v>
+      </c>
+      <c r="B214" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
+        <v>223</v>
+      </c>
+      <c r="B215" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>109</v>
+      </c>
+      <c r="B216" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>110</v>
+      </c>
+      <c r="B217" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>111</v>
+      </c>
+      <c r="B218" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>112</v>
+      </c>
+      <c r="B219" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>113</v>
+      </c>
+      <c r="B220" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>224</v>
+      </c>
+      <c r="B221" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
         <v>189</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B222" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated care data (v40)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A217159E-0874-4B8B-9B5F-BBF1F69EECAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99006286-066C-4A07-A06C-BB3E40ED83AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21120" yWindow="7590" windowWidth="18645" windowHeight="12390" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="28425" yWindow="1260" windowWidth="18375" windowHeight="17265" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="241">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -731,6 +731,27 @@
   </si>
   <si>
     <t>Zorggroep Ter Weel (Stichting)</t>
+  </si>
+  <si>
+    <t>Bartimeus</t>
+  </si>
+  <si>
+    <t>De Lange Wei (Stichting) (Burgemeester De Boer)</t>
+  </si>
+  <si>
+    <t>Joris Zorg (Stichting)</t>
+  </si>
+  <si>
+    <t>Oosterlengte (Stichting)</t>
+  </si>
+  <si>
+    <t>ORO (Stichting)</t>
+  </si>
+  <si>
+    <t>Sint Jozefoord (Stichting)</t>
+  </si>
+  <si>
+    <t>Woonzorgcentrum De Zeeg (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1112,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B231"/>
+  <dimension ref="A1:B238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1311,15 +1332,15 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>234</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
         <v>114</v>
@@ -1327,15 +1348,15 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>143</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="B30" t="s">
         <v>115</v>
@@ -1343,7 +1364,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>199</v>
+        <v>120</v>
       </c>
       <c r="B31" t="s">
         <v>115</v>
@@ -1351,7 +1372,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>199</v>
       </c>
       <c r="B32" t="s">
         <v>115</v>
@@ -1359,15 +1380,15 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>211</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>211</v>
       </c>
       <c r="B34" t="s">
         <v>114</v>
@@ -1375,31 +1396,31 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>212</v>
+        <v>155</v>
       </c>
       <c r="B37" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>156</v>
+        <v>212</v>
       </c>
       <c r="B38" t="s">
         <v>114</v>
@@ -1407,23 +1428,23 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="B39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>139</v>
+        <v>22</v>
       </c>
       <c r="B41" t="s">
         <v>114</v>
@@ -1431,7 +1452,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B42" t="s">
         <v>114</v>
@@ -1439,7 +1460,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
       <c r="B43" t="s">
         <v>114</v>
@@ -1447,15 +1468,15 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>203</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B45" t="s">
         <v>115</v>
@@ -1463,15 +1484,15 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>125</v>
+        <v>204</v>
       </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>213</v>
+        <v>125</v>
       </c>
       <c r="B47" t="s">
         <v>115</v>
@@ -1479,7 +1500,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>157</v>
+        <v>235</v>
       </c>
       <c r="B48" t="s">
         <v>115</v>
@@ -1487,7 +1508,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>213</v>
       </c>
       <c r="B49" t="s">
         <v>115</v>
@@ -1495,7 +1516,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="B50" t="s">
         <v>115</v>
@@ -1503,23 +1524,23 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>24</v>
       </c>
       <c r="B51" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="B52" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="B53" t="s">
         <v>114</v>
@@ -1527,7 +1548,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
         <v>114</v>
@@ -1535,31 +1556,31 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>159</v>
+        <v>27</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>190</v>
+        <v>159</v>
       </c>
       <c r="B58" t="s">
         <v>115</v>
@@ -1567,15 +1588,15 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="B60" t="s">
         <v>115</v>
@@ -1583,7 +1604,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>193</v>
+        <v>30</v>
       </c>
       <c r="B61" t="s">
         <v>115</v>
@@ -1591,15 +1612,15 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>31</v>
+        <v>160</v>
       </c>
       <c r="B62" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>32</v>
+        <v>193</v>
       </c>
       <c r="B63" t="s">
         <v>115</v>
@@ -1607,7 +1628,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>127</v>
+        <v>31</v>
       </c>
       <c r="B64" t="s">
         <v>114</v>
@@ -1615,55 +1636,55 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B66" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B67" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B69" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="B70" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B71" t="s">
         <v>114</v>
@@ -1671,7 +1692,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="B72" t="s">
         <v>115</v>
@@ -1679,15 +1700,15 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>162</v>
+        <v>36</v>
       </c>
       <c r="B73" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>37</v>
+        <v>214</v>
       </c>
       <c r="B74" t="s">
         <v>115</v>
@@ -1695,23 +1716,23 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B75" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B76" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="B77" t="s">
         <v>114</v>
@@ -1719,31 +1740,31 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>226</v>
+        <v>38</v>
       </c>
       <c r="B78" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>200</v>
+        <v>39</v>
       </c>
       <c r="B79" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>40</v>
+        <v>226</v>
       </c>
       <c r="B80" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
       <c r="B81" t="s">
         <v>115</v>
@@ -1751,15 +1772,15 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>164</v>
+        <v>40</v>
       </c>
       <c r="B82" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>145</v>
+        <v>41</v>
       </c>
       <c r="B83" t="s">
         <v>115</v>
@@ -1767,7 +1788,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>42</v>
+        <v>164</v>
       </c>
       <c r="B84" t="s">
         <v>115</v>
@@ -1775,47 +1796,47 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>43</v>
+        <v>236</v>
       </c>
       <c r="B85" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>227</v>
+        <v>145</v>
       </c>
       <c r="B86" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B87" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>165</v>
+        <v>43</v>
       </c>
       <c r="B88" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B89" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>166</v>
+        <v>44</v>
       </c>
       <c r="B90" t="s">
         <v>114</v>
@@ -1823,7 +1844,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="B91" t="s">
         <v>114</v>
@@ -1831,7 +1852,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
       <c r="B92" t="s">
         <v>115</v>
@@ -1839,7 +1860,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>46</v>
+        <v>166</v>
       </c>
       <c r="B93" t="s">
         <v>114</v>
@@ -1847,7 +1868,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>210</v>
+        <v>45</v>
       </c>
       <c r="B94" t="s">
         <v>114</v>
@@ -1855,7 +1876,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>47</v>
+        <v>201</v>
       </c>
       <c r="B95" t="s">
         <v>115</v>
@@ -1863,7 +1884,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>215</v>
+        <v>46</v>
       </c>
       <c r="B96" t="s">
         <v>114</v>
@@ -1871,23 +1892,23 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>116</v>
+        <v>210</v>
       </c>
       <c r="B97" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>167</v>
+        <v>47</v>
       </c>
       <c r="B98" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="B99" t="s">
         <v>114</v>
@@ -1895,23 +1916,23 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="B100" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>49</v>
+        <v>167</v>
       </c>
       <c r="B101" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>50</v>
+        <v>168</v>
       </c>
       <c r="B102" t="s">
         <v>114</v>
@@ -1919,15 +1940,15 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>195</v>
+        <v>48</v>
       </c>
       <c r="B103" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>146</v>
+        <v>49</v>
       </c>
       <c r="B104" t="s">
         <v>114</v>
@@ -1935,7 +1956,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B105" t="s">
         <v>114</v>
@@ -1943,23 +1964,23 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>52</v>
+        <v>195</v>
       </c>
       <c r="B106" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>216</v>
+        <v>146</v>
       </c>
       <c r="B107" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>128</v>
+        <v>51</v>
       </c>
       <c r="B108" t="s">
         <v>114</v>
@@ -1967,23 +1988,23 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B109" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>54</v>
+        <v>216</v>
       </c>
       <c r="B110" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="B111" t="s">
         <v>114</v>
@@ -1991,7 +2012,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>129</v>
+        <v>53</v>
       </c>
       <c r="B112" t="s">
         <v>115</v>
@@ -1999,39 +2020,39 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B113" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B114" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="B115" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B116" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>169</v>
+        <v>57</v>
       </c>
       <c r="B117" t="s">
         <v>114</v>
@@ -2039,7 +2060,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>170</v>
+        <v>58</v>
       </c>
       <c r="B118" t="s">
         <v>114</v>
@@ -2047,7 +2068,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B119" t="s">
         <v>114</v>
@@ -2055,7 +2076,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B120" t="s">
         <v>114</v>
@@ -2063,23 +2084,23 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B121" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B122" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>62</v>
+        <v>237</v>
       </c>
       <c r="B123" t="s">
         <v>114</v>
@@ -2087,55 +2108,55 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>63</v>
+        <v>171</v>
       </c>
       <c r="B124" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>173</v>
+        <v>238</v>
       </c>
       <c r="B125" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="B126" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>121</v>
+        <v>61</v>
       </c>
       <c r="B127" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
       <c r="B128" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B129" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>66</v>
+        <v>173</v>
       </c>
       <c r="B130" t="s">
         <v>114</v>
@@ -2143,7 +2164,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B131" t="s">
         <v>114</v>
@@ -2151,39 +2172,39 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>174</v>
+        <v>121</v>
       </c>
       <c r="B132" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="B133" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B134" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>217</v>
+        <v>66</v>
       </c>
       <c r="B135" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B136" t="s">
         <v>115</v>
@@ -2191,15 +2212,15 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>70</v>
+        <v>174</v>
       </c>
       <c r="B137" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="B138" t="s">
         <v>114</v>
@@ -2207,39 +2228,39 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>131</v>
+        <v>68</v>
       </c>
       <c r="B139" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>175</v>
+        <v>217</v>
       </c>
       <c r="B140" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
       <c r="B141" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>123</v>
+        <v>70</v>
       </c>
       <c r="B142" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B143" t="s">
         <v>114</v>
@@ -2247,23 +2268,23 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B144" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
       <c r="B145" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="B146" t="s">
         <v>114</v>
@@ -2271,7 +2292,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>218</v>
+        <v>123</v>
       </c>
       <c r="B147" t="s">
         <v>115</v>
@@ -2279,7 +2300,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>73</v>
+        <v>137</v>
       </c>
       <c r="B148" t="s">
         <v>114</v>
@@ -2287,15 +2308,15 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="B149" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>219</v>
+        <v>71</v>
       </c>
       <c r="B150" t="s">
         <v>115</v>
@@ -2303,31 +2324,31 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B151" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>75</v>
+        <v>218</v>
       </c>
       <c r="B152" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B153" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>132</v>
+        <v>176</v>
       </c>
       <c r="B154" t="s">
         <v>115</v>
@@ -2335,7 +2356,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="B155" t="s">
         <v>115</v>
@@ -2343,7 +2364,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B156" t="s">
         <v>114</v>
@@ -2351,23 +2372,23 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>229</v>
+        <v>75</v>
       </c>
       <c r="B157" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="B158" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="B159" t="s">
         <v>115</v>
@@ -2375,7 +2396,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>138</v>
+        <v>209</v>
       </c>
       <c r="B160" t="s">
         <v>115</v>
@@ -2383,23 +2404,23 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="B161" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>79</v>
+        <v>229</v>
       </c>
       <c r="B162" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="B163" t="s">
         <v>114</v>
@@ -2407,15 +2428,15 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="B164" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="B165" t="s">
         <v>115</v>
@@ -2423,31 +2444,31 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
       <c r="B166" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>178</v>
+        <v>79</v>
       </c>
       <c r="B167" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="B168" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>205</v>
+        <v>80</v>
       </c>
       <c r="B169" t="s">
         <v>114</v>
@@ -2455,39 +2476,39 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>230</v>
+        <v>118</v>
       </c>
       <c r="B170" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B171" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>83</v>
+        <v>177</v>
       </c>
       <c r="B172" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="B173" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>84</v>
+        <v>179</v>
       </c>
       <c r="B174" t="s">
         <v>114</v>
@@ -2495,7 +2516,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="B175" t="s">
         <v>114</v>
@@ -2503,15 +2524,15 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>85</v>
+        <v>230</v>
       </c>
       <c r="B176" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B177" t="s">
         <v>114</v>
@@ -2519,15 +2540,15 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>181</v>
+        <v>83</v>
       </c>
       <c r="B178" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="B179" t="s">
         <v>114</v>
@@ -2535,7 +2556,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B180" t="s">
         <v>114</v>
@@ -2543,15 +2564,15 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>142</v>
+        <v>85</v>
       </c>
       <c r="B182" t="s">
         <v>114</v>
@@ -2559,7 +2580,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B183" t="s">
         <v>114</v>
@@ -2567,7 +2588,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>89</v>
+        <v>181</v>
       </c>
       <c r="B184" t="s">
         <v>114</v>
@@ -2575,15 +2596,15 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>117</v>
+        <v>182</v>
       </c>
       <c r="B185" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B186" t="s">
         <v>114</v>
@@ -2591,15 +2612,15 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>91</v>
+        <v>220</v>
       </c>
       <c r="B187" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="B188" t="s">
         <v>114</v>
@@ -2607,15 +2628,15 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B189" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>191</v>
+        <v>89</v>
       </c>
       <c r="B190" t="s">
         <v>114</v>
@@ -2623,7 +2644,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="B191" t="s">
         <v>115</v>
@@ -2631,7 +2652,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>183</v>
+        <v>90</v>
       </c>
       <c r="B192" t="s">
         <v>114</v>
@@ -2639,7 +2660,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B193" t="s">
         <v>114</v>
@@ -2647,23 +2668,23 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B194" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B195" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="B196" t="s">
         <v>114</v>
@@ -2671,7 +2692,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>221</v>
+        <v>150</v>
       </c>
       <c r="B197" t="s">
         <v>115</v>
@@ -2679,23 +2700,23 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="B198" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B199" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>231</v>
+        <v>95</v>
       </c>
       <c r="B200" t="s">
         <v>115</v>
@@ -2703,7 +2724,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="B201" t="s">
         <v>114</v>
@@ -2711,63 +2732,63 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>98</v>
+        <v>184</v>
       </c>
       <c r="B202" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>99</v>
+        <v>221</v>
       </c>
       <c r="B203" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>100</v>
+        <v>222</v>
       </c>
       <c r="B204" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B205" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>102</v>
+        <v>240</v>
       </c>
       <c r="B206" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>103</v>
+        <v>231</v>
       </c>
       <c r="B207" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B208" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>202</v>
+        <v>98</v>
       </c>
       <c r="B209" t="s">
         <v>115</v>
@@ -2775,7 +2796,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>185</v>
+        <v>99</v>
       </c>
       <c r="B210" t="s">
         <v>114</v>
@@ -2783,31 +2804,31 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>232</v>
+        <v>100</v>
       </c>
       <c r="B211" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="B212" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B213" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>186</v>
+        <v>103</v>
       </c>
       <c r="B214" t="s">
         <v>114</v>
@@ -2815,7 +2836,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>187</v>
+        <v>104</v>
       </c>
       <c r="B215" t="s">
         <v>115</v>
@@ -2823,39 +2844,39 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>106</v>
+        <v>232</v>
       </c>
       <c r="B216" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B217" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="B218" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>196</v>
+        <v>134</v>
       </c>
       <c r="B219" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>188</v>
+        <v>105</v>
       </c>
       <c r="B220" t="s">
         <v>115</v>
@@ -2863,7 +2884,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>107</v>
+        <v>186</v>
       </c>
       <c r="B221" t="s">
         <v>114</v>
@@ -2871,55 +2892,55 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>108</v>
+        <v>187</v>
       </c>
       <c r="B222" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>233</v>
+        <v>106</v>
       </c>
       <c r="B223" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B224" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="B225" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>110</v>
+        <v>196</v>
       </c>
       <c r="B226" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="B227" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B228" t="s">
         <v>114</v>
@@ -2927,7 +2948,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B229" t="s">
         <v>114</v>
@@ -2935,7 +2956,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="B230" t="s">
         <v>115</v>
@@ -2943,9 +2964,65 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
+        <v>223</v>
+      </c>
+      <c r="B231" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>109</v>
+      </c>
+      <c r="B232" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>110</v>
+      </c>
+      <c r="B233" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>111</v>
+      </c>
+      <c r="B234" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>112</v>
+      </c>
+      <c r="B235" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>113</v>
+      </c>
+      <c r="B236" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>224</v>
+      </c>
+      <c r="B237" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
         <v>189</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B238" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated care data (v47)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CEF7C1-3E6D-408A-8EC2-9C7858BA7FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6B8402-8864-408E-BB00-0D7A62086DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="910" windowWidth="17810" windowHeight="19830" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="430" yWindow="3290" windowWidth="13640" windowHeight="17370" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="265">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -196,9 +196,6 @@
     <t>Middin (Stichting)</t>
   </si>
   <si>
-    <t>Mijzo Schakelring/Eikendonk (Stichting) -&gt; fusie Mijzo (met Riethorst + Volckaert)</t>
-  </si>
-  <si>
     <t>NNCZ (Noord Nederlandse Coöperatie van Zorgorganisaties)</t>
   </si>
   <si>
@@ -247,9 +244,6 @@
     <t>Revant (Stichting)</t>
   </si>
   <si>
-    <t>Rijnhoven (Stichting)</t>
-  </si>
-  <si>
     <t>Rivierduinen</t>
   </si>
   <si>
@@ -607,9 +601,6 @@
     <t>Fundis (Stichting) (beheren meerdere zorginstellingen, zoals Welthuis)</t>
   </si>
   <si>
-    <t>Hartekamp Groep (Stichting)</t>
-  </si>
-  <si>
     <t>Liemerije (Stichting)</t>
   </si>
   <si>
@@ -682,9 +673,6 @@
     <t>Rivas Zorggroep (Stichting)</t>
   </si>
   <si>
-    <t>RST Zorgverleners, RST Zorgverleners Waardenland, RST Zorgverleners (Zwolle) (Stichting)</t>
-  </si>
-  <si>
     <t>Vanboeijen</t>
   </si>
   <si>
@@ -769,9 +757,6 @@
     <t>Sint Jozef Wonen en Zorg (R.K. Stichting)</t>
   </si>
   <si>
-    <t>Thuis met Zorg Zaanstreek B.V.</t>
-  </si>
-  <si>
     <t>Zorgcentrum 't Slot (Stichting)</t>
   </si>
   <si>
@@ -779,6 +764,66 @@
   </si>
   <si>
     <t>Wordt aan gewerkt</t>
+  </si>
+  <si>
+    <t>De Hoven (Stichting)</t>
+  </si>
+  <si>
+    <t>De Zorgcirkel (Stichting)</t>
+  </si>
+  <si>
+    <t>DeniseZorg B.V.</t>
+  </si>
+  <si>
+    <t>Domus Magnus B.V.</t>
+  </si>
+  <si>
+    <t>Fivoor (forensische en intensieve psychiatrie) (Z-H)</t>
+  </si>
+  <si>
+    <t>Gemiva-SVG Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>GGZ Noord-Holland-Noord (NHN) (Stichting)</t>
+  </si>
+  <si>
+    <t>Hervormde Stichting Sonneburgh</t>
+  </si>
+  <si>
+    <t>IJsselheem Holding (Stichting)</t>
+  </si>
+  <si>
+    <t>Nieuw Woelwijck, Dorpsgemeenschap van Geestelijk Gehandicapten (Stichting)</t>
+  </si>
+  <si>
+    <t>RIBW Arnhem &amp; Veluwevallei</t>
+  </si>
+  <si>
+    <t>Samen Zorgen (Stichting) (ssz)</t>
+  </si>
+  <si>
+    <t>Santé Partners (=STMR+Vitras)</t>
+  </si>
+  <si>
+    <t>Vivent (Stichting)</t>
+  </si>
+  <si>
+    <t>Vivium zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Woongemeenschap voor Ouderen Heemzicht (Stichting)</t>
+  </si>
+  <si>
+    <t>Zonnehuisgroep IJssel-Vecht (ZGIJV) (+fusie met Driezorg)</t>
+  </si>
+  <si>
+    <t>Zonnehuisgroep Vlaardingen (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorgcentra Rivierenland (Stichting)</t>
+  </si>
+  <si>
+    <t>ZorgSaam Zorggroep Zeeuws-Vlaanderen (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1184,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B247"/>
+  <dimension ref="A1:B263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1159,10 +1204,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1170,7 +1215,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1178,7 +1223,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1186,31 +1231,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B6" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1218,15 +1263,15 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1234,7 +1279,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -1242,31 +1287,31 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B13" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B14" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B15" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -1274,23 +1319,23 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B17" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B18" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -1298,7 +1343,7 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1306,7 +1351,7 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -1314,7 +1359,7 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -1322,15 +1367,15 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1338,7 +1383,7 @@
         <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -1346,7 +1391,7 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1354,23 +1399,23 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B28" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -1378,7 +1423,7 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -1386,31 +1431,31 @@
         <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B31" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B33" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -1418,15 +1463,15 @@
         <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B35" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -1434,7 +1479,7 @@
         <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -1442,31 +1487,31 @@
         <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B38" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B39" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B40" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -1474,7 +1519,7 @@
         <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -1482,23 +1527,23 @@
         <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B44" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1506,1623 +1551,1751 @@
         <v>23</v>
       </c>
       <c r="B45" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B46" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B47" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B48" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="B49" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="B50" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="B51" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>24</v>
+        <v>153</v>
       </c>
       <c r="B52" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>124</v>
+        <v>246</v>
       </c>
       <c r="B53" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="B54" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B55" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="B56" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>154</v>
       </c>
       <c r="B57" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B58" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>157</v>
+        <v>248</v>
       </c>
       <c r="B59" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B60" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>188</v>
+        <v>27</v>
       </c>
       <c r="B61" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B62" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B63" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>191</v>
+        <v>29</v>
       </c>
       <c r="B64" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>31</v>
+        <v>186</v>
       </c>
       <c r="B65" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B66" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="B67" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>33</v>
+        <v>249</v>
       </c>
       <c r="B68" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>189</v>
       </c>
       <c r="B69" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>34</v>
+        <v>250</v>
       </c>
       <c r="B70" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>159</v>
+        <v>31</v>
       </c>
       <c r="B71" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>192</v>
+        <v>123</v>
       </c>
       <c r="B73" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B74" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>212</v>
+        <v>136</v>
       </c>
       <c r="B75" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>160</v>
+        <v>34</v>
       </c>
       <c r="B76" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>37</v>
+        <v>251</v>
       </c>
       <c r="B77" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B78" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>239</v>
+        <v>35</v>
       </c>
       <c r="B79" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B80" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>39</v>
+        <v>252</v>
       </c>
       <c r="B81" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B82" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="B83" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>240</v>
+        <v>37</v>
       </c>
       <c r="B84" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>40</v>
+        <v>159</v>
       </c>
       <c r="B85" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>41</v>
+        <v>235</v>
       </c>
       <c r="B86" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>162</v>
+        <v>38</v>
       </c>
       <c r="B87" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>234</v>
+        <v>39</v>
       </c>
       <c r="B88" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>143</v>
+        <v>220</v>
       </c>
       <c r="B89" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>42</v>
+        <v>195</v>
       </c>
       <c r="B90" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>43</v>
+        <v>236</v>
       </c>
       <c r="B91" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
       <c r="B92" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B93" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="B94" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>226</v>
+        <v>160</v>
       </c>
       <c r="B95" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>164</v>
+        <v>230</v>
       </c>
       <c r="B96" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>45</v>
+        <v>141</v>
       </c>
       <c r="B97" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>241</v>
+        <v>42</v>
       </c>
       <c r="B98" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>199</v>
+        <v>43</v>
       </c>
       <c r="B99" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>46</v>
+        <v>221</v>
       </c>
       <c r="B100" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>208</v>
+        <v>44</v>
       </c>
       <c r="B101" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>47</v>
+        <v>161</v>
       </c>
       <c r="B102" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B103" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="B104" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>165</v>
+        <v>45</v>
       </c>
       <c r="B105" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B106" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>166</v>
+        <v>196</v>
       </c>
       <c r="B107" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B108" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>49</v>
+        <v>205</v>
       </c>
       <c r="B109" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B110" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="B111" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>51</v>
+        <v>163</v>
       </c>
       <c r="B113" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>52</v>
+        <v>238</v>
       </c>
       <c r="B114" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="B115" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
       <c r="B116" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B117" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B118" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>55</v>
+        <v>190</v>
       </c>
       <c r="B119" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="B120" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B121" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B122" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>58</v>
+        <v>211</v>
       </c>
       <c r="B123" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>167</v>
+        <v>53</v>
       </c>
       <c r="B125" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>168</v>
+        <v>54</v>
       </c>
       <c r="B126" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="B128" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>169</v>
+        <v>55</v>
       </c>
       <c r="B129" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>236</v>
+        <v>56</v>
       </c>
       <c r="B130" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>170</v>
+        <v>57</v>
       </c>
       <c r="B131" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B132" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>62</v>
+        <v>165</v>
       </c>
       <c r="B133" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>63</v>
+        <v>166</v>
       </c>
       <c r="B134" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="B135" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>64</v>
+        <v>231</v>
       </c>
       <c r="B136" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="B137" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>120</v>
+        <v>232</v>
       </c>
       <c r="B138" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>65</v>
+        <v>168</v>
       </c>
       <c r="B139" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B140" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B141" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="B142" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="B143" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B144" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>215</v>
+        <v>117</v>
       </c>
       <c r="B145" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="B146" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B147" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>128</v>
+        <v>65</v>
       </c>
       <c r="B148" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>129</v>
+        <v>66</v>
       </c>
       <c r="B149" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B150" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>243</v>
+        <v>143</v>
       </c>
       <c r="B151" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>146</v>
+        <v>67</v>
       </c>
       <c r="B152" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>121</v>
+        <v>212</v>
       </c>
       <c r="B153" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="B154" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>147</v>
+        <v>69</v>
       </c>
       <c r="B155" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="B156" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="B157" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>244</v>
+        <v>171</v>
       </c>
       <c r="B158" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="B159" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>73</v>
+        <v>144</v>
       </c>
       <c r="B160" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>174</v>
+        <v>119</v>
       </c>
       <c r="B161" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>217</v>
+        <v>133</v>
       </c>
       <c r="B162" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="B163" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B164" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>76</v>
+        <v>255</v>
       </c>
       <c r="B165" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>130</v>
+        <v>240</v>
       </c>
       <c r="B166" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B167" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B168" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>227</v>
+        <v>172</v>
       </c>
       <c r="B169" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>131</v>
+        <v>72</v>
       </c>
       <c r="B170" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B171" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="B172" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>139</v>
+        <v>256</v>
       </c>
       <c r="B173" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>79</v>
+        <v>257</v>
       </c>
       <c r="B174" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>245</v>
+        <v>128</v>
       </c>
       <c r="B175" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>80</v>
+        <v>204</v>
       </c>
       <c r="B176" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="B177" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>81</v>
+        <v>223</v>
       </c>
       <c r="B178" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="B179" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>176</v>
+        <v>76</v>
       </c>
       <c r="B180" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>177</v>
+        <v>134</v>
       </c>
       <c r="B181" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>203</v>
+        <v>137</v>
       </c>
       <c r="B182" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>228</v>
+        <v>77</v>
       </c>
       <c r="B183" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>82</v>
+        <v>241</v>
       </c>
       <c r="B184" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B185" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>205</v>
+        <v>114</v>
       </c>
       <c r="B186" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B187" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B188" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>246</v>
+        <v>174</v>
       </c>
       <c r="B189" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>85</v>
+        <v>175</v>
       </c>
       <c r="B190" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>86</v>
+        <v>200</v>
       </c>
       <c r="B191" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
       <c r="B192" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>180</v>
+        <v>80</v>
       </c>
       <c r="B193" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B194" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="B195" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>140</v>
+        <v>202</v>
       </c>
       <c r="B196" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B197" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="B198" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="B199" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B200" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
       <c r="B201" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="B202" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B203" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="B204" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B205" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>181</v>
+        <v>86</v>
       </c>
       <c r="B206" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B207" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="B208" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B209" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>182</v>
+        <v>89</v>
       </c>
       <c r="B210" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>219</v>
+        <v>90</v>
       </c>
       <c r="B211" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>220</v>
+        <v>258</v>
       </c>
       <c r="B212" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>97</v>
+        <v>259</v>
       </c>
       <c r="B213" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>237</v>
+        <v>91</v>
       </c>
       <c r="B214" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>229</v>
+        <v>187</v>
       </c>
       <c r="B215" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="B216" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>98</v>
+        <v>179</v>
       </c>
       <c r="B217" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B218" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B219" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B220" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>102</v>
+        <v>180</v>
       </c>
       <c r="B221" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>103</v>
+        <v>215</v>
       </c>
       <c r="B222" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>104</v>
+        <v>216</v>
       </c>
       <c r="B223" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="B224" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="B225" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B226" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B228" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B229" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>184</v>
+        <v>97</v>
       </c>
       <c r="B230" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>185</v>
+        <v>98</v>
       </c>
       <c r="B231" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>106</v>
+        <v>261</v>
       </c>
       <c r="B232" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>206</v>
+        <v>99</v>
       </c>
       <c r="B233" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>149</v>
+        <v>262</v>
       </c>
       <c r="B234" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>194</v>
+        <v>100</v>
       </c>
       <c r="B235" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>186</v>
+        <v>101</v>
       </c>
       <c r="B236" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B237" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>108</v>
+        <v>263</v>
       </c>
       <c r="B238" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="B239" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>221</v>
+        <v>181</v>
       </c>
       <c r="B240" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>109</v>
+        <v>226</v>
       </c>
       <c r="B241" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>110</v>
+        <v>242</v>
       </c>
       <c r="B242" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="B243" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B244" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>113</v>
+        <v>182</v>
       </c>
       <c r="B245" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="B246" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>187</v>
+        <v>104</v>
       </c>
       <c r="B247" t="s">
-        <v>249</v>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A248" t="s">
+        <v>203</v>
+      </c>
+      <c r="B248" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A249" t="s">
+        <v>147</v>
+      </c>
+      <c r="B249" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A250" t="s">
+        <v>191</v>
+      </c>
+      <c r="B250" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A251" t="s">
+        <v>184</v>
+      </c>
+      <c r="B251" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A252" t="s">
+        <v>105</v>
+      </c>
+      <c r="B252" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A253" t="s">
+        <v>106</v>
+      </c>
+      <c r="B253" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A254" t="s">
+        <v>227</v>
+      </c>
+      <c r="B254" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
+        <v>217</v>
+      </c>
+      <c r="B255" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
+        <v>107</v>
+      </c>
+      <c r="B256" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>264</v>
+      </c>
+      <c r="B257" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
+        <v>108</v>
+      </c>
+      <c r="B258" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>109</v>
+      </c>
+      <c r="B259" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
+        <v>110</v>
+      </c>
+      <c r="B260" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
+        <v>111</v>
+      </c>
+      <c r="B261" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
+        <v>218</v>
+      </c>
+      <c r="B262" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
+        <v>185</v>
+      </c>
+      <c r="B263" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed status of Carint Reggeland
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6B8402-8864-408E-BB00-0D7A62086DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9107AC5-5B1C-4E68-9342-327141AC2CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="430" yWindow="3290" windowWidth="13640" windowHeight="17370" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="16340" yWindow="2790" windowWidth="21190" windowHeight="17370" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1186,7 +1186,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
   <dimension ref="A1:B263"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1495,7 +1497,7 @@
         <v>151</v>
       </c>
       <c r="B38" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated care data (v48)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9107AC5-5B1C-4E68-9342-327141AC2CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9623CC74-6644-441D-8F09-CAB6A8A68A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16340" yWindow="2790" windowWidth="21190" windowHeight="17370" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="3400" yWindow="2070" windowWidth="13570" windowHeight="17120" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="240">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -43,9 +43,6 @@
     <t>ActiVite (Stichting)</t>
   </si>
   <si>
-    <t>Adelante Groep (Stichting)</t>
-  </si>
-  <si>
     <t>Altrecht (Stichting)</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>Baalderborg Groep (Stichting)</t>
   </si>
   <si>
-    <t>Basalt revalidatie</t>
-  </si>
-  <si>
     <t>Bethanië (Stichting)</t>
   </si>
   <si>
@@ -139,18 +133,12 @@
     <t>GGzE (Stichting) GGz Eindhoven</t>
   </si>
   <si>
-    <t>Heliomare (Stichting)</t>
-  </si>
-  <si>
     <t>Het Laar (Stichting)</t>
   </si>
   <si>
     <t>HilverZorg (Stichting)</t>
   </si>
   <si>
-    <t>Hoogstraat Revalidatie (Stichting)</t>
-  </si>
-  <si>
     <t>Innoforte (Stichting)</t>
   </si>
   <si>
@@ -181,9 +169,6 @@
     <t>Liante (Stichting)</t>
   </si>
   <si>
-    <t>Libra Revalidatie &amp; Audiologie (Stichting)</t>
-  </si>
-  <si>
     <t>Magenta</t>
   </si>
   <si>
@@ -241,18 +226,12 @@
     <t>PSW (Stichting)</t>
   </si>
   <si>
-    <t>Revant (Stichting)</t>
-  </si>
-  <si>
     <t>Rivierduinen</t>
   </si>
   <si>
     <t>S&amp;L Zorg (Stichting)</t>
   </si>
   <si>
-    <t>Saffier - De Residentie (Stichting Zorginstelling ...))</t>
-  </si>
-  <si>
     <t>Salem Verpleeghuis (Stichting)</t>
   </si>
   <si>
@@ -304,18 +283,12 @@
     <t>ViVa! Zorggroep (Stichting)</t>
   </si>
   <si>
-    <t>Vogellanden, Centrum voor Revalidatie (Stichting)</t>
-  </si>
-  <si>
     <t>Wever (Stichting)</t>
   </si>
   <si>
     <t>WIJdezorg (Stichting)</t>
   </si>
   <si>
-    <t>WilgaerdenLeekerweide Groep (Stichting)</t>
-  </si>
-  <si>
     <t>Woonzorg Samen (Stichting)</t>
   </si>
   <si>
@@ -346,9 +319,6 @@
     <t>Zorggroep Ena (Stichting)</t>
   </si>
   <si>
-    <t>Zorggroep Tangenborgh (Stichting)</t>
-  </si>
-  <si>
     <t>Zorggroep Tellus (Stichting)</t>
   </si>
   <si>
@@ -400,9 +370,6 @@
     <t>Dichterbij (Stichting)</t>
   </si>
   <si>
-    <t>GGz Centraal (Stichting)</t>
-  </si>
-  <si>
     <t>Mediant, Stichting voor Geestelijke Gezondheidszorg Oost- en Midden Twente</t>
   </si>
   <si>
@@ -415,18 +382,12 @@
     <t>R.K. Zorgcentrum Roomburgh (Stichting)</t>
   </si>
   <si>
-    <t>Savant, Organisatie voor Zorg (Stichting)</t>
-  </si>
-  <si>
     <t>Severinusstichting</t>
   </si>
   <si>
     <t>Zorgfederatie Oldenzaal (Stichting)</t>
   </si>
   <si>
-    <t>Avoord Zorg en Wonen (Stichting)</t>
-  </si>
-  <si>
     <t>Cosis</t>
   </si>
   <si>
@@ -445,9 +406,6 @@
     <t>Sint Anna Boxmeer (Stichting)</t>
   </si>
   <si>
-    <t>Vecht &amp; Ijssel (Stichting)</t>
-  </si>
-  <si>
     <t>Beweging 3.0 (Stichting)</t>
   </si>
   <si>
@@ -457,18 +415,9 @@
     <t>Kalorama (Stichting)</t>
   </si>
   <si>
-    <t>Lister (Stichting)</t>
-  </si>
-  <si>
     <t>Pro Persona</t>
   </si>
   <si>
-    <t>Reade</t>
-  </si>
-  <si>
-    <t>Revalidatie Friesland</t>
-  </si>
-  <si>
     <t>Warande (Stichting)</t>
   </si>
   <si>
@@ -493,18 +442,9 @@
     <t>De Zijlen (Stichting) (Ilmarinen)</t>
   </si>
   <si>
-    <t>Dienstencentrum Oud Burgeren Gasthuis (OBG) (Stichting)</t>
-  </si>
-  <si>
-    <t>DZN B.V. (directe zorg nijmegen)</t>
-  </si>
-  <si>
     <t>Fier Fryslan (Stichting)</t>
   </si>
   <si>
-    <t>GGZ Westelijk Noord-Brabant / GGZ-WNB (Stichting)</t>
-  </si>
-  <si>
     <t>Het Gasthuis Millingen aan de Rijn (Sint Jan De Deo) (Stichting)</t>
   </si>
   <si>
@@ -514,9 +454,6 @@
     <t>Ipse de Bruggen (Stichting)</t>
   </si>
   <si>
-    <t>Klimmendaal (Stichting)</t>
-  </si>
-  <si>
     <t>Koninklijke Visio, expertisecentrum voor slechtziende en blinde mensen (Stichting)</t>
   </si>
   <si>
@@ -526,12 +463,6 @@
     <t>Lentis incl. Dignis</t>
   </si>
   <si>
-    <t>Odion (Stichting)</t>
-  </si>
-  <si>
-    <t>Omega (Groep, Zwolle!)</t>
-  </si>
-  <si>
     <t>Opbouw (Stichting) incl. Prinsenstichting</t>
   </si>
   <si>
@@ -562,9 +493,6 @@
     <t>Thebe (Zorggroep west en midden Brabant, incl. Ruitersbos)</t>
   </si>
   <si>
-    <t>Treant Zorggroep (Stichting)</t>
-  </si>
-  <si>
     <t>Valkenhof (Stichting)</t>
   </si>
   <si>
@@ -589,9 +517,6 @@
     <t>ZZG Zorggroep (Stichting)</t>
   </si>
   <si>
-    <t>Emergis (Stichting)</t>
-  </si>
-  <si>
     <t>Waardeburgh (Stichting)</t>
   </si>
   <si>
@@ -610,9 +535,6 @@
     <t xml:space="preserve">Alliade </t>
   </si>
   <si>
-    <t>Ambiq (Stichting)</t>
-  </si>
-  <si>
     <t>Breederzorg Thuiszorg (Stichting)</t>
   </si>
   <si>
@@ -640,15 +562,9 @@
     <t>Teamzorg B.V.</t>
   </si>
   <si>
-    <t>Zorggroep Florence (Stichting)</t>
-  </si>
-  <si>
     <t>Schärwachter B.V.</t>
   </si>
   <si>
-    <t>Kwintes (Stichting)</t>
-  </si>
-  <si>
     <t>Careander (Stichting)</t>
   </si>
   <si>
@@ -772,27 +688,12 @@
     <t>De Zorgcirkel (Stichting)</t>
   </si>
   <si>
-    <t>DeniseZorg B.V.</t>
-  </si>
-  <si>
     <t>Domus Magnus B.V.</t>
   </si>
   <si>
     <t>Fivoor (forensische en intensieve psychiatrie) (Z-H)</t>
   </si>
   <si>
-    <t>Gemiva-SVG Groep (Stichting)</t>
-  </si>
-  <si>
-    <t>GGZ Noord-Holland-Noord (NHN) (Stichting)</t>
-  </si>
-  <si>
-    <t>Hervormde Stichting Sonneburgh</t>
-  </si>
-  <si>
-    <t>IJsselheem Holding (Stichting)</t>
-  </si>
-  <si>
     <t>Nieuw Woelwijck, Dorpsgemeenschap van Geestelijk Gehandicapten (Stichting)</t>
   </si>
   <si>
@@ -808,15 +709,9 @@
     <t>Vivent (Stichting)</t>
   </si>
   <si>
-    <t>Vivium zorggroep (Stichting)</t>
-  </si>
-  <si>
     <t>Woongemeenschap voor Ouderen Heemzicht (Stichting)</t>
   </si>
   <si>
-    <t>Zonnehuisgroep IJssel-Vecht (ZGIJV) (+fusie met Driezorg)</t>
-  </si>
-  <si>
     <t>Zonnehuisgroep Vlaardingen (Stichting)</t>
   </si>
   <si>
@@ -824,6 +719,36 @@
   </si>
   <si>
     <t>ZorgSaam Zorggroep Zeeuws-Vlaanderen (Stichting)</t>
+  </si>
+  <si>
+    <t>Humanitas voor Dienstverlening aan Mensen met een Handicap / Humanitas DMH (Stichting)</t>
+  </si>
+  <si>
+    <t>IrisZorg</t>
+  </si>
+  <si>
+    <t>Kempenhaeghe (Stichting)</t>
+  </si>
+  <si>
+    <t>Laurens (Stichting)</t>
+  </si>
+  <si>
+    <t>Livio (Stichting)</t>
+  </si>
+  <si>
+    <t>Rijnhoven (Stichting)</t>
+  </si>
+  <si>
+    <t>Riwis Zorg &amp; Welzijn</t>
+  </si>
+  <si>
+    <t>RST Zorgverleners, RST Zorgverleners Waardenland, RST Zorgverleners (Zwolle) (Stichting)</t>
+  </si>
+  <si>
+    <t>Sensire (Stichting)</t>
+  </si>
+  <si>
+    <t>Thuis met Zorg Zaanstreek B.V.</t>
   </si>
 </sst>
 </file>
@@ -1184,11 +1109,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B263"/>
+  <dimension ref="A1:B238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1206,10 +1129,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1217,7 +1140,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1225,55 +1148,55 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1281,119 +1204,119 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>201</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>191</v>
       </c>
       <c r="B16" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>219</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="B24" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>200</v>
       </c>
       <c r="B25" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1401,119 +1324,119 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>228</v>
+        <v>106</v>
       </c>
       <c r="B28" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>168</v>
       </c>
       <c r="B29" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="B31" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>194</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>134</v>
       </c>
       <c r="B34" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="B35" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="B36" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>207</v>
+        <v>122</v>
       </c>
       <c r="B39" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="B40" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -1521,1135 +1444,1135 @@
         <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>172</v>
       </c>
       <c r="B42" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="B43" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>217</v>
       </c>
       <c r="B45" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B46" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="B47" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="B48" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="B49" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>229</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>208</v>
+        <v>112</v>
       </c>
       <c r="B51" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>153</v>
+        <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>246</v>
+        <v>219</v>
       </c>
       <c r="B53" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>247</v>
+        <v>24</v>
       </c>
       <c r="B54" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B55" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="B56" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>27</v>
       </c>
       <c r="B57" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B58" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>248</v>
+        <v>137</v>
       </c>
       <c r="B59" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>26</v>
+        <v>220</v>
       </c>
       <c r="B60" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>27</v>
+        <v>164</v>
       </c>
       <c r="B61" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B62" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>155</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B64" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>186</v>
+        <v>123</v>
       </c>
       <c r="B65" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
       <c r="B67" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>249</v>
+        <v>181</v>
       </c>
       <c r="B68" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>189</v>
+        <v>138</v>
       </c>
       <c r="B69" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>250</v>
+        <v>34</v>
       </c>
       <c r="B70" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>31</v>
+        <v>139</v>
       </c>
       <c r="B71" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>32</v>
+        <v>207</v>
       </c>
       <c r="B72" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>123</v>
+        <v>35</v>
       </c>
       <c r="B73" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>33</v>
+        <v>192</v>
       </c>
       <c r="B74" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="B75" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="B76" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="B77" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>157</v>
+        <v>36</v>
       </c>
       <c r="B78" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B79" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="B80" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="B81" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B82" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="B83" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B84" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>159</v>
+        <v>232</v>
       </c>
       <c r="B85" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>235</v>
+        <v>39</v>
       </c>
       <c r="B86" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>38</v>
+        <v>193</v>
       </c>
       <c r="B87" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B88" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="B89" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>195</v>
+        <v>141</v>
       </c>
       <c r="B90" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>236</v>
+        <v>41</v>
       </c>
       <c r="B91" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>253</v>
+        <v>209</v>
       </c>
       <c r="B92" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>40</v>
+        <v>170</v>
       </c>
       <c r="B93" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B94" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>160</v>
+        <v>43</v>
       </c>
       <c r="B95" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>230</v>
+        <v>182</v>
       </c>
       <c r="B96" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>141</v>
+        <v>233</v>
       </c>
       <c r="B97" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="B98" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="B99" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B100" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>44</v>
+        <v>143</v>
       </c>
       <c r="B101" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>161</v>
+        <v>44</v>
       </c>
       <c r="B102" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>222</v>
+        <v>45</v>
       </c>
       <c r="B103" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B104" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>45</v>
+        <v>234</v>
       </c>
       <c r="B105" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>237</v>
+        <v>46</v>
       </c>
       <c r="B106" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>196</v>
+        <v>47</v>
       </c>
       <c r="B107" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>46</v>
+        <v>183</v>
       </c>
       <c r="B108" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>205</v>
+        <v>113</v>
       </c>
       <c r="B109" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B110" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>210</v>
+        <v>49</v>
       </c>
       <c r="B111" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>163</v>
+        <v>221</v>
       </c>
       <c r="B113" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>238</v>
+        <v>50</v>
       </c>
       <c r="B114" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>164</v>
+        <v>51</v>
       </c>
       <c r="B115" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B116" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B117" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B118" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="B119" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B120" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>51</v>
+        <v>204</v>
       </c>
       <c r="B121" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="B122" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>211</v>
+        <v>55</v>
       </c>
       <c r="B123" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>124</v>
+        <v>56</v>
       </c>
       <c r="B124" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B125" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>54</v>
+        <v>146</v>
       </c>
       <c r="B126" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
       <c r="B127" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>254</v>
+        <v>107</v>
       </c>
       <c r="B128" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B129" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B130" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B131" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B132" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="B133" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
       <c r="B134" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B135" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="B136" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>167</v>
+        <v>63</v>
       </c>
       <c r="B137" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>232</v>
+        <v>64</v>
       </c>
       <c r="B138" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>168</v>
+        <v>115</v>
       </c>
       <c r="B139" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="B140" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>61</v>
+        <v>148</v>
       </c>
       <c r="B141" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>62</v>
+        <v>211</v>
       </c>
       <c r="B142" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>169</v>
+        <v>109</v>
       </c>
       <c r="B143" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="B144" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>117</v>
+        <v>222</v>
       </c>
       <c r="B145" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>118</v>
+        <v>235</v>
       </c>
       <c r="B146" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>64</v>
+        <v>212</v>
       </c>
       <c r="B147" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>65</v>
+        <v>185</v>
       </c>
       <c r="B148" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B149" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>170</v>
+        <v>236</v>
       </c>
       <c r="B150" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>67</v>
+        <v>237</v>
       </c>
       <c r="B152" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>212</v>
+        <v>66</v>
       </c>
       <c r="B153" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B154" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>69</v>
+        <v>223</v>
       </c>
       <c r="B155" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>126</v>
+        <v>224</v>
       </c>
       <c r="B156" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>127</v>
+        <v>177</v>
       </c>
       <c r="B157" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>171</v>
+        <v>68</v>
       </c>
       <c r="B158" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B159" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="B160" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B161" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="B162" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="B163" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="B164" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>255</v>
+        <v>70</v>
       </c>
       <c r="B165" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>240</v>
+        <v>213</v>
       </c>
       <c r="B166" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>213</v>
+        <v>71</v>
       </c>
       <c r="B167" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="B168" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>172</v>
+        <v>72</v>
       </c>
       <c r="B169" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="B170" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>73</v>
+        <v>151</v>
       </c>
       <c r="B171" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="B172" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>256</v>
+        <v>174</v>
       </c>
       <c r="B173" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>257</v>
+        <v>196</v>
       </c>
       <c r="B174" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>128</v>
+        <v>73</v>
       </c>
       <c r="B175" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>204</v>
+        <v>74</v>
       </c>
       <c r="B176" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>75</v>
+        <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>223</v>
+        <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="B179" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>76</v>
+        <v>153</v>
       </c>
       <c r="B180" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>134</v>
+        <v>239</v>
       </c>
       <c r="B181" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>137</v>
+        <v>76</v>
       </c>
       <c r="B182" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
@@ -2657,15 +2580,15 @@
         <v>77</v>
       </c>
       <c r="B183" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>241</v>
+        <v>154</v>
       </c>
       <c r="B184" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
@@ -2673,15 +2596,15 @@
         <v>78</v>
       </c>
       <c r="B185" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>114</v>
+        <v>186</v>
       </c>
       <c r="B186" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
@@ -2689,159 +2612,159 @@
         <v>79</v>
       </c>
       <c r="B187" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>173</v>
+        <v>80</v>
       </c>
       <c r="B188" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="B189" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>175</v>
+        <v>81</v>
       </c>
       <c r="B190" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>200</v>
+        <v>82</v>
       </c>
       <c r="B191" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>224</v>
+        <v>83</v>
       </c>
       <c r="B192" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>80</v>
+        <v>225</v>
       </c>
       <c r="B193" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="B194" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>202</v>
+        <v>129</v>
       </c>
       <c r="B195" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>202</v>
+        <v>155</v>
       </c>
       <c r="B196" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B197" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>176</v>
+        <v>85</v>
       </c>
       <c r="B198" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>83</v>
+        <v>156</v>
       </c>
       <c r="B199" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>84</v>
+        <v>187</v>
       </c>
       <c r="B200" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="B201" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>178</v>
+        <v>226</v>
       </c>
       <c r="B202" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B203" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B204" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>138</v>
+        <v>197</v>
       </c>
       <c r="B205" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="B206" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
@@ -2849,223 +2772,223 @@
         <v>87</v>
       </c>
       <c r="B207" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="B208" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B209" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B210" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>90</v>
+        <v>227</v>
       </c>
       <c r="B211" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>258</v>
+        <v>91</v>
       </c>
       <c r="B212" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>259</v>
+        <v>92</v>
       </c>
       <c r="B213" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B214" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>187</v>
+        <v>228</v>
       </c>
       <c r="B215" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="B216" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="B217" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>92</v>
+        <v>198</v>
       </c>
       <c r="B218" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>93</v>
+        <v>214</v>
       </c>
       <c r="B219" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="B220" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>180</v>
+        <v>94</v>
       </c>
       <c r="B221" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>215</v>
+        <v>158</v>
       </c>
       <c r="B222" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>216</v>
+        <v>159</v>
       </c>
       <c r="B223" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>260</v>
+        <v>95</v>
       </c>
       <c r="B224" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="B225" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>233</v>
+        <v>166</v>
       </c>
       <c r="B226" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>225</v>
+        <v>160</v>
       </c>
       <c r="B227" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="B228" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>96</v>
+        <v>199</v>
       </c>
       <c r="B229" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>97</v>
+        <v>189</v>
       </c>
       <c r="B230" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B231" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
       <c r="B232" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B233" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>262</v>
+        <v>99</v>
       </c>
       <c r="B234" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
@@ -3073,7 +2996,7 @@
         <v>100</v>
       </c>
       <c r="B235" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
@@ -3081,223 +3004,23 @@
         <v>101</v>
       </c>
       <c r="B236" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>102</v>
+        <v>190</v>
       </c>
       <c r="B237" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>263</v>
+        <v>161</v>
       </c>
       <c r="B238" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A239" t="s">
-        <v>197</v>
-      </c>
-      <c r="B239" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A240" t="s">
-        <v>181</v>
-      </c>
-      <c r="B240" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A241" t="s">
-        <v>226</v>
-      </c>
-      <c r="B241" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A242" t="s">
-        <v>242</v>
-      </c>
-      <c r="B242" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A243" t="s">
-        <v>130</v>
-      </c>
-      <c r="B243" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A244" t="s">
-        <v>103</v>
-      </c>
-      <c r="B244" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A245" t="s">
-        <v>182</v>
-      </c>
-      <c r="B245" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A246" t="s">
-        <v>183</v>
-      </c>
-      <c r="B246" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A247" t="s">
-        <v>104</v>
-      </c>
-      <c r="B247" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A248" t="s">
-        <v>203</v>
-      </c>
-      <c r="B248" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A249" t="s">
-        <v>147</v>
-      </c>
-      <c r="B249" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A250" t="s">
-        <v>191</v>
-      </c>
-      <c r="B250" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A251" t="s">
-        <v>184</v>
-      </c>
-      <c r="B251" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A252" t="s">
-        <v>105</v>
-      </c>
-      <c r="B252" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A253" t="s">
-        <v>106</v>
-      </c>
-      <c r="B253" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A254" t="s">
-        <v>227</v>
-      </c>
-      <c r="B254" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A255" t="s">
-        <v>217</v>
-      </c>
-      <c r="B255" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A256" t="s">
-        <v>107</v>
-      </c>
-      <c r="B256" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A257" t="s">
-        <v>264</v>
-      </c>
-      <c r="B257" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A258" t="s">
-        <v>108</v>
-      </c>
-      <c r="B258" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A259" t="s">
-        <v>109</v>
-      </c>
-      <c r="B259" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A260" t="s">
-        <v>110</v>
-      </c>
-      <c r="B260" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A261" t="s">
-        <v>111</v>
-      </c>
-      <c r="B261" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A262" t="s">
-        <v>218</v>
-      </c>
-      <c r="B262" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A263" t="s">
-        <v>185</v>
-      </c>
-      <c r="B263" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated care data (v49)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9623CC74-6644-441D-8F09-CAB6A8A68A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A00F1D-BB3F-45E4-8D42-FFDF46C6DAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="2070" windowWidth="13570" windowHeight="17120" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="750" yWindow="1180" windowWidth="21240" windowHeight="18960" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="266">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -749,6 +749,84 @@
   </si>
   <si>
     <t>Thuis met Zorg Zaanstreek B.V.</t>
+  </si>
+  <si>
+    <t>Ambiq (Stichting)</t>
+  </si>
+  <si>
+    <t>Avoord Zorg en Wonen (Stichting)</t>
+  </si>
+  <si>
+    <t>DeniseZorg B.V.</t>
+  </si>
+  <si>
+    <t>Dienstencentrum Oud Burgeren Gasthuis (OBG) (Stichting)</t>
+  </si>
+  <si>
+    <t>DZN B.V. (directe zorg nijmegen)</t>
+  </si>
+  <si>
+    <t>Emergis (Stichting)</t>
+  </si>
+  <si>
+    <t>ENA</t>
+  </si>
+  <si>
+    <t>Futura Zorg</t>
+  </si>
+  <si>
+    <t>GGz Centraal (Stichting)</t>
+  </si>
+  <si>
+    <t>GGZ Noord-Holland-Noord (NHN) (Stichting)</t>
+  </si>
+  <si>
+    <t>GGZ Westelijk Noord-Brabant / GGZ-WNB (Stichting)</t>
+  </si>
+  <si>
+    <t>Hervormde Stichting Sonneburgh</t>
+  </si>
+  <si>
+    <t>Ivovum</t>
+  </si>
+  <si>
+    <t>Kwintes (Stichting)</t>
+  </si>
+  <si>
+    <t>Lister (Stichting)</t>
+  </si>
+  <si>
+    <t>Odion (Stichting)</t>
+  </si>
+  <si>
+    <t>Omega (Groep, Zwolle!)</t>
+  </si>
+  <si>
+    <t>Radiotherapiegroep</t>
+  </si>
+  <si>
+    <t>Saffier - De Residentie (Stichting Zorginstelling ...))</t>
+  </si>
+  <si>
+    <t>Savant, Organisatie voor Zorg (Stichting)</t>
+  </si>
+  <si>
+    <t>Vecht &amp; Ijssel (Stichting)</t>
+  </si>
+  <si>
+    <t>Vivium zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>WilgaerdenLeekerweide Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>ZGT</t>
+  </si>
+  <si>
+    <t>Zorggroep Florence (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorggroep Tangenborgh (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -1109,9 +1187,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B238"/>
+  <dimension ref="A1:B264"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1209,7 +1289,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>240</v>
       </c>
       <c r="B12" t="s">
         <v>216</v>
@@ -1217,7 +1297,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>175</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
         <v>216</v>
@@ -1225,39 +1305,39 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="B14" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>191</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>191</v>
       </c>
       <c r="B17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>216</v>
@@ -1265,7 +1345,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
         <v>216</v>
@@ -1273,7 +1353,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
         <v>216</v>
@@ -1281,15 +1361,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>241</v>
       </c>
       <c r="B22" t="s">
         <v>216</v>
@@ -1297,15 +1377,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>133</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
         <v>216</v>
@@ -1313,23 +1393,23 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>200</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="B26" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>200</v>
       </c>
       <c r="B27" t="s">
         <v>215</v>
@@ -1337,7 +1417,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
         <v>215</v>
@@ -1345,7 +1425,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>168</v>
+        <v>125</v>
       </c>
       <c r="B29" t="s">
         <v>215</v>
@@ -1353,7 +1433,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
         <v>215</v>
@@ -1361,15 +1441,15 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
         <v>215</v>
@@ -1377,7 +1457,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>178</v>
       </c>
       <c r="B33" t="s">
         <v>216</v>
@@ -1385,7 +1465,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
         <v>215</v>
@@ -1393,23 +1473,23 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>179</v>
       </c>
       <c r="B37" t="s">
         <v>215</v>
@@ -1417,7 +1497,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="B38" t="s">
         <v>216</v>
@@ -1425,15 +1505,15 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
         <v>216</v>
@@ -1441,7 +1521,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="B41" t="s">
         <v>216</v>
@@ -1449,23 +1529,23 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>172</v>
+        <v>119</v>
       </c>
       <c r="B42" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>173</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>172</v>
       </c>
       <c r="B44" t="s">
         <v>215</v>
@@ -1473,15 +1553,15 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="B45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
         <v>215</v>
@@ -1489,15 +1569,15 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="B47" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>201</v>
       </c>
       <c r="B48" t="s">
         <v>215</v>
@@ -1505,7 +1585,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>218</v>
+        <v>180</v>
       </c>
       <c r="B49" t="s">
         <v>215</v>
@@ -1513,7 +1593,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>22</v>
+        <v>136</v>
       </c>
       <c r="B50" t="s">
         <v>215</v>
@@ -1521,7 +1601,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>112</v>
+        <v>218</v>
       </c>
       <c r="B51" t="s">
         <v>215</v>
@@ -1529,15 +1609,15 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>242</v>
       </c>
       <c r="B52" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>219</v>
+        <v>22</v>
       </c>
       <c r="B53" t="s">
         <v>215</v>
@@ -1545,15 +1625,15 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="B54" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>243</v>
       </c>
       <c r="B55" t="s">
         <v>216</v>
@@ -1561,7 +1641,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B56" t="s">
         <v>215</v>
@@ -1569,31 +1649,31 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>219</v>
       </c>
       <c r="B57" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B58" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>137</v>
+        <v>25</v>
       </c>
       <c r="B59" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>220</v>
+        <v>26</v>
       </c>
       <c r="B60" t="s">
         <v>215</v>
@@ -1601,7 +1681,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>164</v>
+        <v>244</v>
       </c>
       <c r="B61" t="s">
         <v>215</v>
@@ -1609,15 +1689,15 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B62" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>30</v>
+        <v>245</v>
       </c>
       <c r="B63" t="s">
         <v>215</v>
@@ -1625,15 +1705,15 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>31</v>
+        <v>246</v>
       </c>
       <c r="B64" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>123</v>
+        <v>28</v>
       </c>
       <c r="B65" t="s">
         <v>215</v>
@@ -1641,7 +1721,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
       <c r="B66" t="s">
         <v>215</v>
@@ -1649,15 +1729,15 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>33</v>
+        <v>220</v>
       </c>
       <c r="B67" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="B68" t="s">
         <v>215</v>
@@ -1665,47 +1745,47 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>247</v>
       </c>
       <c r="B69" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B70" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
       <c r="B71" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>207</v>
+        <v>248</v>
       </c>
       <c r="B72" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B73" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>192</v>
+        <v>123</v>
       </c>
       <c r="B74" t="s">
         <v>215</v>
@@ -1713,7 +1793,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>169</v>
+        <v>32</v>
       </c>
       <c r="B75" t="s">
         <v>215</v>
@@ -1721,7 +1801,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
       <c r="B76" t="s">
         <v>216</v>
@@ -1729,7 +1809,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="B77" t="s">
         <v>216</v>
@@ -1737,7 +1817,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B78" t="s">
         <v>216</v>
@@ -1745,15 +1825,15 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>37</v>
+        <v>251</v>
       </c>
       <c r="B79" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>140</v>
+        <v>181</v>
       </c>
       <c r="B80" t="s">
         <v>215</v>
@@ -1761,7 +1841,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>231</v>
+        <v>138</v>
       </c>
       <c r="B81" t="s">
         <v>215</v>
@@ -1769,23 +1849,23 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>202</v>
+        <v>34</v>
       </c>
       <c r="B82" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B83" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>38</v>
+        <v>207</v>
       </c>
       <c r="B84" t="s">
         <v>215</v>
@@ -1793,7 +1873,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>232</v>
+        <v>35</v>
       </c>
       <c r="B85" t="s">
         <v>216</v>
@@ -1801,7 +1881,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>39</v>
+        <v>192</v>
       </c>
       <c r="B86" t="s">
         <v>215</v>
@@ -1809,31 +1889,31 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="B87" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>40</v>
+        <v>208</v>
       </c>
       <c r="B88" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>194</v>
+        <v>230</v>
       </c>
       <c r="B89" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>141</v>
+        <v>36</v>
       </c>
       <c r="B90" t="s">
         <v>216</v>
@@ -1841,23 +1921,23 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B91" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>209</v>
+        <v>140</v>
       </c>
       <c r="B92" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>170</v>
+        <v>231</v>
       </c>
       <c r="B93" t="s">
         <v>215</v>
@@ -1865,23 +1945,23 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>42</v>
+        <v>252</v>
       </c>
       <c r="B94" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>43</v>
+        <v>202</v>
       </c>
       <c r="B95" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>182</v>
+        <v>127</v>
       </c>
       <c r="B96" t="s">
         <v>215</v>
@@ -1889,7 +1969,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>233</v>
+        <v>38</v>
       </c>
       <c r="B97" t="s">
         <v>215</v>
@@ -1897,15 +1977,15 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>102</v>
+        <v>232</v>
       </c>
       <c r="B98" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>142</v>
+        <v>39</v>
       </c>
       <c r="B99" t="s">
         <v>215</v>
@@ -1913,31 +1993,31 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="B100" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>143</v>
+        <v>40</v>
       </c>
       <c r="B101" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>44</v>
+        <v>194</v>
       </c>
       <c r="B102" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>45</v>
+        <v>141</v>
       </c>
       <c r="B103" t="s">
         <v>216</v>
@@ -1945,55 +2025,55 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>165</v>
+        <v>41</v>
       </c>
       <c r="B104" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="B105" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
       <c r="B106" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B107" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>183</v>
+        <v>253</v>
       </c>
       <c r="B108" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="B109" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>48</v>
+        <v>182</v>
       </c>
       <c r="B110" t="s">
         <v>215</v>
@@ -2001,15 +2081,15 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>49</v>
+        <v>233</v>
       </c>
       <c r="B111" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B112" t="s">
         <v>215</v>
@@ -2017,15 +2097,15 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>221</v>
+        <v>142</v>
       </c>
       <c r="B113" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>50</v>
+        <v>210</v>
       </c>
       <c r="B114" t="s">
         <v>215</v>
@@ -2033,7 +2113,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>51</v>
+        <v>143</v>
       </c>
       <c r="B115" t="s">
         <v>216</v>
@@ -2041,15 +2121,15 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B116" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B117" t="s">
         <v>216</v>
@@ -2057,7 +2137,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>54</v>
+        <v>165</v>
       </c>
       <c r="B118" t="s">
         <v>215</v>
@@ -2065,7 +2145,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>203</v>
+        <v>254</v>
       </c>
       <c r="B119" t="s">
         <v>216</v>
@@ -2073,31 +2153,31 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>144</v>
+        <v>234</v>
       </c>
       <c r="B120" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>204</v>
+        <v>46</v>
       </c>
       <c r="B121" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>145</v>
+        <v>47</v>
       </c>
       <c r="B122" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>55</v>
+        <v>183</v>
       </c>
       <c r="B123" t="s">
         <v>215</v>
@@ -2105,15 +2185,15 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="B124" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B125" t="s">
         <v>215</v>
@@ -2121,7 +2201,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>146</v>
+        <v>49</v>
       </c>
       <c r="B126" t="s">
         <v>216</v>
@@ -2129,15 +2209,15 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="B127" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>107</v>
+        <v>221</v>
       </c>
       <c r="B128" t="s">
         <v>216</v>
@@ -2145,7 +2225,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="B129" t="s">
         <v>215</v>
@@ -2153,87 +2233,87 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B130" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B131" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B132" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>147</v>
+        <v>255</v>
       </c>
       <c r="B133" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="B134" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B135" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="B136" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
       <c r="B137" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>64</v>
+        <v>204</v>
       </c>
       <c r="B138" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>115</v>
+        <v>145</v>
       </c>
       <c r="B139" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="B140" t="s">
         <v>215</v>
@@ -2241,31 +2321,31 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>148</v>
+        <v>56</v>
       </c>
       <c r="B141" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>211</v>
+        <v>57</v>
       </c>
       <c r="B142" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
       <c r="B143" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>120</v>
+        <v>58</v>
       </c>
       <c r="B144" t="s">
         <v>216</v>
@@ -2273,15 +2353,15 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>222</v>
+        <v>107</v>
       </c>
       <c r="B145" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>235</v>
+        <v>108</v>
       </c>
       <c r="B146" t="s">
         <v>215</v>
@@ -2289,7 +2369,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="B147" t="s">
         <v>215</v>
@@ -2297,23 +2377,23 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>185</v>
+        <v>60</v>
       </c>
       <c r="B148" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B149" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>236</v>
+        <v>147</v>
       </c>
       <c r="B150" t="s">
         <v>215</v>
@@ -2321,7 +2401,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="B151" t="s">
         <v>215</v>
@@ -2329,23 +2409,23 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>237</v>
+        <v>62</v>
       </c>
       <c r="B152" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>66</v>
+        <v>184</v>
       </c>
       <c r="B153" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B154" t="s">
         <v>215</v>
@@ -2353,7 +2433,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>223</v>
+        <v>64</v>
       </c>
       <c r="B155" t="s">
         <v>216</v>
@@ -2361,15 +2441,15 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>224</v>
+        <v>115</v>
       </c>
       <c r="B156" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>177</v>
+        <v>116</v>
       </c>
       <c r="B157" t="s">
         <v>215</v>
@@ -2377,7 +2457,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>68</v>
+        <v>257</v>
       </c>
       <c r="B158" t="s">
         <v>216</v>
@@ -2385,39 +2465,39 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>238</v>
+        <v>148</v>
       </c>
       <c r="B159" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="B160" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B161" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="B162" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>121</v>
+        <v>222</v>
       </c>
       <c r="B163" t="s">
         <v>215</v>
@@ -2425,7 +2505,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>124</v>
+        <v>235</v>
       </c>
       <c r="B164" t="s">
         <v>215</v>
@@ -2433,15 +2513,15 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>70</v>
+        <v>212</v>
       </c>
       <c r="B165" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="B166" t="s">
         <v>215</v>
@@ -2449,7 +2529,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B167" t="s">
         <v>216</v>
@@ -2457,15 +2537,15 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>104</v>
+        <v>236</v>
       </c>
       <c r="B168" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>72</v>
+        <v>149</v>
       </c>
       <c r="B169" t="s">
         <v>215</v>
@@ -2473,23 +2553,23 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>150</v>
+        <v>237</v>
       </c>
       <c r="B170" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>151</v>
+        <v>66</v>
       </c>
       <c r="B171" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>152</v>
+        <v>258</v>
       </c>
       <c r="B172" t="s">
         <v>216</v>
@@ -2497,31 +2577,31 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>174</v>
+        <v>67</v>
       </c>
       <c r="B173" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="B174" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>73</v>
+        <v>224</v>
       </c>
       <c r="B175" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>74</v>
+        <v>259</v>
       </c>
       <c r="B176" t="s">
         <v>215</v>
@@ -2529,15 +2609,15 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>176</v>
+        <v>68</v>
       </c>
       <c r="B178" t="s">
         <v>216</v>
@@ -2545,39 +2625,39 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>75</v>
+        <v>238</v>
       </c>
       <c r="B179" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="B180" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>239</v>
+        <v>117</v>
       </c>
       <c r="B181" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B182" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>77</v>
+        <v>121</v>
       </c>
       <c r="B183" t="s">
         <v>215</v>
@@ -2585,15 +2665,15 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="B184" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B185" t="s">
         <v>216</v>
@@ -2601,7 +2681,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="B186" t="s">
         <v>215</v>
@@ -2609,7 +2689,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B187" t="s">
         <v>216</v>
@@ -2617,7 +2697,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="B188" t="s">
         <v>216</v>
@@ -2625,7 +2705,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="B189" t="s">
         <v>215</v>
@@ -2633,7 +2713,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>81</v>
+        <v>150</v>
       </c>
       <c r="B190" t="s">
         <v>216</v>
@@ -2641,15 +2721,15 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>82</v>
+        <v>151</v>
       </c>
       <c r="B191" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="B192" t="s">
         <v>216</v>
@@ -2657,55 +2737,55 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>225</v>
+        <v>174</v>
       </c>
       <c r="B193" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
       <c r="B194" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="B195" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>155</v>
+        <v>74</v>
       </c>
       <c r="B196" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>84</v>
+        <v>176</v>
       </c>
       <c r="B197" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>85</v>
+        <v>176</v>
       </c>
       <c r="B198" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
       <c r="B199" t="s">
         <v>216</v>
@@ -2713,15 +2793,15 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="B200" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>188</v>
+        <v>239</v>
       </c>
       <c r="B201" t="s">
         <v>215</v>
@@ -2729,15 +2809,15 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>226</v>
+        <v>76</v>
       </c>
       <c r="B202" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B203" t="s">
         <v>215</v>
@@ -2745,39 +2825,39 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>205</v>
+        <v>154</v>
       </c>
       <c r="B204" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>197</v>
+        <v>78</v>
       </c>
       <c r="B205" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>110</v>
+        <v>186</v>
       </c>
       <c r="B206" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>87</v>
+        <v>260</v>
       </c>
       <c r="B207" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B208" t="s">
         <v>216</v>
@@ -2785,31 +2865,31 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B209" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="B210" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>227</v>
+        <v>81</v>
       </c>
       <c r="B211" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B212" t="s">
         <v>216</v>
@@ -2817,7 +2897,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B213" t="s">
         <v>216</v>
@@ -2825,15 +2905,15 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>93</v>
+        <v>225</v>
       </c>
       <c r="B214" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>228</v>
+        <v>261</v>
       </c>
       <c r="B215" t="s">
         <v>216</v>
@@ -2841,31 +2921,31 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B216" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="B217" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>198</v>
+        <v>155</v>
       </c>
       <c r="B218" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>214</v>
+        <v>84</v>
       </c>
       <c r="B219" t="s">
         <v>215</v>
@@ -2873,7 +2953,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="B220" t="s">
         <v>215</v>
@@ -2881,15 +2961,15 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>94</v>
+        <v>262</v>
       </c>
       <c r="B221" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B222" t="s">
         <v>216</v>
@@ -2897,7 +2977,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
       <c r="B223" t="s">
         <v>215</v>
@@ -2905,15 +2985,15 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>95</v>
+        <v>188</v>
       </c>
       <c r="B224" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>130</v>
+        <v>226</v>
       </c>
       <c r="B225" t="s">
         <v>215</v>
@@ -2921,15 +3001,15 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>166</v>
+        <v>86</v>
       </c>
       <c r="B226" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="B227" t="s">
         <v>215</v>
@@ -2937,23 +3017,23 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>96</v>
+        <v>197</v>
       </c>
       <c r="B228" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>199</v>
+        <v>110</v>
       </c>
       <c r="B229" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>189</v>
+        <v>87</v>
       </c>
       <c r="B230" t="s">
         <v>215</v>
@@ -2961,15 +3041,15 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B231" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>229</v>
+        <v>89</v>
       </c>
       <c r="B232" t="s">
         <v>215</v>
@@ -2977,15 +3057,15 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>98</v>
+        <v>263</v>
       </c>
       <c r="B233" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B234" t="s">
         <v>216</v>
@@ -2993,15 +3073,15 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>100</v>
+        <v>227</v>
       </c>
       <c r="B235" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B236" t="s">
         <v>216</v>
@@ -3009,17 +3089,225 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>190</v>
+        <v>92</v>
       </c>
       <c r="B237" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
+        <v>93</v>
+      </c>
+      <c r="B238" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A239" t="s">
+        <v>228</v>
+      </c>
+      <c r="B239" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A240" t="s">
+        <v>171</v>
+      </c>
+      <c r="B240" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
+        <v>157</v>
+      </c>
+      <c r="B241" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A242" t="s">
+        <v>198</v>
+      </c>
+      <c r="B242" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A243" t="s">
+        <v>214</v>
+      </c>
+      <c r="B243" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A244" t="s">
+        <v>118</v>
+      </c>
+      <c r="B244" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A245" t="s">
+        <v>94</v>
+      </c>
+      <c r="B245" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A246" t="s">
+        <v>158</v>
+      </c>
+      <c r="B246" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
+        <v>159</v>
+      </c>
+      <c r="B247" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A248" t="s">
+        <v>95</v>
+      </c>
+      <c r="B248" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A249" t="s">
+        <v>264</v>
+      </c>
+      <c r="B249" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A250" t="s">
+        <v>130</v>
+      </c>
+      <c r="B250" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A251" t="s">
+        <v>166</v>
+      </c>
+      <c r="B251" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A252" t="s">
+        <v>160</v>
+      </c>
+      <c r="B252" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A253" t="s">
+        <v>265</v>
+      </c>
+      <c r="B253" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A254" t="s">
+        <v>96</v>
+      </c>
+      <c r="B254" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
+        <v>199</v>
+      </c>
+      <c r="B255" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
+        <v>189</v>
+      </c>
+      <c r="B256" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>97</v>
+      </c>
+      <c r="B257" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
+        <v>229</v>
+      </c>
+      <c r="B258" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>98</v>
+      </c>
+      <c r="B259" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
+        <v>99</v>
+      </c>
+      <c r="B260" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
+        <v>100</v>
+      </c>
+      <c r="B261" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
+        <v>101</v>
+      </c>
+      <c r="B262" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
+        <v>190</v>
+      </c>
+      <c r="B263" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A264" t="s">
         <v>161</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B264" t="s">
         <v>216</v>
       </c>
     </row>

</xml_diff>

<commit_message>
U[dated care data (v51)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A00F1D-BB3F-45E4-8D42-FFDF46C6DAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6635CF0E-8C83-437B-B7B0-158719E46DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="1180" windowWidth="21240" windowHeight="18960" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="580" yWindow="1680" windowWidth="24210" windowHeight="16100" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="269">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -827,6 +827,15 @@
   </si>
   <si>
     <t>Zorggroep Tangenborgh (Stichting)</t>
+  </si>
+  <si>
+    <t>Oktober</t>
+  </si>
+  <si>
+    <t>SVVG De Schutse (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorggroep Noord- en Midden-Limburg / De Zorggroep (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -1187,11 +1196,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B264"/>
+  <dimension ref="A1:B267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1212,7 +1219,7 @@
         <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1260,7 +1267,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1316,7 +1323,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -1380,7 +1387,7 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1436,7 +1443,7 @@
         <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -1468,7 +1475,7 @@
         <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -1492,7 +1499,7 @@
         <v>179</v>
       </c>
       <c r="B37" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -1548,7 +1555,7 @@
         <v>172</v>
       </c>
       <c r="B44" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1580,7 +1587,7 @@
         <v>201</v>
       </c>
       <c r="B48" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -1588,7 +1595,7 @@
         <v>180</v>
       </c>
       <c r="B49" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1596,7 +1603,7 @@
         <v>136</v>
       </c>
       <c r="B50" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -1604,7 +1611,7 @@
         <v>218</v>
       </c>
       <c r="B51" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -1628,7 +1635,7 @@
         <v>112</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -1644,7 +1651,7 @@
         <v>23</v>
       </c>
       <c r="B56" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -1652,7 +1659,7 @@
         <v>219</v>
       </c>
       <c r="B57" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -1676,7 +1683,7 @@
         <v>26</v>
       </c>
       <c r="B60" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -1684,7 +1691,7 @@
         <v>244</v>
       </c>
       <c r="B61" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -1700,7 +1707,7 @@
         <v>245</v>
       </c>
       <c r="B63" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -1716,7 +1723,7 @@
         <v>28</v>
       </c>
       <c r="B65" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
@@ -1724,7 +1731,7 @@
         <v>137</v>
       </c>
       <c r="B66" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
@@ -1780,7 +1787,7 @@
         <v>31</v>
       </c>
       <c r="B73" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -1788,7 +1795,7 @@
         <v>123</v>
       </c>
       <c r="B74" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -1796,7 +1803,7 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
@@ -1852,7 +1859,7 @@
         <v>34</v>
       </c>
       <c r="B82" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -1892,7 +1899,7 @@
         <v>169</v>
       </c>
       <c r="B87" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -1932,7 +1939,7 @@
         <v>140</v>
       </c>
       <c r="B92" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -1964,7 +1971,7 @@
         <v>127</v>
       </c>
       <c r="B96" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
@@ -2044,7 +2051,7 @@
         <v>170</v>
       </c>
       <c r="B106" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
@@ -2068,7 +2075,7 @@
         <v>43</v>
       </c>
       <c r="B109" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
@@ -2084,7 +2091,7 @@
         <v>233</v>
       </c>
       <c r="B111" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -2100,7 +2107,7 @@
         <v>142</v>
       </c>
       <c r="B113" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
@@ -2180,7 +2187,7 @@
         <v>183</v>
       </c>
       <c r="B123" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -2212,7 +2219,7 @@
         <v>114</v>
       </c>
       <c r="B127" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
@@ -2228,7 +2235,7 @@
         <v>50</v>
       </c>
       <c r="B129" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
@@ -2265,7 +2272,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="B134" t="s">
         <v>216</v>
@@ -2273,23 +2280,23 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="B135" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>203</v>
+        <v>54</v>
       </c>
       <c r="B136" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>144</v>
+        <v>203</v>
       </c>
       <c r="B137" t="s">
         <v>216</v>
@@ -2297,15 +2304,15 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>204</v>
+        <v>144</v>
       </c>
       <c r="B138" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>145</v>
+        <v>204</v>
       </c>
       <c r="B139" t="s">
         <v>215</v>
@@ -2313,7 +2320,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>55</v>
+        <v>145</v>
       </c>
       <c r="B140" t="s">
         <v>215</v>
@@ -2321,7 +2328,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B141" t="s">
         <v>215</v>
@@ -2329,23 +2336,23 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B142" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>146</v>
+        <v>57</v>
       </c>
       <c r="B143" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>58</v>
+        <v>146</v>
       </c>
       <c r="B144" t="s">
         <v>216</v>
@@ -2353,7 +2360,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="B145" t="s">
         <v>216</v>
@@ -2361,15 +2368,15 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B146" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B147" t="s">
         <v>215</v>
@@ -2377,23 +2384,23 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B148" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B149" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>147</v>
+        <v>61</v>
       </c>
       <c r="B150" t="s">
         <v>215</v>
@@ -2401,15 +2408,15 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="B151" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>62</v>
+        <v>128</v>
       </c>
       <c r="B152" t="s">
         <v>216</v>
@@ -2417,15 +2424,15 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>184</v>
+        <v>62</v>
       </c>
       <c r="B153" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>63</v>
+        <v>184</v>
       </c>
       <c r="B154" t="s">
         <v>215</v>
@@ -2433,7 +2440,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B155" t="s">
         <v>216</v>
@@ -2441,7 +2448,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="B156" t="s">
         <v>216</v>
@@ -2449,23 +2456,23 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B157" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>257</v>
+        <v>116</v>
       </c>
       <c r="B158" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>148</v>
+        <v>257</v>
       </c>
       <c r="B159" t="s">
         <v>216</v>
@@ -2473,7 +2480,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>211</v>
+        <v>148</v>
       </c>
       <c r="B160" t="s">
         <v>216</v>
@@ -2481,15 +2488,15 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>109</v>
+        <v>211</v>
       </c>
       <c r="B161" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B162" t="s">
         <v>216</v>
@@ -2497,15 +2504,15 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>222</v>
+        <v>120</v>
       </c>
       <c r="B163" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="B164" t="s">
         <v>215</v>
@@ -2513,7 +2520,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="B165" t="s">
         <v>215</v>
@@ -2521,7 +2528,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="B166" t="s">
         <v>215</v>
@@ -2529,7 +2536,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>65</v>
+        <v>185</v>
       </c>
       <c r="B167" t="s">
         <v>216</v>
@@ -2537,23 +2544,23 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>236</v>
+        <v>65</v>
       </c>
       <c r="B168" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>149</v>
+        <v>236</v>
       </c>
       <c r="B169" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>237</v>
+        <v>149</v>
       </c>
       <c r="B170" t="s">
         <v>215</v>
@@ -2561,7 +2568,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>66</v>
+        <v>237</v>
       </c>
       <c r="B171" t="s">
         <v>216</v>
@@ -2569,7 +2576,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>258</v>
+        <v>66</v>
       </c>
       <c r="B172" t="s">
         <v>216</v>
@@ -2577,87 +2584,87 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>67</v>
+        <v>258</v>
       </c>
       <c r="B173" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>223</v>
+        <v>67</v>
       </c>
       <c r="B174" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B175" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="B176" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>177</v>
+        <v>259</v>
       </c>
       <c r="B177" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>68</v>
+        <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>238</v>
+        <v>68</v>
       </c>
       <c r="B179" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>195</v>
+        <v>238</v>
       </c>
       <c r="B180" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>117</v>
+        <v>195</v>
       </c>
       <c r="B181" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="B182" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>121</v>
+        <v>69</v>
       </c>
       <c r="B183" t="s">
         <v>215</v>
@@ -2665,7 +2672,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B184" t="s">
         <v>215</v>
@@ -2673,31 +2680,31 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="B185" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>213</v>
+        <v>70</v>
       </c>
       <c r="B186" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>71</v>
+        <v>213</v>
       </c>
       <c r="B187" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="B188" t="s">
         <v>216</v>
@@ -2705,15 +2712,15 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="B189" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>150</v>
+        <v>72</v>
       </c>
       <c r="B190" t="s">
         <v>216</v>
@@ -2721,47 +2728,47 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B191" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B192" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="B193" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>196</v>
+        <v>267</v>
       </c>
       <c r="B194" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
       <c r="B195" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>74</v>
+        <v>196</v>
       </c>
       <c r="B196" t="s">
         <v>215</v>
@@ -2769,7 +2776,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>176</v>
+        <v>73</v>
       </c>
       <c r="B197" t="s">
         <v>216</v>
@@ -2777,15 +2784,15 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>176</v>
+        <v>74</v>
       </c>
       <c r="B198" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>75</v>
+        <v>176</v>
       </c>
       <c r="B199" t="s">
         <v>216</v>
@@ -2793,7 +2800,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="B200" t="s">
         <v>216</v>
@@ -2801,15 +2808,15 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>239</v>
+        <v>75</v>
       </c>
       <c r="B201" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>76</v>
+        <v>153</v>
       </c>
       <c r="B202" t="s">
         <v>216</v>
@@ -2817,7 +2824,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>77</v>
+        <v>239</v>
       </c>
       <c r="B203" t="s">
         <v>215</v>
@@ -2825,7 +2832,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>154</v>
+        <v>76</v>
       </c>
       <c r="B204" t="s">
         <v>216</v>
@@ -2833,23 +2840,23 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B205" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="B206" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>260</v>
+        <v>78</v>
       </c>
       <c r="B207" t="s">
         <v>216</v>
@@ -2857,7 +2864,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>79</v>
+        <v>186</v>
       </c>
       <c r="B208" t="s">
         <v>216</v>
@@ -2865,7 +2872,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>80</v>
+        <v>260</v>
       </c>
       <c r="B209" t="s">
         <v>216</v>
@@ -2873,15 +2880,15 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="B210" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B211" t="s">
         <v>216</v>
@@ -2889,15 +2896,15 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="B212" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B213" t="s">
         <v>216</v>
@@ -2905,7 +2912,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>225</v>
+        <v>82</v>
       </c>
       <c r="B214" t="s">
         <v>216</v>
@@ -2913,15 +2920,15 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>261</v>
+        <v>83</v>
       </c>
       <c r="B215" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>162</v>
+        <v>225</v>
       </c>
       <c r="B216" t="s">
         <v>216</v>
@@ -2929,15 +2936,15 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>129</v>
+        <v>261</v>
       </c>
       <c r="B217" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B218" t="s">
         <v>216</v>
@@ -2945,7 +2952,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="B219" t="s">
         <v>215</v>
@@ -2953,23 +2960,23 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>85</v>
+        <v>155</v>
       </c>
       <c r="B220" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>262</v>
+        <v>84</v>
       </c>
       <c r="B221" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="B222" t="s">
         <v>216</v>
@@ -2977,23 +2984,23 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>187</v>
+        <v>262</v>
       </c>
       <c r="B223" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>188</v>
+        <v>156</v>
       </c>
       <c r="B224" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="B225" t="s">
         <v>215</v>
@@ -3001,7 +3008,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>86</v>
+        <v>188</v>
       </c>
       <c r="B226" t="s">
         <v>215</v>
@@ -3009,7 +3016,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="B227" t="s">
         <v>215</v>
@@ -3017,7 +3024,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>197</v>
+        <v>86</v>
       </c>
       <c r="B228" t="s">
         <v>215</v>
@@ -3025,15 +3032,15 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>110</v>
+        <v>205</v>
       </c>
       <c r="B229" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
       <c r="B230" t="s">
         <v>215</v>
@@ -3041,7 +3048,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="B231" t="s">
         <v>216</v>
@@ -3049,15 +3056,15 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B232" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>263</v>
+        <v>88</v>
       </c>
       <c r="B233" t="s">
         <v>216</v>
@@ -3065,23 +3072,23 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B234" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>227</v>
+        <v>263</v>
       </c>
       <c r="B235" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B236" t="s">
         <v>216</v>
@@ -3089,23 +3096,23 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>92</v>
+        <v>227</v>
       </c>
       <c r="B237" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B238" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>228</v>
+        <v>92</v>
       </c>
       <c r="B239" t="s">
         <v>216</v>
@@ -3113,7 +3120,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="B240" t="s">
         <v>215</v>
@@ -3121,7 +3128,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>157</v>
+        <v>228</v>
       </c>
       <c r="B241" t="s">
         <v>216</v>
@@ -3129,7 +3136,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="B242" t="s">
         <v>215</v>
@@ -3137,15 +3144,15 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>214</v>
+        <v>157</v>
       </c>
       <c r="B243" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>118</v>
+        <v>198</v>
       </c>
       <c r="B244" t="s">
         <v>215</v>
@@ -3153,7 +3160,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>94</v>
+        <v>214</v>
       </c>
       <c r="B245" t="s">
         <v>215</v>
@@ -3161,23 +3168,23 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>158</v>
+        <v>118</v>
       </c>
       <c r="B246" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
       <c r="B247" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="B248" t="s">
         <v>216</v>
@@ -3185,7 +3192,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>264</v>
+        <v>159</v>
       </c>
       <c r="B249" t="s">
         <v>216</v>
@@ -3193,15 +3200,15 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="B250" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>166</v>
+        <v>264</v>
       </c>
       <c r="B251" t="s">
         <v>216</v>
@@ -3209,7 +3216,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="B252" t="s">
         <v>215</v>
@@ -3217,7 +3224,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B253" t="s">
         <v>216</v>
@@ -3225,7 +3232,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="B254" t="s">
         <v>216</v>
@@ -3233,7 +3240,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="B255" t="s">
         <v>215</v>
@@ -3241,31 +3248,31 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>189</v>
+        <v>265</v>
       </c>
       <c r="B256" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B257" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="B258" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
       <c r="B259" t="s">
         <v>215</v>
@@ -3273,7 +3280,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B260" t="s">
         <v>216</v>
@@ -3281,7 +3288,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>100</v>
+        <v>229</v>
       </c>
       <c r="B261" t="s">
         <v>216</v>
@@ -3289,25 +3296,49 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B262" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>190</v>
+        <v>99</v>
       </c>
       <c r="B263" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
+        <v>100</v>
+      </c>
+      <c r="B264" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A265" t="s">
+        <v>101</v>
+      </c>
+      <c r="B265" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A266" t="s">
+        <v>190</v>
+      </c>
+      <c r="B266" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A267" t="s">
         <v>161</v>
       </c>
-      <c r="B264" t="s">
+      <c r="B267" t="s">
         <v>216</v>
       </c>
     </row>

</xml_diff>

<commit_message>
U[dated care data (v52)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6635CF0E-8C83-437B-B7B0-158719E46DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E8449F-9043-46E2-9AAC-A91FD49E09F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="1680" windowWidth="24210" windowHeight="16100" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="9740" yWindow="1390" windowWidth="25650" windowHeight="14930" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="274">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -836,6 +836,21 @@
   </si>
   <si>
     <t>Zorggroep Noord- en Midden-Limburg / De Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Ananz wonen-welzijn-zorg (sint anna zorggroep)</t>
+  </si>
+  <si>
+    <t>Envida (Stichting)</t>
+  </si>
+  <si>
+    <t>Hartekamp Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Interakt Contour Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Laverhof (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1211,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B267"/>
+  <dimension ref="A1:B272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1320,7 +1335,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>269</v>
       </c>
       <c r="B15" t="s">
         <v>216</v>
@@ -1328,7 +1343,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>216</v>
@@ -1336,23 +1351,23 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>191</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>191</v>
       </c>
       <c r="B18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
         <v>216</v>
@@ -1360,7 +1375,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
         <v>216</v>
@@ -1368,7 +1383,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>216</v>
@@ -1376,7 +1391,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>241</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
         <v>216</v>
@@ -1384,7 +1399,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>241</v>
       </c>
       <c r="B23" t="s">
         <v>216</v>
@@ -1392,7 +1407,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
         <v>216</v>
@@ -1400,7 +1415,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
         <v>216</v>
@@ -1408,7 +1423,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
         <v>216</v>
@@ -1416,15 +1431,15 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="B27" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>200</v>
       </c>
       <c r="B28" t="s">
         <v>215</v>
@@ -1432,7 +1447,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
         <v>215</v>
@@ -1440,23 +1455,23 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="B30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>168</v>
       </c>
       <c r="B32" t="s">
         <v>215</v>
@@ -1464,15 +1479,15 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>178</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>178</v>
       </c>
       <c r="B34" t="s">
         <v>216</v>
@@ -1480,7 +1495,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
         <v>216</v>
@@ -1488,23 +1503,23 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>179</v>
+        <v>134</v>
       </c>
       <c r="B37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>179</v>
       </c>
       <c r="B38" t="s">
         <v>216</v>
@@ -1512,23 +1527,23 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="B39" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>122</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
         <v>216</v>
@@ -1536,7 +1551,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B42" t="s">
         <v>216</v>
@@ -1544,7 +1559,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="B43" t="s">
         <v>216</v>
@@ -1552,7 +1567,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>172</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
         <v>216</v>
@@ -1560,15 +1575,15 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B45" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>173</v>
       </c>
       <c r="B46" t="s">
         <v>215</v>
@@ -1576,15 +1591,15 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>217</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="B48" t="s">
         <v>216</v>
@@ -1592,7 +1607,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="B49" t="s">
         <v>216</v>
@@ -1600,7 +1615,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>180</v>
       </c>
       <c r="B50" t="s">
         <v>216</v>
@@ -1608,7 +1623,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>218</v>
+        <v>136</v>
       </c>
       <c r="B51" t="s">
         <v>216</v>
@@ -1616,7 +1631,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="B52" t="s">
         <v>216</v>
@@ -1624,23 +1639,23 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>22</v>
+        <v>242</v>
       </c>
       <c r="B53" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="B54" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>243</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
         <v>216</v>
@@ -1648,7 +1663,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>23</v>
+        <v>243</v>
       </c>
       <c r="B56" t="s">
         <v>216</v>
@@ -1656,7 +1671,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>219</v>
+        <v>23</v>
       </c>
       <c r="B57" t="s">
         <v>216</v>
@@ -1664,7 +1679,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>24</v>
+        <v>219</v>
       </c>
       <c r="B58" t="s">
         <v>216</v>
@@ -1672,7 +1687,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B59" t="s">
         <v>216</v>
@@ -1680,7 +1695,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B60" t="s">
         <v>216</v>
@@ -1688,7 +1703,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>244</v>
+        <v>26</v>
       </c>
       <c r="B61" t="s">
         <v>216</v>
@@ -1696,23 +1711,23 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>27</v>
+        <v>244</v>
       </c>
       <c r="B62" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>245</v>
+        <v>27</v>
       </c>
       <c r="B63" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B64" t="s">
         <v>216</v>
@@ -1720,7 +1735,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>28</v>
+        <v>246</v>
       </c>
       <c r="B65" t="s">
         <v>216</v>
@@ -1728,7 +1743,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>137</v>
+        <v>270</v>
       </c>
       <c r="B66" t="s">
         <v>216</v>
@@ -1736,47 +1751,47 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>220</v>
+        <v>28</v>
       </c>
       <c r="B67" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="B68" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>247</v>
+        <v>220</v>
       </c>
       <c r="B69" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="B70" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>30</v>
+        <v>247</v>
       </c>
       <c r="B71" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>248</v>
+        <v>29</v>
       </c>
       <c r="B72" t="s">
         <v>216</v>
@@ -1784,15 +1799,15 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B73" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>123</v>
+        <v>248</v>
       </c>
       <c r="B74" t="s">
         <v>216</v>
@@ -1800,15 +1815,15 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B75" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>249</v>
+        <v>123</v>
       </c>
       <c r="B76" t="s">
         <v>216</v>
@@ -1816,7 +1831,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>250</v>
+        <v>32</v>
       </c>
       <c r="B77" t="s">
         <v>216</v>
@@ -1824,7 +1839,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>33</v>
+        <v>249</v>
       </c>
       <c r="B78" t="s">
         <v>216</v>
@@ -1832,7 +1847,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B79" t="s">
         <v>216</v>
@@ -1840,23 +1855,23 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>181</v>
+        <v>33</v>
       </c>
       <c r="B80" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>138</v>
+        <v>271</v>
       </c>
       <c r="B81" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>34</v>
+        <v>251</v>
       </c>
       <c r="B82" t="s">
         <v>216</v>
@@ -1864,15 +1879,15 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="B83" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="B84" t="s">
         <v>215</v>
@@ -1880,7 +1895,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B85" t="s">
         <v>216</v>
@@ -1888,23 +1903,23 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>192</v>
+        <v>139</v>
       </c>
       <c r="B86" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>169</v>
+        <v>207</v>
       </c>
       <c r="B87" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>208</v>
+        <v>35</v>
       </c>
       <c r="B88" t="s">
         <v>216</v>
@@ -1912,15 +1927,15 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>230</v>
+        <v>192</v>
       </c>
       <c r="B89" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>36</v>
+        <v>169</v>
       </c>
       <c r="B90" t="s">
         <v>216</v>
@@ -1928,15 +1943,15 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>37</v>
+        <v>208</v>
       </c>
       <c r="B91" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>140</v>
+        <v>230</v>
       </c>
       <c r="B92" t="s">
         <v>216</v>
@@ -1944,15 +1959,15 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>231</v>
+        <v>36</v>
       </c>
       <c r="B93" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="B94" t="s">
         <v>216</v>
@@ -1960,15 +1975,15 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>202</v>
+        <v>37</v>
       </c>
       <c r="B95" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B96" t="s">
         <v>216</v>
@@ -1976,7 +1991,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>38</v>
+        <v>231</v>
       </c>
       <c r="B97" t="s">
         <v>215</v>
@@ -1984,7 +1999,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="B98" t="s">
         <v>216</v>
@@ -1992,15 +2007,15 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>39</v>
+        <v>202</v>
       </c>
       <c r="B99" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>193</v>
+        <v>127</v>
       </c>
       <c r="B100" t="s">
         <v>216</v>
@@ -2008,7 +2023,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B101" t="s">
         <v>215</v>
@@ -2016,23 +2031,23 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="B102" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="B103" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>41</v>
+        <v>193</v>
       </c>
       <c r="B104" t="s">
         <v>216</v>
@@ -2040,31 +2055,31 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>209</v>
+        <v>40</v>
       </c>
       <c r="B105" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="B106" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>42</v>
+        <v>141</v>
       </c>
       <c r="B107" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>253</v>
+        <v>41</v>
       </c>
       <c r="B108" t="s">
         <v>216</v>
@@ -2072,7 +2087,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>43</v>
+        <v>209</v>
       </c>
       <c r="B109" t="s">
         <v>216</v>
@@ -2080,31 +2095,31 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="B110" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>233</v>
+        <v>42</v>
       </c>
       <c r="B111" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>102</v>
+        <v>253</v>
       </c>
       <c r="B112" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="B113" t="s">
         <v>216</v>
@@ -2112,7 +2127,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="B114" t="s">
         <v>215</v>
@@ -2120,15 +2135,15 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>143</v>
+        <v>233</v>
       </c>
       <c r="B115" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>44</v>
+        <v>273</v>
       </c>
       <c r="B116" t="s">
         <v>216</v>
@@ -2136,31 +2151,31 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="B117" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="B118" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>254</v>
+        <v>210</v>
       </c>
       <c r="B119" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>234</v>
+        <v>143</v>
       </c>
       <c r="B120" t="s">
         <v>215</v>
@@ -2168,7 +2183,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B121" t="s">
         <v>216</v>
@@ -2176,7 +2191,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B122" t="s">
         <v>216</v>
@@ -2184,15 +2199,15 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="B123" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>113</v>
+        <v>254</v>
       </c>
       <c r="B124" t="s">
         <v>216</v>
@@ -2200,7 +2215,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>48</v>
+        <v>234</v>
       </c>
       <c r="B125" t="s">
         <v>215</v>
@@ -2208,7 +2223,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B126" t="s">
         <v>216</v>
@@ -2216,7 +2231,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="B127" t="s">
         <v>216</v>
@@ -2224,7 +2239,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>221</v>
+        <v>183</v>
       </c>
       <c r="B128" t="s">
         <v>216</v>
@@ -2232,7 +2247,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="B129" t="s">
         <v>216</v>
@@ -2240,23 +2255,23 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B130" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B131" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="B132" t="s">
         <v>216</v>
@@ -2264,7 +2279,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
       <c r="B133" t="s">
         <v>216</v>
@@ -2272,15 +2287,15 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>266</v>
+        <v>50</v>
       </c>
       <c r="B134" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>256</v>
+        <v>51</v>
       </c>
       <c r="B135" t="s">
         <v>216</v>
@@ -2288,7 +2303,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B136" t="s">
         <v>215</v>
@@ -2296,7 +2311,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>203</v>
+        <v>53</v>
       </c>
       <c r="B137" t="s">
         <v>216</v>
@@ -2304,7 +2319,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>144</v>
+        <v>255</v>
       </c>
       <c r="B138" t="s">
         <v>216</v>
@@ -2312,7 +2327,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>204</v>
+        <v>266</v>
       </c>
       <c r="B139" t="s">
         <v>215</v>
@@ -2320,15 +2335,15 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>145</v>
+        <v>256</v>
       </c>
       <c r="B140" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B141" t="s">
         <v>215</v>
@@ -2336,7 +2351,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>56</v>
+        <v>203</v>
       </c>
       <c r="B142" t="s">
         <v>216</v>
@@ -2344,47 +2359,47 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>57</v>
+        <v>144</v>
       </c>
       <c r="B143" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>146</v>
+        <v>204</v>
       </c>
       <c r="B144" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>58</v>
+        <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="B146" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="B147" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B148" t="s">
         <v>215</v>
@@ -2392,7 +2407,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>60</v>
+        <v>146</v>
       </c>
       <c r="B149" t="s">
         <v>216</v>
@@ -2400,15 +2415,15 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B150" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="B151" t="s">
         <v>216</v>
@@ -2416,39 +2431,39 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="B152" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B153" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="B154" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B155" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>64</v>
+        <v>147</v>
       </c>
       <c r="B156" t="s">
         <v>216</v>
@@ -2456,7 +2471,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="B157" t="s">
         <v>216</v>
@@ -2464,23 +2479,23 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="B158" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>257</v>
+        <v>184</v>
       </c>
       <c r="B159" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>148</v>
+        <v>63</v>
       </c>
       <c r="B160" t="s">
         <v>216</v>
@@ -2488,15 +2503,15 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>211</v>
+        <v>64</v>
       </c>
       <c r="B161" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B162" t="s">
         <v>216</v>
@@ -2504,39 +2519,39 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B163" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>222</v>
+        <v>257</v>
       </c>
       <c r="B164" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>235</v>
+        <v>148</v>
       </c>
       <c r="B165" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B166" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>185</v>
+        <v>109</v>
       </c>
       <c r="B167" t="s">
         <v>216</v>
@@ -2544,7 +2559,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="B168" t="s">
         <v>216</v>
@@ -2552,15 +2567,15 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B169" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>149</v>
+        <v>235</v>
       </c>
       <c r="B170" t="s">
         <v>215</v>
@@ -2568,15 +2583,15 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="B171" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>66</v>
+        <v>185</v>
       </c>
       <c r="B172" t="s">
         <v>216</v>
@@ -2584,7 +2599,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>258</v>
+        <v>65</v>
       </c>
       <c r="B173" t="s">
         <v>216</v>
@@ -2592,23 +2607,23 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>67</v>
+        <v>236</v>
       </c>
       <c r="B174" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>223</v>
+        <v>149</v>
       </c>
       <c r="B175" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="B176" t="s">
         <v>216</v>
@@ -2616,7 +2631,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>259</v>
+        <v>66</v>
       </c>
       <c r="B177" t="s">
         <v>216</v>
@@ -2624,23 +2639,23 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>177</v>
+        <v>258</v>
       </c>
       <c r="B178" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B179" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="B180" t="s">
         <v>216</v>
@@ -2648,15 +2663,15 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>195</v>
+        <v>224</v>
       </c>
       <c r="B181" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>117</v>
+        <v>259</v>
       </c>
       <c r="B182" t="s">
         <v>216</v>
@@ -2664,7 +2679,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="B183" t="s">
         <v>215</v>
@@ -2672,63 +2687,63 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
       <c r="B184" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>124</v>
+        <v>238</v>
       </c>
       <c r="B185" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>70</v>
+        <v>195</v>
       </c>
       <c r="B186" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>213</v>
+        <v>117</v>
       </c>
       <c r="B187" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B188" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="B189" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="B190" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>150</v>
+        <v>70</v>
       </c>
       <c r="B191" t="s">
         <v>216</v>
@@ -2736,7 +2751,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>151</v>
+        <v>213</v>
       </c>
       <c r="B192" t="s">
         <v>215</v>
@@ -2744,7 +2759,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>152</v>
+        <v>71</v>
       </c>
       <c r="B193" t="s">
         <v>216</v>
@@ -2752,7 +2767,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>267</v>
+        <v>104</v>
       </c>
       <c r="B194" t="s">
         <v>216</v>
@@ -2760,63 +2775,63 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>174</v>
+        <v>72</v>
       </c>
       <c r="B195" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>196</v>
+        <v>150</v>
       </c>
       <c r="B196" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>73</v>
+        <v>151</v>
       </c>
       <c r="B197" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="B198" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>176</v>
+        <v>267</v>
       </c>
       <c r="B199" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B200" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>75</v>
+        <v>196</v>
       </c>
       <c r="B201" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>153</v>
+        <v>73</v>
       </c>
       <c r="B202" t="s">
         <v>216</v>
@@ -2824,7 +2839,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>239</v>
+        <v>74</v>
       </c>
       <c r="B203" t="s">
         <v>215</v>
@@ -2832,7 +2847,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>76</v>
+        <v>176</v>
       </c>
       <c r="B204" t="s">
         <v>216</v>
@@ -2840,15 +2855,15 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>77</v>
+        <v>176</v>
       </c>
       <c r="B205" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>154</v>
+        <v>75</v>
       </c>
       <c r="B206" t="s">
         <v>216</v>
@@ -2856,7 +2871,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="B207" t="s">
         <v>216</v>
@@ -2864,15 +2879,15 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>186</v>
+        <v>239</v>
       </c>
       <c r="B208" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>260</v>
+        <v>76</v>
       </c>
       <c r="B209" t="s">
         <v>216</v>
@@ -2880,15 +2895,15 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B210" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>80</v>
+        <v>154</v>
       </c>
       <c r="B211" t="s">
         <v>216</v>
@@ -2896,15 +2911,15 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="B212" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>81</v>
+        <v>186</v>
       </c>
       <c r="B213" t="s">
         <v>216</v>
@@ -2912,7 +2927,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>82</v>
+        <v>260</v>
       </c>
       <c r="B214" t="s">
         <v>216</v>
@@ -2920,15 +2935,15 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B215" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>225</v>
+        <v>80</v>
       </c>
       <c r="B216" t="s">
         <v>216</v>
@@ -2936,15 +2951,15 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>261</v>
+        <v>103</v>
       </c>
       <c r="B217" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>162</v>
+        <v>81</v>
       </c>
       <c r="B218" t="s">
         <v>216</v>
@@ -2952,31 +2967,31 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>129</v>
+        <v>82</v>
       </c>
       <c r="B219" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>155</v>
+        <v>83</v>
       </c>
       <c r="B220" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>84</v>
+        <v>225</v>
       </c>
       <c r="B221" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>85</v>
+        <v>261</v>
       </c>
       <c r="B222" t="s">
         <v>216</v>
@@ -2984,7 +2999,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>262</v>
+        <v>162</v>
       </c>
       <c r="B223" t="s">
         <v>216</v>
@@ -2992,23 +3007,23 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="B224" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="B225" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>188</v>
+        <v>84</v>
       </c>
       <c r="B226" t="s">
         <v>215</v>
@@ -3016,31 +3031,31 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>226</v>
+        <v>85</v>
       </c>
       <c r="B227" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>86</v>
+        <v>262</v>
       </c>
       <c r="B228" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>205</v>
+        <v>156</v>
       </c>
       <c r="B229" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B230" t="s">
         <v>215</v>
@@ -3048,31 +3063,31 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
       <c r="B231" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>87</v>
+        <v>226</v>
       </c>
       <c r="B232" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B233" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>89</v>
+        <v>205</v>
       </c>
       <c r="B234" t="s">
         <v>215</v>
@@ -3080,15 +3095,15 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>263</v>
+        <v>197</v>
       </c>
       <c r="B235" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="B236" t="s">
         <v>216</v>
@@ -3096,15 +3111,15 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>227</v>
+        <v>87</v>
       </c>
       <c r="B237" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B238" t="s">
         <v>216</v>
@@ -3112,23 +3127,23 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B239" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>93</v>
+        <v>263</v>
       </c>
       <c r="B240" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>228</v>
+        <v>90</v>
       </c>
       <c r="B241" t="s">
         <v>216</v>
@@ -3136,7 +3151,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>171</v>
+        <v>227</v>
       </c>
       <c r="B242" t="s">
         <v>215</v>
@@ -3144,7 +3159,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>157</v>
+        <v>91</v>
       </c>
       <c r="B243" t="s">
         <v>216</v>
@@ -3152,15 +3167,15 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>198</v>
+        <v>92</v>
       </c>
       <c r="B244" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>214</v>
+        <v>93</v>
       </c>
       <c r="B245" t="s">
         <v>215</v>
@@ -3168,23 +3183,23 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>118</v>
+        <v>228</v>
       </c>
       <c r="B246" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>94</v>
+        <v>171</v>
       </c>
       <c r="B247" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B248" t="s">
         <v>216</v>
@@ -3192,39 +3207,39 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>159</v>
+        <v>198</v>
       </c>
       <c r="B249" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="B250" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>264</v>
+        <v>118</v>
       </c>
       <c r="B251" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="B252" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>268</v>
+        <v>158</v>
       </c>
       <c r="B253" t="s">
         <v>216</v>
@@ -3232,7 +3247,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B254" t="s">
         <v>216</v>
@@ -3240,15 +3255,15 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="B255" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B256" t="s">
         <v>216</v>
@@ -3256,15 +3271,15 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="B257" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>199</v>
+        <v>268</v>
       </c>
       <c r="B258" t="s">
         <v>216</v>
@@ -3272,23 +3287,23 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="B259" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="B260" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>229</v>
+        <v>265</v>
       </c>
       <c r="B261" t="s">
         <v>216</v>
@@ -3296,15 +3311,15 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B262" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>99</v>
+        <v>199</v>
       </c>
       <c r="B263" t="s">
         <v>216</v>
@@ -3312,15 +3327,15 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>100</v>
+        <v>189</v>
       </c>
       <c r="B264" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B265" t="s">
         <v>216</v>
@@ -3328,7 +3343,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>190</v>
+        <v>229</v>
       </c>
       <c r="B266" t="s">
         <v>216</v>
@@ -3336,9 +3351,49 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
+        <v>98</v>
+      </c>
+      <c r="B267" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A268" t="s">
+        <v>99</v>
+      </c>
+      <c r="B268" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A269" t="s">
+        <v>100</v>
+      </c>
+      <c r="B269" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A270" t="s">
+        <v>101</v>
+      </c>
+      <c r="B270" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A271" t="s">
+        <v>190</v>
+      </c>
+      <c r="B271" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A272" t="s">
         <v>161</v>
       </c>
-      <c r="B267" t="s">
+      <c r="B272" t="s">
         <v>216</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated care data (v53)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E8449F-9043-46E2-9AAC-A91FD49E09F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272D675C-FBE9-464C-B15B-CDBE2200AA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9740" yWindow="1390" windowWidth="25650" windowHeight="14930" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="13250" yWindow="460" windowWidth="24170" windowHeight="15410" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="276">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Proteion Groep (Stichting)</t>
   </si>
   <si>
-    <t>PSW (Stichting)</t>
-  </si>
-  <si>
     <t>Rivierduinen</t>
   </si>
   <si>
@@ -574,9 +571,6 @@
     <t>De Wijngaerd (Stichting)</t>
   </si>
   <si>
-    <t>Het Gastenhuis B.V.</t>
-  </si>
-  <si>
     <t>Landelijke Stichting Vredenoord</t>
   </si>
   <si>
@@ -748,9 +742,6 @@
     <t>Sensire (Stichting)</t>
   </si>
   <si>
-    <t>Thuis met Zorg Zaanstreek B.V.</t>
-  </si>
-  <si>
     <t>Ambiq (Stichting)</t>
   </si>
   <si>
@@ -838,12 +829,6 @@
     <t>Zorggroep Noord- en Midden-Limburg / De Zorggroep (Stichting)</t>
   </si>
   <si>
-    <t>Ananz wonen-welzijn-zorg (sint anna zorggroep)</t>
-  </si>
-  <si>
-    <t>Envida (Stichting)</t>
-  </si>
-  <si>
     <t>Hartekamp Groep (Stichting)</t>
   </si>
   <si>
@@ -851,6 +836,27 @@
   </si>
   <si>
     <t>Laverhof (Stichting)</t>
+  </si>
+  <si>
+    <t>Daelzicht (Stichting)</t>
+  </si>
+  <si>
+    <t>Geestelijke gezondheidszorg Oost Brabant (Stichting)</t>
+  </si>
+  <si>
+    <t>Gemiva-SVG Groep (Stichting)</t>
+  </si>
+  <si>
+    <t>Groenhuysen (Stichting)</t>
+  </si>
+  <si>
+    <t>Markenheem, Centra voor Zorg en Dienstverlening (Stichting)</t>
+  </si>
+  <si>
+    <t>Patyna (Stichting)</t>
+  </si>
+  <si>
+    <t>Vredewold (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -915,9 +921,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -955,7 +961,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1061,7 +1067,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1203,7 +1209,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1211,7 +1217,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B272"/>
+  <dimension ref="A1:B274"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1231,10 +1237,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1242,7 +1248,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1250,31 +1256,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1282,15 +1288,15 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1298,7 +1304,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1306,343 +1312,343 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>269</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>132</v>
+        <v>189</v>
       </c>
       <c r="B17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>191</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>238</v>
       </c>
       <c r="B22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>241</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>132</v>
       </c>
       <c r="B26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>133</v>
+        <v>198</v>
       </c>
       <c r="B27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>200</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="B29" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="B31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>177</v>
       </c>
       <c r="B33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>178</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>133</v>
       </c>
       <c r="B36" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>178</v>
       </c>
       <c r="B37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>179</v>
+        <v>134</v>
       </c>
       <c r="B38" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="B41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>269</v>
       </c>
       <c r="B44" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B49" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B51" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B52" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B53" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -1650,23 +1656,23 @@
         <v>22</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B55" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B56" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -1674,15 +1680,15 @@
         <v>23</v>
       </c>
       <c r="B57" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B58" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -1690,7 +1696,7 @@
         <v>24</v>
       </c>
       <c r="B59" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -1698,7 +1704,7 @@
         <v>25</v>
       </c>
       <c r="B60" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -1706,15 +1712,15 @@
         <v>26</v>
       </c>
       <c r="B61" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B62" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -1722,1679 +1728,1695 @@
         <v>27</v>
       </c>
       <c r="B63" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B64" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B65" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>270</v>
+        <v>28</v>
       </c>
       <c r="B66" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="B67" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>137</v>
+        <v>218</v>
       </c>
       <c r="B68" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>220</v>
+        <v>163</v>
       </c>
       <c r="B69" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>164</v>
+        <v>244</v>
       </c>
       <c r="B70" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>247</v>
+        <v>270</v>
       </c>
       <c r="B71" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>29</v>
+        <v>271</v>
       </c>
       <c r="B72" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B73" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>248</v>
+        <v>30</v>
       </c>
       <c r="B74" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>31</v>
+        <v>245</v>
       </c>
       <c r="B75" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>123</v>
+        <v>31</v>
       </c>
       <c r="B76" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B77" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>249</v>
+        <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B79" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>33</v>
+        <v>247</v>
       </c>
       <c r="B80" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>271</v>
+        <v>33</v>
       </c>
       <c r="B81" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>251</v>
+        <v>272</v>
       </c>
       <c r="B82" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>181</v>
+        <v>266</v>
       </c>
       <c r="B83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>138</v>
+        <v>248</v>
       </c>
       <c r="B84" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>34</v>
+        <v>137</v>
       </c>
       <c r="B85" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>139</v>
+        <v>34</v>
       </c>
       <c r="B86" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="B87" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>35</v>
+        <v>205</v>
       </c>
       <c r="B88" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>192</v>
+        <v>35</v>
       </c>
       <c r="B89" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="B90" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>208</v>
+        <v>168</v>
       </c>
       <c r="B91" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="B92" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>36</v>
+        <v>228</v>
       </c>
       <c r="B93" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>272</v>
+        <v>36</v>
       </c>
       <c r="B94" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>37</v>
+        <v>267</v>
       </c>
       <c r="B95" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>140</v>
+        <v>37</v>
       </c>
       <c r="B96" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>231</v>
+        <v>139</v>
       </c>
       <c r="B97" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
       <c r="B98" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>202</v>
+        <v>249</v>
       </c>
       <c r="B99" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>127</v>
+        <v>200</v>
       </c>
       <c r="B100" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="B101" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>232</v>
+        <v>38</v>
       </c>
       <c r="B102" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>39</v>
+        <v>230</v>
       </c>
       <c r="B103" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>193</v>
+        <v>39</v>
       </c>
       <c r="B104" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>40</v>
+        <v>191</v>
       </c>
       <c r="B105" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>194</v>
+        <v>40</v>
       </c>
       <c r="B106" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
       <c r="B107" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>41</v>
+        <v>140</v>
       </c>
       <c r="B108" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>209</v>
+        <v>41</v>
       </c>
       <c r="B109" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="B110" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>42</v>
+        <v>169</v>
       </c>
       <c r="B111" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>253</v>
+        <v>42</v>
       </c>
       <c r="B112" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>43</v>
+        <v>250</v>
       </c>
       <c r="B113" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>182</v>
+        <v>43</v>
       </c>
       <c r="B114" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>233</v>
+        <v>180</v>
       </c>
       <c r="B115" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>273</v>
+        <v>231</v>
       </c>
       <c r="B116" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>102</v>
+        <v>268</v>
       </c>
       <c r="B117" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="B118" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>210</v>
+        <v>141</v>
       </c>
       <c r="B119" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>143</v>
+        <v>208</v>
       </c>
       <c r="B120" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="B121" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B122" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>165</v>
+        <v>45</v>
       </c>
       <c r="B123" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>254</v>
+        <v>164</v>
       </c>
       <c r="B124" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="B125" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>46</v>
+        <v>232</v>
       </c>
       <c r="B126" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B127" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>183</v>
+        <v>47</v>
       </c>
       <c r="B128" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>113</v>
+        <v>181</v>
       </c>
       <c r="B129" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>48</v>
+        <v>273</v>
       </c>
       <c r="B130" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="B131" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="B132" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>221</v>
+        <v>49</v>
       </c>
       <c r="B133" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="B134" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>51</v>
+        <v>219</v>
       </c>
       <c r="B135" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B136" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B137" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>255</v>
+        <v>52</v>
       </c>
       <c r="B138" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>266</v>
+        <v>53</v>
       </c>
       <c r="B139" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B140" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>54</v>
+        <v>263</v>
       </c>
       <c r="B141" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>203</v>
+        <v>253</v>
       </c>
       <c r="B142" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="B143" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B144" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>55</v>
+        <v>202</v>
       </c>
       <c r="B146" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>56</v>
+        <v>144</v>
       </c>
       <c r="B147" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B148" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="B149" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B150" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="B151" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>108</v>
+        <v>274</v>
       </c>
       <c r="B152" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B153" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="B154" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="B155" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>147</v>
+        <v>59</v>
       </c>
       <c r="B156" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>128</v>
+        <v>60</v>
       </c>
       <c r="B157" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B158" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>184</v>
+        <v>146</v>
       </c>
       <c r="B159" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>63</v>
+        <v>127</v>
       </c>
       <c r="B160" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B161" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="B162" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="B163" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>257</v>
+        <v>114</v>
       </c>
       <c r="B164" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
       <c r="B165" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>211</v>
+        <v>254</v>
       </c>
       <c r="B166" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="B167" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="B168" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>222</v>
+        <v>108</v>
       </c>
       <c r="B169" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>235</v>
+        <v>119</v>
       </c>
       <c r="B170" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B171" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
       <c r="B172" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>65</v>
+        <v>210</v>
       </c>
       <c r="B173" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>236</v>
+        <v>183</v>
       </c>
       <c r="B174" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>149</v>
+        <v>64</v>
       </c>
       <c r="B175" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B176" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>66</v>
+        <v>148</v>
       </c>
       <c r="B177" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
       <c r="B178" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B179" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
       <c r="B180" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>224</v>
+        <v>66</v>
       </c>
       <c r="B181" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="B182" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
       <c r="B183" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>68</v>
+        <v>256</v>
       </c>
       <c r="B184" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>238</v>
+        <v>176</v>
       </c>
       <c r="B185" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>195</v>
+        <v>67</v>
       </c>
       <c r="B186" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>117</v>
+        <v>236</v>
       </c>
       <c r="B187" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>69</v>
+        <v>193</v>
       </c>
       <c r="B188" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B189" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="B190" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="B191" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>213</v>
+        <v>123</v>
       </c>
       <c r="B192" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B193" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>104</v>
+        <v>211</v>
       </c>
       <c r="B194" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B195" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="B196" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>151</v>
+        <v>71</v>
       </c>
       <c r="B197" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B198" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>267</v>
+        <v>150</v>
       </c>
       <c r="B199" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="B200" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>196</v>
+        <v>264</v>
       </c>
       <c r="B201" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>73</v>
+        <v>173</v>
       </c>
       <c r="B202" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>74</v>
+        <v>194</v>
       </c>
       <c r="B203" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>176</v>
+        <v>72</v>
       </c>
       <c r="B204" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>176</v>
+        <v>73</v>
       </c>
       <c r="B205" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="B206" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="B207" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>239</v>
+        <v>74</v>
       </c>
       <c r="B208" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="B209" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B210" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>154</v>
+        <v>76</v>
       </c>
       <c r="B211" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="B212" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>186</v>
+        <v>77</v>
       </c>
       <c r="B213" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>260</v>
+        <v>184</v>
       </c>
       <c r="B214" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>79</v>
+        <v>257</v>
       </c>
       <c r="B215" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B216" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="B217" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="B218" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B219" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B220" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>225</v>
+        <v>82</v>
       </c>
       <c r="B221" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="B222" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>162</v>
+        <v>258</v>
       </c>
       <c r="B223" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>129</v>
+        <v>275</v>
       </c>
       <c r="B224" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B225" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="B226" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>85</v>
+        <v>154</v>
       </c>
       <c r="B227" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>262</v>
+        <v>83</v>
       </c>
       <c r="B228" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>156</v>
+        <v>84</v>
       </c>
       <c r="B229" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>187</v>
+        <v>259</v>
       </c>
       <c r="B230" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="B231" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>226</v>
+        <v>185</v>
       </c>
       <c r="B232" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>86</v>
+        <v>186</v>
       </c>
       <c r="B233" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="B234" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>197</v>
+        <v>85</v>
       </c>
       <c r="B235" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="B236" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="B237" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="B238" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B239" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>263</v>
+        <v>87</v>
       </c>
       <c r="B240" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B241" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>227</v>
+        <v>260</v>
       </c>
       <c r="B242" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B243" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>92</v>
+        <v>225</v>
       </c>
       <c r="B244" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B245" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>228</v>
+        <v>91</v>
       </c>
       <c r="B246" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>171</v>
+        <v>92</v>
       </c>
       <c r="B247" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>157</v>
+        <v>226</v>
       </c>
       <c r="B248" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="B249" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>214</v>
+        <v>156</v>
       </c>
       <c r="B250" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>118</v>
+        <v>196</v>
       </c>
       <c r="B251" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>94</v>
+        <v>212</v>
       </c>
       <c r="B252" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="B253" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>159</v>
+        <v>93</v>
       </c>
       <c r="B254" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
       <c r="B255" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>264</v>
+        <v>158</v>
       </c>
       <c r="B256" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="B257" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="B258" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="B259" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>160</v>
+        <v>265</v>
       </c>
       <c r="B260" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>265</v>
+        <v>165</v>
       </c>
       <c r="B261" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>96</v>
+        <v>159</v>
       </c>
       <c r="B262" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>199</v>
+        <v>262</v>
       </c>
       <c r="B263" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>189</v>
+        <v>95</v>
       </c>
       <c r="B264" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>97</v>
+        <v>197</v>
       </c>
       <c r="B265" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>229</v>
+        <v>187</v>
       </c>
       <c r="B266" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B267" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>99</v>
+        <v>227</v>
       </c>
       <c r="B268" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B269" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B270" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>190</v>
+        <v>99</v>
       </c>
       <c r="B271" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>161</v>
+        <v>100</v>
       </c>
       <c r="B272" t="s">
-        <v>216</v>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A273" t="s">
+        <v>188</v>
+      </c>
+      <c r="B273" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A274" t="s">
+        <v>160</v>
+      </c>
+      <c r="B274" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected care data (v53)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272D675C-FBE9-464C-B15B-CDBE2200AA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B0C2FB-089A-442C-B831-DC7277FB7A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13250" yWindow="460" windowWidth="24170" windowHeight="15410" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="7430" yWindow="1220" windowWidth="27020" windowHeight="19280" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1264,7 +1264,7 @@
         <v>204</v>
       </c>
       <c r="B5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1272,7 +1272,7 @@
         <v>162</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1280,7 +1280,7 @@
         <v>166</v>
       </c>
       <c r="B7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1296,7 +1296,7 @@
         <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1304,7 +1304,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1360,7 +1360,7 @@
         <v>189</v>
       </c>
       <c r="B17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -1440,7 +1440,7 @@
         <v>198</v>
       </c>
       <c r="B27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -1464,7 +1464,7 @@
         <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -1472,7 +1472,7 @@
         <v>167</v>
       </c>
       <c r="B31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -1480,7 +1480,7 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -1488,7 +1488,7 @@
         <v>177</v>
       </c>
       <c r="B33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -1512,7 +1512,7 @@
         <v>133</v>
       </c>
       <c r="B36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -1536,7 +1536,7 @@
         <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1592,7 +1592,7 @@
         <v>172</v>
       </c>
       <c r="B46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -1600,7 +1600,7 @@
         <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -1632,7 +1632,7 @@
         <v>135</v>
       </c>
       <c r="B51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -1768,7 +1768,7 @@
         <v>218</v>
       </c>
       <c r="B68" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
@@ -1792,7 +1792,7 @@
         <v>270</v>
       </c>
       <c r="B71" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -1816,7 +1816,7 @@
         <v>30</v>
       </c>
       <c r="B74" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -1840,7 +1840,7 @@
         <v>122</v>
       </c>
       <c r="B77" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
@@ -1848,7 +1848,7 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -1880,7 +1880,7 @@
         <v>272</v>
       </c>
       <c r="B82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -1888,7 +1888,7 @@
         <v>266</v>
       </c>
       <c r="B83" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
@@ -1896,7 +1896,7 @@
         <v>248</v>
       </c>
       <c r="B84" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -1904,7 +1904,7 @@
         <v>137</v>
       </c>
       <c r="B85" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -1928,7 +1928,7 @@
         <v>205</v>
       </c>
       <c r="B88" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -1984,7 +1984,7 @@
         <v>267</v>
       </c>
       <c r="B95" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -1992,7 +1992,7 @@
         <v>37</v>
       </c>
       <c r="B96" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
@@ -2008,7 +2008,7 @@
         <v>229</v>
       </c>
       <c r="B98" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -2040,7 +2040,7 @@
         <v>38</v>
       </c>
       <c r="B102" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -2056,7 +2056,7 @@
         <v>39</v>
       </c>
       <c r="B104" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
@@ -2072,7 +2072,7 @@
         <v>40</v>
       </c>
       <c r="B106" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
@@ -2120,7 +2120,7 @@
         <v>42</v>
       </c>
       <c r="B112" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -2144,7 +2144,7 @@
         <v>180</v>
       </c>
       <c r="B115" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -2160,7 +2160,7 @@
         <v>268</v>
       </c>
       <c r="B117" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -2184,7 +2184,7 @@
         <v>208</v>
       </c>
       <c r="B120" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -2216,7 +2216,7 @@
         <v>164</v>
       </c>
       <c r="B124" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -2232,7 +2232,7 @@
         <v>232</v>
       </c>
       <c r="B126" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
@@ -2280,7 +2280,7 @@
         <v>48</v>
       </c>
       <c r="B132" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
@@ -2296,7 +2296,7 @@
         <v>113</v>
       </c>
       <c r="B134" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
@@ -2328,7 +2328,7 @@
         <v>52</v>
       </c>
       <c r="B138" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
@@ -2368,7 +2368,7 @@
         <v>54</v>
       </c>
       <c r="B143" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
@@ -2392,7 +2392,7 @@
         <v>202</v>
       </c>
       <c r="B146" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
@@ -2400,7 +2400,7 @@
         <v>144</v>
       </c>
       <c r="B147" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -2424,7 +2424,7 @@
         <v>57</v>
       </c>
       <c r="B150" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
@@ -2464,7 +2464,7 @@
         <v>107</v>
       </c>
       <c r="B155" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
@@ -2488,7 +2488,7 @@
         <v>61</v>
       </c>
       <c r="B158" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
@@ -2496,7 +2496,7 @@
         <v>146</v>
       </c>
       <c r="B159" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
@@ -2504,7 +2504,7 @@
         <v>127</v>
       </c>
       <c r="B160" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
@@ -2520,7 +2520,7 @@
         <v>182</v>
       </c>
       <c r="B162" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
@@ -2576,7 +2576,7 @@
         <v>108</v>
       </c>
       <c r="B169" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
@@ -2592,7 +2592,7 @@
         <v>220</v>
       </c>
       <c r="B171" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -2600,7 +2600,7 @@
         <v>233</v>
       </c>
       <c r="B172" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
@@ -2640,7 +2640,7 @@
         <v>148</v>
       </c>
       <c r="B177" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -2648,7 +2648,7 @@
         <v>235</v>
       </c>
       <c r="B178" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
@@ -2672,7 +2672,7 @@
         <v>66</v>
       </c>
       <c r="B181" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
@@ -2704,7 +2704,7 @@
         <v>176</v>
       </c>
       <c r="B185" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
@@ -2728,7 +2728,7 @@
         <v>193</v>
       </c>
       <c r="B188" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
@@ -2744,7 +2744,7 @@
         <v>68</v>
       </c>
       <c r="B190" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
@@ -2752,7 +2752,7 @@
         <v>120</v>
       </c>
       <c r="B191" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
@@ -2760,7 +2760,7 @@
         <v>123</v>
       </c>
       <c r="B192" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
@@ -2776,7 +2776,7 @@
         <v>211</v>
       </c>
       <c r="B194" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
@@ -2816,7 +2816,7 @@
         <v>150</v>
       </c>
       <c r="B199" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
@@ -2840,7 +2840,7 @@
         <v>173</v>
       </c>
       <c r="B202" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
@@ -2848,7 +2848,7 @@
         <v>194</v>
       </c>
       <c r="B203" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -2864,7 +2864,7 @@
         <v>73</v>
       </c>
       <c r="B205" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
@@ -2912,7 +2912,7 @@
         <v>76</v>
       </c>
       <c r="B211" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
@@ -2968,7 +2968,7 @@
         <v>102</v>
       </c>
       <c r="B218" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
@@ -3016,7 +3016,7 @@
         <v>275</v>
       </c>
       <c r="B224" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
@@ -3032,7 +3032,7 @@
         <v>128</v>
       </c>
       <c r="B226" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
@@ -3048,7 +3048,7 @@
         <v>83</v>
       </c>
       <c r="B228" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
@@ -3080,7 +3080,7 @@
         <v>185</v>
       </c>
       <c r="B232" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
@@ -3096,7 +3096,7 @@
         <v>224</v>
       </c>
       <c r="B234" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
@@ -3104,7 +3104,7 @@
         <v>85</v>
       </c>
       <c r="B235" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
@@ -3112,7 +3112,7 @@
         <v>203</v>
       </c>
       <c r="B236" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
@@ -3120,7 +3120,7 @@
         <v>195</v>
       </c>
       <c r="B237" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
@@ -3136,7 +3136,7 @@
         <v>86</v>
       </c>
       <c r="B239" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
@@ -3152,7 +3152,7 @@
         <v>88</v>
       </c>
       <c r="B241" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
@@ -3176,7 +3176,7 @@
         <v>225</v>
       </c>
       <c r="B244" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
@@ -3216,7 +3216,7 @@
         <v>170</v>
       </c>
       <c r="B249" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
@@ -3232,7 +3232,7 @@
         <v>196</v>
       </c>
       <c r="B251" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
@@ -3240,7 +3240,7 @@
         <v>212</v>
       </c>
       <c r="B252" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
@@ -3272,7 +3272,7 @@
         <v>158</v>
       </c>
       <c r="B256" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
@@ -3296,7 +3296,7 @@
         <v>129</v>
       </c>
       <c r="B259" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
@@ -3320,7 +3320,7 @@
         <v>159</v>
       </c>
       <c r="B262" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
@@ -3344,7 +3344,7 @@
         <v>197</v>
       </c>
       <c r="B265" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
@@ -3352,7 +3352,7 @@
         <v>187</v>
       </c>
       <c r="B266" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
@@ -3376,7 +3376,7 @@
         <v>97</v>
       </c>
       <c r="B269" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
@@ -3392,7 +3392,7 @@
         <v>99</v>
       </c>
       <c r="B271" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated status for GGD Delfland
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B0C2FB-089A-442C-B831-DC7277FB7A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D9259C-FA47-446C-A36C-8D5212F6596E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7430" yWindow="1220" windowWidth="27020" windowHeight="19280" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="26310" windowHeight="17520" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1221,13 +1221,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>204</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>162</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>166</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>237</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>130</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>174</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>131</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>189</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>238</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>132</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>198</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>105</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>167</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>177</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>178</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>134</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>118</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>269</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>171</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>172</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>110</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>215</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>199</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>179</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>135</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>216</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>239</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>111</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>240</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>217</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>241</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>27</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>242</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>243</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>136</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>218</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>163</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>244</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>270</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>271</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>29</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>30</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>245</v>
       </c>
@@ -1827,15 +1827,15 @@
         <v>214</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>31</v>
       </c>
       <c r="B76" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>122</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>32</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>246</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>247</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>33</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>272</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>266</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>248</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>137</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>34</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>138</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>205</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>35</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>190</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>168</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>206</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>228</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>36</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>267</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>37</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>139</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>229</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>249</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>200</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>126</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>38</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>230</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>39</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>191</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>40</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>192</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>140</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>41</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>207</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>169</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>42</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>250</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>43</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>180</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>231</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>268</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>101</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>141</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>208</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>142</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>44</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>45</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>164</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>251</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>232</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>46</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>47</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>181</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>273</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>112</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>48</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>49</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>113</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>219</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>50</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>51</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>52</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>53</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>252</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>263</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>253</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>54</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>201</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>143</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>202</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>144</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>55</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>56</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>57</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>145</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>274</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>58</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>106</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>107</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>59</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>60</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>61</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>146</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>127</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>62</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>182</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>63</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>114</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>115</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>254</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>147</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>209</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>108</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>119</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>220</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>233</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>210</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>183</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>64</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>234</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>148</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>235</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>65</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>255</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>66</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>221</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>222</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>256</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>176</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>67</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>236</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>193</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>116</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>68</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>120</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>123</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>69</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>211</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>70</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>103</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>71</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>149</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>150</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>151</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>264</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>173</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>194</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>72</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>73</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>175</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>175</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>74</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>152</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>75</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>76</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>153</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>77</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>184</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>257</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>78</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>79</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>102</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>80</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>81</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>82</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>223</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>258</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>275</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>161</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>128</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>154</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>83</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>84</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>259</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>155</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>185</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>186</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>224</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>85</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>203</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>195</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>109</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>86</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>87</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>88</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>260</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>89</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>225</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>90</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>91</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>92</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>226</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>170</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>156</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>196</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>212</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>117</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>93</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>157</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>158</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>94</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>261</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>129</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>265</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>165</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>159</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>95</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>197</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>187</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>96</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>227</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>97</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>98</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>99</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>100</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>188</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>160</v>
       </c>

</xml_diff>

<commit_message>
Updated data for care; v57
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425E30FD-AFB5-46FA-941C-9E665156EE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0940A1CA-02DC-4880-8FE4-7C01FA22CC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10070" yWindow="2180" windowWidth="26510" windowHeight="18330" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="19965" yWindow="2115" windowWidth="23205" windowHeight="18645" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1251,13 +1251,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>203</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>161</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>165</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>236</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>129</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>173</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>188</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>237</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>274</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>197</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>123</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>166</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>176</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>132</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>177</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>133</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>120</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>117</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>267</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>170</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>171</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>214</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>198</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>178</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>134</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>215</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>238</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>21</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>110</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>239</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>216</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>23</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>24</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>25</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>240</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>241</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>242</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>27</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>135</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>217</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>275</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>162</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>243</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>268</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>269</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>28</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>29</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>244</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>30</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>121</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>31</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>245</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>246</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>32</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>270</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>264</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>247</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>276</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>136</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>33</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>137</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>204</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>34</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>189</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>167</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>205</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>227</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>277</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>35</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>265</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>36</v>
       </c>
@@ -2049,15 +2049,15 @@
         <v>212</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>138</v>
       </c>
       <c r="B100" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>228</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>248</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>199</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>125</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>37</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>229</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>38</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>190</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>39</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>191</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>139</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>40</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>206</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>168</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>41</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>249</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>42</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>179</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>230</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>266</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>100</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>140</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>207</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>141</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>43</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>44</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>163</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>250</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>231</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>45</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>46</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>180</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>271</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>111</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>47</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>48</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>112</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>218</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>49</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>50</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>51</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>52</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>251</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>261</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>252</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>53</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>200</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>142</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>201</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>143</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>54</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>55</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>56</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>144</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>272</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>57</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>105</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>106</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>58</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>59</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>60</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>145</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>126</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>61</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>181</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>62</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>278</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>113</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>114</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>253</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>146</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>208</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>107</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>118</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>219</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>279</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>232</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>209</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>182</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>63</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>233</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>147</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>234</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>64</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>254</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>65</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>220</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>221</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>255</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>175</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>66</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>235</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>115</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>67</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>119</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>280</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>122</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>68</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>210</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>69</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>102</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>70</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>148</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>149</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>150</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>262</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>172</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>193</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>71</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>72</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>174</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>174</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>73</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>151</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>74</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>75</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>152</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>76</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>183</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>256</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>77</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>78</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>101</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>79</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>80</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>81</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>222</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>257</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>273</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>160</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>127</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>153</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>82</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>83</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>281</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>282</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>154</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>184</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>185</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>223</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>84</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>202</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>194</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>108</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>85</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>86</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>87</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>258</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>283</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>88</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>224</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>284</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>89</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>90</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>91</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>225</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>169</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>155</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>195</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>211</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>116</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>92</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>156</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>157</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>93</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>259</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>128</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>263</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>164</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>158</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>260</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>94</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>196</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>186</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>285</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>95</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>226</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>96</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>97</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>98</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>99</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>187</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>159</v>
       </c>

</xml_diff>

<commit_message>
Updated data for care, v57 (added Viattence)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0940A1CA-02DC-4880-8FE4-7C01FA22CC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46D97A9-BB72-41FD-91CF-C8DB04D936E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19965" yWindow="2115" windowWidth="23205" windowHeight="18645" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="2100" yWindow="4215" windowWidth="22935" windowHeight="15285" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="287">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -887,13 +887,16 @@
   </si>
   <si>
     <t>Zorggroep Zaanstreek (Stichting) (was pennemes en mennistenerf)</t>
+  </si>
+  <si>
+    <t>Viattence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -908,6 +911,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -930,9 +939,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1247,9 +1257,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B284"/>
+  <dimension ref="A1:B285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="A223" sqref="A223"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3025,7 +3037,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>77</v>
       </c>
@@ -3033,33 +3045,33 @@
         <v>213</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
+    <row r="223" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B223" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>78</v>
       </c>
-      <c r="B223" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>101</v>
-      </c>
       <c r="B224" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B225" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B226" t="s">
         <v>213</v>
@@ -3067,23 +3079,23 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B227" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>222</v>
+        <v>81</v>
       </c>
       <c r="B228" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
       <c r="B229" t="s">
         <v>213</v>
@@ -3091,55 +3103,55 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="B230" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>160</v>
+        <v>273</v>
       </c>
       <c r="B231" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="B232" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="B233" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
       <c r="B234" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B235" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>281</v>
+        <v>83</v>
       </c>
       <c r="B236" t="s">
         <v>213</v>
@@ -3147,31 +3159,31 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B237" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>154</v>
+        <v>282</v>
       </c>
       <c r="B238" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="B239" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B240" t="s">
         <v>212</v>
@@ -3179,7 +3191,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>223</v>
+        <v>185</v>
       </c>
       <c r="B241" t="s">
         <v>212</v>
@@ -3187,7 +3199,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>84</v>
+        <v>223</v>
       </c>
       <c r="B242" t="s">
         <v>212</v>
@@ -3195,7 +3207,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>202</v>
+        <v>84</v>
       </c>
       <c r="B243" t="s">
         <v>212</v>
@@ -3203,7 +3215,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B244" t="s">
         <v>212</v>
@@ -3211,15 +3223,15 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="B245" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="B246" t="s">
         <v>213</v>
@@ -3227,15 +3239,15 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B247" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B248" t="s">
         <v>212</v>
@@ -3243,15 +3255,15 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>258</v>
+        <v>87</v>
       </c>
       <c r="B249" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
       <c r="B250" t="s">
         <v>213</v>
@@ -3259,15 +3271,15 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>88</v>
+        <v>283</v>
       </c>
       <c r="B251" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>224</v>
+        <v>88</v>
       </c>
       <c r="B252" t="s">
         <v>212</v>
@@ -3275,7 +3287,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>284</v>
+        <v>224</v>
       </c>
       <c r="B253" t="s">
         <v>212</v>
@@ -3283,15 +3295,15 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>89</v>
+        <v>284</v>
       </c>
       <c r="B254" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B255" t="s">
         <v>213</v>
@@ -3299,47 +3311,47 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B256" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>225</v>
+        <v>91</v>
       </c>
       <c r="B257" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>169</v>
+        <v>225</v>
       </c>
       <c r="B258" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="B259" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
       <c r="B260" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="B261" t="s">
         <v>212</v>
@@ -3347,7 +3359,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>116</v>
+        <v>211</v>
       </c>
       <c r="B262" t="s">
         <v>212</v>
@@ -3355,15 +3367,15 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="B263" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="B264" t="s">
         <v>213</v>
@@ -3371,23 +3383,23 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B265" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>93</v>
+        <v>157</v>
       </c>
       <c r="B266" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>259</v>
+        <v>93</v>
       </c>
       <c r="B267" t="s">
         <v>213</v>
@@ -3395,23 +3407,23 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="B268" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>263</v>
+        <v>128</v>
       </c>
       <c r="B269" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>164</v>
+        <v>263</v>
       </c>
       <c r="B270" t="s">
         <v>213</v>
@@ -3419,7 +3431,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B271" t="s">
         <v>213</v>
@@ -3427,23 +3439,23 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>260</v>
+        <v>158</v>
       </c>
       <c r="B272" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>94</v>
+        <v>260</v>
       </c>
       <c r="B273" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>196</v>
+        <v>94</v>
       </c>
       <c r="B274" t="s">
         <v>213</v>
@@ -3451,15 +3463,15 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B275" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>285</v>
+        <v>186</v>
       </c>
       <c r="B276" t="s">
         <v>212</v>
@@ -3467,23 +3479,23 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>95</v>
+        <v>285</v>
       </c>
       <c r="B277" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>226</v>
+        <v>95</v>
       </c>
       <c r="B278" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>96</v>
+        <v>226</v>
       </c>
       <c r="B279" t="s">
         <v>212</v>
@@ -3491,31 +3503,31 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B280" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B281" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B282" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>187</v>
+        <v>99</v>
       </c>
       <c r="B283" t="s">
         <v>213</v>
@@ -3523,9 +3535,17 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
+        <v>187</v>
+      </c>
+      <c r="B284" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
         <v>159</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B285" t="s">
         <v>213</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated data for care; v59
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46D97A9-BB72-41FD-91CF-C8DB04D936E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210FDF76-E046-4708-BCD2-58F159B37B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="4215" windowWidth="22935" windowHeight="15285" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="4200" yWindow="790" windowWidth="27460" windowHeight="19920" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="290">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -454,9 +454,6 @@
     <t>Lelie Zorggroep (Stichting)</t>
   </si>
   <si>
-    <t>Lentis incl. Dignis</t>
-  </si>
-  <si>
     <t>Opbouw (Stichting) incl. Prinsenstichting</t>
   </si>
   <si>
@@ -589,9 +586,6 @@
     <t>Woon- en Zorgcentrum Humanitas (Stichting)</t>
   </si>
   <si>
-    <t>Zorggroep Triade B.V. (incl. Vitree)</t>
-  </si>
-  <si>
     <t>Zuyderland Zorg (Stichting)</t>
   </si>
   <si>
@@ -886,10 +880,25 @@
     <t>Zorg- en Wooncentrum De Haven (Stichting)</t>
   </si>
   <si>
-    <t>Zorggroep Zaanstreek (Stichting) (was pennemes en mennistenerf)</t>
-  </si>
-  <si>
     <t>Viattence</t>
+  </si>
+  <si>
+    <t>Ananz wonen-welzijn-zorg (sint anna zorggroep)</t>
+  </si>
+  <si>
+    <t>De Lichtenvoorde (Sius) (Stichting)</t>
+  </si>
+  <si>
+    <t>Lentis</t>
+  </si>
+  <si>
+    <t>Lunet (Stichting)</t>
+  </si>
+  <si>
+    <t>Zinzia Zorggroep (Stichting)</t>
+  </si>
+  <si>
+    <t>Stichting Triade Vitree</t>
   </si>
 </sst>
 </file>
@@ -1257,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B285"/>
+  <dimension ref="A1:B288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="A223" sqref="A223"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,7 +1291,7 @@
         <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1290,7 +1299,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1298,31 +1307,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1330,7 +1339,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1338,7 +1347,7 @@
         <v>124</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1346,7 +1355,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1354,15 +1363,15 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1370,2183 +1379,2207 @@
         <v>129</v>
       </c>
       <c r="B13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>284</v>
       </c>
       <c r="B15" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>186</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>237</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>235</v>
       </c>
       <c r="B23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>274</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>272</v>
       </c>
       <c r="B26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>197</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="B30" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
       <c r="B31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>165</v>
       </c>
       <c r="B32" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>176</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="B34" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>177</v>
+        <v>132</v>
       </c>
       <c r="B37" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>133</v>
+        <v>176</v>
       </c>
       <c r="B38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>133</v>
       </c>
       <c r="B39" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>120</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="B43" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>267</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>170</v>
+        <v>265</v>
       </c>
       <c r="B45" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>214</v>
+        <v>109</v>
       </c>
       <c r="B48" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="B49" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="B50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>134</v>
+        <v>285</v>
       </c>
       <c r="B51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="B52" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>238</v>
+        <v>134</v>
       </c>
       <c r="B53" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>213</v>
       </c>
       <c r="B54" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>236</v>
       </c>
       <c r="B55" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>239</v>
+        <v>21</v>
       </c>
       <c r="B56" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="B57" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>216</v>
+        <v>237</v>
       </c>
       <c r="B58" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>24</v>
+        <v>214</v>
       </c>
       <c r="B60" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B61" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>240</v>
+        <v>24</v>
       </c>
       <c r="B62" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B64" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>242</v>
+        <v>26</v>
       </c>
       <c r="B65" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>27</v>
+        <v>239</v>
       </c>
       <c r="B66" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>135</v>
+        <v>240</v>
       </c>
       <c r="B67" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>217</v>
+        <v>27</v>
       </c>
       <c r="B68" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>275</v>
+        <v>135</v>
       </c>
       <c r="B69" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>162</v>
+        <v>215</v>
       </c>
       <c r="B70" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
       <c r="B71" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>268</v>
-      </c>
-      <c r="B72" t="s">
-        <v>212</v>
+        <v>161</v>
+      </c>
+      <c r="B72" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="B73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>266</v>
       </c>
       <c r="B74" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>29</v>
+        <v>267</v>
       </c>
       <c r="B75" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>244</v>
+        <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>242</v>
       </c>
       <c r="B78" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B79" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>245</v>
+        <v>121</v>
       </c>
       <c r="B80" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>246</v>
+        <v>31</v>
       </c>
       <c r="B81" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>32</v>
+        <v>243</v>
       </c>
       <c r="B82" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="B83" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>264</v>
+        <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>247</v>
+        <v>268</v>
       </c>
       <c r="B85" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="B86" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>136</v>
+        <v>245</v>
       </c>
       <c r="B87" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>33</v>
+        <v>274</v>
       </c>
       <c r="B88" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B89" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>204</v>
+        <v>33</v>
       </c>
       <c r="B90" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>34</v>
+        <v>137</v>
       </c>
       <c r="B91" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="B92" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>167</v>
+        <v>34</v>
       </c>
       <c r="B93" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="B94" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>227</v>
+        <v>166</v>
       </c>
       <c r="B95" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>277</v>
+        <v>203</v>
       </c>
       <c r="B96" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>35</v>
+        <v>225</v>
       </c>
       <c r="B97" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="B98" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B99" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="B100" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>228</v>
+        <v>36</v>
       </c>
       <c r="B101" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>248</v>
+        <v>138</v>
       </c>
       <c r="B102" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="B103" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>125</v>
+        <v>246</v>
       </c>
       <c r="B104" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>37</v>
+        <v>197</v>
       </c>
       <c r="B105" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>229</v>
+        <v>125</v>
       </c>
       <c r="B106" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B107" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>190</v>
+        <v>227</v>
       </c>
       <c r="B108" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B109" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B110" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="B111" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>40</v>
+        <v>189</v>
       </c>
       <c r="B112" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>206</v>
+        <v>139</v>
       </c>
       <c r="B113" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="B114" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>41</v>
+        <v>204</v>
       </c>
       <c r="B115" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>249</v>
+        <v>167</v>
       </c>
       <c r="B116" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B117" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>179</v>
+        <v>247</v>
       </c>
       <c r="B118" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>230</v>
+        <v>42</v>
       </c>
       <c r="B119" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>266</v>
+        <v>178</v>
       </c>
       <c r="B120" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>100</v>
+        <v>228</v>
       </c>
       <c r="B121" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>140</v>
+        <v>264</v>
       </c>
       <c r="B122" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>207</v>
+        <v>100</v>
       </c>
       <c r="B123" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B124" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>43</v>
+        <v>205</v>
       </c>
       <c r="B125" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>44</v>
+        <v>286</v>
       </c>
       <c r="B126" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="B127" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>250</v>
+        <v>44</v>
       </c>
       <c r="B128" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>231</v>
+        <v>162</v>
       </c>
       <c r="B129" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>45</v>
+        <v>248</v>
       </c>
       <c r="B130" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>46</v>
+        <v>229</v>
       </c>
       <c r="B131" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>180</v>
+        <v>287</v>
       </c>
       <c r="B132" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>271</v>
+        <v>45</v>
       </c>
       <c r="B133" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>111</v>
+        <v>46</v>
       </c>
       <c r="B134" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="B135" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>48</v>
+        <v>269</v>
       </c>
       <c r="B136" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B137" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>218</v>
+        <v>47</v>
       </c>
       <c r="B138" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B139" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="B140" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>51</v>
+        <v>216</v>
       </c>
       <c r="B141" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B142" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>251</v>
+        <v>50</v>
       </c>
       <c r="B143" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>261</v>
+        <v>51</v>
       </c>
       <c r="B144" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>252</v>
+        <v>52</v>
       </c>
       <c r="B145" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>53</v>
+        <v>249</v>
       </c>
       <c r="B146" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>200</v>
+        <v>259</v>
       </c>
       <c r="B147" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>142</v>
+        <v>250</v>
       </c>
       <c r="B148" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>201</v>
+        <v>53</v>
       </c>
       <c r="B149" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>143</v>
+        <v>198</v>
       </c>
       <c r="B150" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>54</v>
+        <v>141</v>
       </c>
       <c r="B151" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>55</v>
+        <v>199</v>
       </c>
       <c r="B152" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>56</v>
+        <v>142</v>
       </c>
       <c r="B153" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="B154" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>272</v>
+        <v>55</v>
       </c>
       <c r="B155" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B156" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="B157" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>106</v>
+        <v>270</v>
       </c>
       <c r="B158" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B159" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="B160" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="B161" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>145</v>
+        <v>58</v>
       </c>
       <c r="B162" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>126</v>
+        <v>59</v>
       </c>
       <c r="B163" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B164" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="B165" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="B166" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>278</v>
+        <v>61</v>
       </c>
       <c r="B167" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>113</v>
+        <v>180</v>
       </c>
       <c r="B168" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="B169" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="B170" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="B171" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>208</v>
+        <v>114</v>
       </c>
       <c r="B172" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>107</v>
+        <v>251</v>
       </c>
       <c r="B173" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="B174" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="B175" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>279</v>
+        <v>107</v>
       </c>
       <c r="B176" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>232</v>
+        <v>118</v>
       </c>
       <c r="B177" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B178" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>182</v>
+        <v>277</v>
       </c>
       <c r="B179" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>63</v>
+        <v>230</v>
       </c>
       <c r="B180" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>233</v>
+        <v>207</v>
       </c>
       <c r="B181" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>234</v>
+        <v>63</v>
       </c>
       <c r="B183" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>64</v>
+        <v>231</v>
       </c>
       <c r="B184" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>254</v>
+        <v>146</v>
       </c>
       <c r="B185" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>65</v>
+        <v>232</v>
       </c>
       <c r="B186" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>220</v>
+        <v>64</v>
       </c>
       <c r="B187" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>221</v>
+        <v>252</v>
       </c>
       <c r="B188" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>255</v>
+        <v>65</v>
       </c>
       <c r="B189" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>175</v>
+        <v>218</v>
       </c>
       <c r="B190" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>66</v>
+        <v>219</v>
       </c>
       <c r="B191" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="B192" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B193" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="B194" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>67</v>
+        <v>233</v>
       </c>
       <c r="B195" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>119</v>
+        <v>190</v>
       </c>
       <c r="B196" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>280</v>
+        <v>115</v>
       </c>
       <c r="B197" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>122</v>
+        <v>67</v>
       </c>
       <c r="B198" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
       <c r="B199" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>210</v>
+        <v>278</v>
       </c>
       <c r="B200" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
       <c r="B201" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="B202" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>70</v>
+        <v>208</v>
       </c>
       <c r="B203" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
       <c r="B204" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="B205" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>150</v>
+        <v>70</v>
       </c>
       <c r="B206" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>262</v>
+        <v>147</v>
       </c>
       <c r="B207" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B208" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>193</v>
+        <v>149</v>
       </c>
       <c r="B209" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>71</v>
+        <v>260</v>
       </c>
       <c r="B210" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>72</v>
+        <v>171</v>
       </c>
       <c r="B211" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="B212" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>174</v>
+        <v>71</v>
       </c>
       <c r="B213" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B214" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="B215" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>74</v>
+        <v>173</v>
       </c>
       <c r="B216" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B217" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B218" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B219" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>183</v>
+        <v>75</v>
       </c>
       <c r="B220" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>256</v>
+        <v>151</v>
       </c>
       <c r="B221" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B222" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="223" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>286</v>
+        <v>182</v>
       </c>
       <c r="B223" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>78</v>
+        <v>254</v>
       </c>
       <c r="B224" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="B225" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>79</v>
+        <v>283</v>
       </c>
       <c r="B226" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B227" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="B228" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>222</v>
+        <v>79</v>
       </c>
       <c r="B229" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>257</v>
+        <v>80</v>
       </c>
       <c r="B230" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>273</v>
+        <v>81</v>
       </c>
       <c r="B231" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>160</v>
+        <v>220</v>
       </c>
       <c r="B232" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="B233" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>153</v>
+        <v>271</v>
       </c>
       <c r="B234" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
       <c r="B235" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
       <c r="B236" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>281</v>
+        <v>152</v>
       </c>
       <c r="B237" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>282</v>
+        <v>82</v>
       </c>
       <c r="B238" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="B239" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>184</v>
+        <v>279</v>
       </c>
       <c r="B240" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>185</v>
+        <v>280</v>
       </c>
       <c r="B241" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>223</v>
+        <v>153</v>
       </c>
       <c r="B242" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>84</v>
+        <v>183</v>
       </c>
       <c r="B243" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="B244" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="B245" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="B246" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>85</v>
+        <v>200</v>
       </c>
       <c r="B247" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>86</v>
+        <v>192</v>
       </c>
       <c r="B248" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="B249" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>258</v>
+        <v>85</v>
       </c>
       <c r="B250" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>283</v>
+        <v>86</v>
       </c>
       <c r="B251" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B252" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>224</v>
+        <v>256</v>
       </c>
       <c r="B253" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B254" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>89</v>
+        <v>281</v>
       </c>
       <c r="B255" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B256" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>91</v>
+        <v>222</v>
       </c>
       <c r="B257" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>225</v>
+        <v>282</v>
       </c>
       <c r="B258" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>169</v>
+        <v>89</v>
       </c>
       <c r="B259" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>155</v>
+        <v>90</v>
       </c>
       <c r="B260" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>195</v>
+        <v>91</v>
       </c>
       <c r="B261" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="B262" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>116</v>
+        <v>168</v>
       </c>
       <c r="B263" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="B264" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>156</v>
+        <v>193</v>
       </c>
       <c r="B265" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>157</v>
+        <v>209</v>
       </c>
       <c r="B266" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="B267" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>259</v>
+        <v>92</v>
       </c>
       <c r="B268" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="B269" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>263</v>
+        <v>156</v>
       </c>
       <c r="B270" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>164</v>
+        <v>93</v>
       </c>
       <c r="B271" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>158</v>
+        <v>257</v>
       </c>
       <c r="B272" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>260</v>
+        <v>128</v>
       </c>
       <c r="B273" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>94</v>
+        <v>261</v>
       </c>
       <c r="B274" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>196</v>
+        <v>163</v>
       </c>
       <c r="B275" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="B276" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>285</v>
+        <v>258</v>
       </c>
       <c r="B277" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B278" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="B279" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>96</v>
+        <v>289</v>
       </c>
       <c r="B280" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B281" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>98</v>
+        <v>224</v>
       </c>
       <c r="B282" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B283" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="B284" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>159</v>
+        <v>98</v>
       </c>
       <c r="B285" t="s">
-        <v>213</v>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>99</v>
+      </c>
+      <c r="B286" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>185</v>
+      </c>
+      <c r="B287" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>158</v>
+      </c>
+      <c r="B288" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data for care (v62b)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1392AE-AA43-4239-A982-872D8FAE45D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD3FD1F-C5D1-42D3-B406-9293EDB9EC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16750" yWindow="5090" windowWidth="19980" windowHeight="15370" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="4200" yWindow="5280" windowWidth="26880" windowHeight="15390" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1268,17 +1268,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
   <dimension ref="A1:B287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
-      <selection activeCell="A288" sqref="A288"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1286,7 +1284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -1294,7 +1292,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1302,7 +1300,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1310,7 +1308,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>201</v>
       </c>
@@ -1318,7 +1316,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>160</v>
       </c>
@@ -1326,7 +1324,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -1334,7 +1332,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1342,7 +1340,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -1350,7 +1348,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1358,7 +1356,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1366,7 +1364,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>234</v>
       </c>
@@ -1374,7 +1372,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>129</v>
       </c>
@@ -1382,7 +1380,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>172</v>
       </c>
@@ -1390,7 +1388,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>279</v>
       </c>
@@ -1398,7 +1396,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1406,7 +1404,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>130</v>
       </c>
@@ -1414,7 +1412,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>186</v>
       </c>
@@ -1422,7 +1420,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1430,7 +1428,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1438,7 +1436,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1446,7 +1444,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1454,7 +1452,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>235</v>
       </c>
@@ -1462,7 +1460,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1470,7 +1468,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1478,7 +1476,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>267</v>
       </c>
@@ -1486,7 +1484,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>131</v>
       </c>
@@ -1494,7 +1492,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>195</v>
       </c>
@@ -1502,7 +1500,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1510,7 +1508,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -1518,7 +1516,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -1526,7 +1524,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>165</v>
       </c>
@@ -1534,7 +1532,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>274</v>
       </c>
@@ -1542,7 +1540,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -1550,7 +1548,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -1558,7 +1556,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1566,7 +1564,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1574,7 +1572,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>132</v>
       </c>
@@ -1582,7 +1580,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>176</v>
       </c>
@@ -1590,7 +1588,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>133</v>
       </c>
@@ -1598,7 +1596,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -1606,7 +1604,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -1614,7 +1612,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>120</v>
       </c>
@@ -1622,7 +1620,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>117</v>
       </c>
@@ -1630,7 +1628,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -1638,7 +1636,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>260</v>
       </c>
@@ -1646,7 +1644,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -1654,7 +1652,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>170</v>
       </c>
@@ -1662,7 +1660,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>109</v>
       </c>
@@ -1670,7 +1668,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>212</v>
       </c>
@@ -1678,7 +1676,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>196</v>
       </c>
@@ -1686,7 +1684,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>280</v>
       </c>
@@ -1694,7 +1692,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>284</v>
       </c>
@@ -1702,7 +1700,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>177</v>
       </c>
@@ -1710,7 +1708,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>134</v>
       </c>
@@ -1718,7 +1716,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>213</v>
       </c>
@@ -1726,7 +1724,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>236</v>
       </c>
@@ -1734,7 +1732,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>21</v>
       </c>
@@ -1742,7 +1740,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -1750,7 +1748,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>237</v>
       </c>
@@ -1758,15 +1756,15 @@
         <v>211</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>285</v>
       </c>
       <c r="B61" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>22</v>
       </c>
@@ -1774,7 +1772,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>214</v>
       </c>
@@ -1782,7 +1780,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>23</v>
       </c>
@@ -1790,7 +1788,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -1798,7 +1796,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -1806,7 +1804,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>238</v>
       </c>
@@ -1814,7 +1812,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>286</v>
       </c>
@@ -1822,7 +1820,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -1830,7 +1828,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>239</v>
       </c>
@@ -1838,7 +1836,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>27</v>
       </c>
@@ -1846,7 +1844,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>287</v>
       </c>
@@ -1854,7 +1852,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>135</v>
       </c>
@@ -1862,7 +1860,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>215</v>
       </c>
@@ -1870,7 +1868,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>268</v>
       </c>
@@ -1878,7 +1876,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>161</v>
       </c>
@@ -1886,7 +1884,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>261</v>
       </c>
@@ -1894,7 +1892,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>262</v>
       </c>
@@ -1902,7 +1900,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>28</v>
       </c>
@@ -1910,7 +1908,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>29</v>
       </c>
@@ -1918,7 +1916,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>240</v>
       </c>
@@ -1926,7 +1924,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>30</v>
       </c>
@@ -1934,7 +1932,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>121</v>
       </c>
@@ -1942,7 +1940,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>31</v>
       </c>
@@ -1950,7 +1948,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>241</v>
       </c>
@@ -1958,7 +1956,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>242</v>
       </c>
@@ -1966,7 +1964,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>32</v>
       </c>
@@ -1974,7 +1972,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>263</v>
       </c>
@@ -1982,7 +1980,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>257</v>
       </c>
@@ -1990,7 +1988,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>243</v>
       </c>
@@ -1998,7 +1996,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>269</v>
       </c>
@@ -2006,7 +2004,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>136</v>
       </c>
@@ -2014,7 +2012,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>33</v>
       </c>
@@ -2022,7 +2020,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>137</v>
       </c>
@@ -2030,7 +2028,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>202</v>
       </c>
@@ -2038,7 +2036,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>34</v>
       </c>
@@ -2046,7 +2044,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>187</v>
       </c>
@@ -2054,7 +2052,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>166</v>
       </c>
@@ -2062,7 +2060,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>203</v>
       </c>
@@ -2070,7 +2068,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>225</v>
       </c>
@@ -2078,7 +2076,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>270</v>
       </c>
@@ -2086,7 +2084,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>35</v>
       </c>
@@ -2094,7 +2092,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>288</v>
       </c>
@@ -2102,7 +2100,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>258</v>
       </c>
@@ -2110,7 +2108,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>36</v>
       </c>
@@ -2118,7 +2116,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>138</v>
       </c>
@@ -2126,7 +2124,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>226</v>
       </c>
@@ -2134,7 +2132,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>197</v>
       </c>
@@ -2142,7 +2140,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>125</v>
       </c>
@@ -2150,7 +2148,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>37</v>
       </c>
@@ -2158,7 +2156,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>227</v>
       </c>
@@ -2166,7 +2164,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>38</v>
       </c>
@@ -2174,7 +2172,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>188</v>
       </c>
@@ -2182,7 +2180,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>39</v>
       </c>
@@ -2190,7 +2188,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>189</v>
       </c>
@@ -2198,7 +2196,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>139</v>
       </c>
@@ -2206,7 +2204,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>40</v>
       </c>
@@ -2214,7 +2212,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>204</v>
       </c>
@@ -2222,7 +2220,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>167</v>
       </c>
@@ -2230,7 +2228,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>41</v>
       </c>
@@ -2238,7 +2236,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -2246,7 +2244,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>42</v>
       </c>
@@ -2254,7 +2252,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>178</v>
       </c>
@@ -2262,7 +2260,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>228</v>
       </c>
@@ -2270,7 +2268,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>259</v>
       </c>
@@ -2278,7 +2276,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>100</v>
       </c>
@@ -2286,7 +2284,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>140</v>
       </c>
@@ -2294,7 +2292,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>205</v>
       </c>
@@ -2302,7 +2300,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>43</v>
       </c>
@@ -2310,7 +2308,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>44</v>
       </c>
@@ -2318,7 +2316,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>162</v>
       </c>
@@ -2326,7 +2324,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>245</v>
       </c>
@@ -2334,7 +2332,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>229</v>
       </c>
@@ -2342,7 +2340,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>281</v>
       </c>
@@ -2350,7 +2348,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>45</v>
       </c>
@@ -2358,7 +2356,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>46</v>
       </c>
@@ -2366,7 +2364,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>179</v>
       </c>
@@ -2374,7 +2372,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>264</v>
       </c>
@@ -2382,7 +2380,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>111</v>
       </c>
@@ -2390,7 +2388,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>47</v>
       </c>
@@ -2398,7 +2396,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>48</v>
       </c>
@@ -2406,7 +2404,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>112</v>
       </c>
@@ -2414,7 +2412,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>216</v>
       </c>
@@ -2422,7 +2420,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>49</v>
       </c>
@@ -2430,7 +2428,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>50</v>
       </c>
@@ -2438,7 +2436,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>51</v>
       </c>
@@ -2446,7 +2444,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>52</v>
       </c>
@@ -2454,7 +2452,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>246</v>
       </c>
@@ -2462,7 +2460,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>254</v>
       </c>
@@ -2470,7 +2468,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>247</v>
       </c>
@@ -2478,7 +2476,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>53</v>
       </c>
@@ -2486,7 +2484,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>198</v>
       </c>
@@ -2494,7 +2492,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>141</v>
       </c>
@@ -2502,7 +2500,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>289</v>
       </c>
@@ -2510,7 +2508,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>199</v>
       </c>
@@ -2518,7 +2516,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>142</v>
       </c>
@@ -2526,7 +2524,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>54</v>
       </c>
@@ -2534,7 +2532,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>55</v>
       </c>
@@ -2542,7 +2540,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>56</v>
       </c>
@@ -2550,7 +2548,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>143</v>
       </c>
@@ -2558,7 +2556,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>265</v>
       </c>
@@ -2566,7 +2564,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>57</v>
       </c>
@@ -2574,7 +2572,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>105</v>
       </c>
@@ -2582,7 +2580,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>106</v>
       </c>
@@ -2590,7 +2588,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>58</v>
       </c>
@@ -2598,7 +2596,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>59</v>
       </c>
@@ -2606,7 +2604,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>60</v>
       </c>
@@ -2614,7 +2612,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>144</v>
       </c>
@@ -2622,7 +2620,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>126</v>
       </c>
@@ -2630,7 +2628,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>61</v>
       </c>
@@ -2638,7 +2636,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>180</v>
       </c>
@@ -2646,7 +2644,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>62</v>
       </c>
@@ -2654,7 +2652,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>271</v>
       </c>
@@ -2662,7 +2660,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>113</v>
       </c>
@@ -2670,7 +2668,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>114</v>
       </c>
@@ -2678,7 +2676,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>145</v>
       </c>
@@ -2686,7 +2684,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>206</v>
       </c>
@@ -2694,7 +2692,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>107</v>
       </c>
@@ -2702,7 +2700,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>118</v>
       </c>
@@ -2710,7 +2708,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>217</v>
       </c>
@@ -2718,7 +2716,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>272</v>
       </c>
@@ -2726,7 +2724,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>230</v>
       </c>
@@ -2734,7 +2732,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>207</v>
       </c>
@@ -2742,7 +2740,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>181</v>
       </c>
@@ -2750,7 +2748,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>63</v>
       </c>
@@ -2758,7 +2756,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>231</v>
       </c>
@@ -2766,7 +2764,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>146</v>
       </c>
@@ -2774,7 +2772,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>232</v>
       </c>
@@ -2782,7 +2780,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>64</v>
       </c>
@@ -2790,7 +2788,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>248</v>
       </c>
@@ -2798,7 +2796,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>65</v>
       </c>
@@ -2806,7 +2804,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>218</v>
       </c>
@@ -2814,7 +2812,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>219</v>
       </c>
@@ -2822,7 +2820,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>249</v>
       </c>
@@ -2830,7 +2828,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>174</v>
       </c>
@@ -2838,7 +2836,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>66</v>
       </c>
@@ -2846,7 +2844,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>233</v>
       </c>
@@ -2854,7 +2852,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>190</v>
       </c>
@@ -2862,7 +2860,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>115</v>
       </c>
@@ -2870,7 +2868,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>67</v>
       </c>
@@ -2878,7 +2876,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>119</v>
       </c>
@@ -2886,7 +2884,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>273</v>
       </c>
@@ -2894,7 +2892,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>122</v>
       </c>
@@ -2902,7 +2900,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>68</v>
       </c>
@@ -2910,7 +2908,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>208</v>
       </c>
@@ -2918,7 +2916,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>69</v>
       </c>
@@ -2926,7 +2924,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>102</v>
       </c>
@@ -2934,7 +2932,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>70</v>
       </c>
@@ -2942,7 +2940,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>147</v>
       </c>
@@ -2950,7 +2948,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>283</v>
       </c>
@@ -2958,7 +2956,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>148</v>
       </c>
@@ -2966,7 +2964,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>149</v>
       </c>
@@ -2974,7 +2972,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>255</v>
       </c>
@@ -2982,7 +2980,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>171</v>
       </c>
@@ -2990,7 +2988,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>191</v>
       </c>
@@ -2998,7 +2996,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>71</v>
       </c>
@@ -3006,7 +3004,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>72</v>
       </c>
@@ -3014,7 +3012,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>173</v>
       </c>
@@ -3022,7 +3020,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>73</v>
       </c>
@@ -3030,7 +3028,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>150</v>
       </c>
@@ -3038,7 +3036,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>74</v>
       </c>
@@ -3046,7 +3044,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>75</v>
       </c>
@@ -3054,7 +3052,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="223" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>151</v>
       </c>
@@ -3062,7 +3060,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>76</v>
       </c>
@@ -3070,7 +3068,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>182</v>
       </c>
@@ -3078,7 +3076,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>250</v>
       </c>
@@ -3086,7 +3084,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>276</v>
       </c>
@@ -3094,7 +3092,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>77</v>
       </c>
@@ -3102,7 +3100,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>278</v>
       </c>
@@ -3110,7 +3108,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>78</v>
       </c>
@@ -3118,7 +3116,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>101</v>
       </c>
@@ -3126,7 +3124,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>79</v>
       </c>
@@ -3134,7 +3132,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>80</v>
       </c>
@@ -3142,7 +3140,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>81</v>
       </c>
@@ -3150,7 +3148,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>220</v>
       </c>
@@ -3158,7 +3156,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>251</v>
       </c>
@@ -3166,7 +3164,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>266</v>
       </c>
@@ -3174,7 +3172,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>159</v>
       </c>
@@ -3182,7 +3180,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>127</v>
       </c>
@@ -3190,7 +3188,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>152</v>
       </c>
@@ -3198,7 +3196,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>82</v>
       </c>
@@ -3206,7 +3204,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>83</v>
       </c>
@@ -3214,7 +3212,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>275</v>
       </c>
@@ -3222,7 +3220,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>153</v>
       </c>
@@ -3230,7 +3228,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>183</v>
       </c>
@@ -3238,7 +3236,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>184</v>
       </c>
@@ -3246,7 +3244,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>221</v>
       </c>
@@ -3254,7 +3252,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>84</v>
       </c>
@@ -3262,7 +3260,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>200</v>
       </c>
@@ -3270,7 +3268,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>192</v>
       </c>
@@ -3278,7 +3276,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>108</v>
       </c>
@@ -3286,7 +3284,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>85</v>
       </c>
@@ -3294,7 +3292,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>86</v>
       </c>
@@ -3302,7 +3300,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>87</v>
       </c>
@@ -3310,7 +3308,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>282</v>
       </c>
@@ -3318,7 +3316,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>88</v>
       </c>
@@ -3326,7 +3324,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>222</v>
       </c>
@@ -3334,7 +3332,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>277</v>
       </c>
@@ -3342,7 +3340,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>89</v>
       </c>
@@ -3350,7 +3348,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>90</v>
       </c>
@@ -3358,7 +3356,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>91</v>
       </c>
@@ -3366,7 +3364,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>223</v>
       </c>
@@ -3374,7 +3372,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>168</v>
       </c>
@@ -3382,7 +3380,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>154</v>
       </c>
@@ -3390,7 +3388,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>193</v>
       </c>
@@ -3398,7 +3396,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>209</v>
       </c>
@@ -3406,7 +3404,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>116</v>
       </c>
@@ -3414,7 +3412,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>92</v>
       </c>
@@ -3422,7 +3420,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>155</v>
       </c>
@@ -3430,7 +3428,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>156</v>
       </c>
@@ -3438,7 +3436,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>93</v>
       </c>
@@ -3446,7 +3444,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>252</v>
       </c>
@@ -3454,7 +3452,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>128</v>
       </c>
@@ -3462,7 +3460,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>256</v>
       </c>
@@ -3470,7 +3468,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>163</v>
       </c>
@@ -3478,7 +3476,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>157</v>
       </c>
@@ -3486,7 +3484,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>253</v>
       </c>
@@ -3494,7 +3492,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>94</v>
       </c>
@@ -3502,7 +3500,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>194</v>
       </c>
@@ -3510,7 +3508,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>95</v>
       </c>
@@ -3518,7 +3516,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>224</v>
       </c>
@@ -3526,7 +3524,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>96</v>
       </c>
@@ -3534,7 +3532,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>97</v>
       </c>
@@ -3542,7 +3540,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>98</v>
       </c>
@@ -3550,7 +3548,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>99</v>
       </c>
@@ -3558,7 +3556,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>185</v>
       </c>
@@ -3566,7 +3564,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>158</v>
       </c>

</xml_diff>

<commit_message>
Updated data for care (v66)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E21ED12-FC90-478F-A162-412CB692DA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CD2481-A03F-488B-B04F-43A3185762FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13310" yWindow="4070" windowWidth="24370" windowHeight="15370" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="6870" yWindow="620" windowWidth="28800" windowHeight="19890" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="301">
   <si>
     <t>Status inleveren routekaart</t>
   </si>
@@ -868,9 +868,6 @@
     <t>Ananz wonen-welzijn-zorg (sint anna zorggroep)</t>
   </si>
   <si>
-    <t>De Lichtenvoorde (Sius) (Stichting)</t>
-  </si>
-  <si>
     <t>Lunet (Stichting)</t>
   </si>
   <si>
@@ -914,6 +911,27 @@
   </si>
   <si>
     <t xml:space="preserve">Zorggroep Zaanstreek (Stichting) </t>
+  </si>
+  <si>
+    <t>De Posten (Stichting)</t>
+  </si>
+  <si>
+    <t>De Waalboog, Zorg, Welzijn en Wonen (Stichting)</t>
+  </si>
+  <si>
+    <t>PZC Dordrecht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sius </t>
+  </si>
+  <si>
+    <t>Sjaloom Zorg (Stichting)</t>
+  </si>
+  <si>
+    <t>Sprank (Stichting)</t>
+  </si>
+  <si>
+    <t>Zorgverlening Het Baken (Stichting)</t>
   </si>
 </sst>
 </file>
@@ -1281,11 +1299,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B292"/>
+  <dimension ref="A1:B298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1562,7 +1578,7 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -1578,7 +1594,7 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -1594,7 +1610,7 @@
         <v>132</v>
       </c>
       <c r="B38" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -1602,7 +1618,7 @@
         <v>175</v>
       </c>
       <c r="B39" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1610,7 +1626,7 @@
         <v>133</v>
       </c>
       <c r="B40" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -1642,7 +1658,7 @@
         <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1658,7 +1674,7 @@
         <v>259</v>
       </c>
       <c r="B46" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -1666,7 +1682,7 @@
         <v>169</v>
       </c>
       <c r="B47" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -1674,7 +1690,7 @@
         <v>170</v>
       </c>
       <c r="B48" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -1703,7 +1719,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="B52" t="s">
         <v>210</v>
@@ -1711,7 +1727,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="B53" t="s">
         <v>209</v>
@@ -1719,7 +1735,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>176</v>
+        <v>282</v>
       </c>
       <c r="B54" t="s">
         <v>210</v>
@@ -1727,7 +1743,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>134</v>
+        <v>176</v>
       </c>
       <c r="B55" t="s">
         <v>209</v>
@@ -1735,7 +1751,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>212</v>
+        <v>134</v>
       </c>
       <c r="B56" t="s">
         <v>210</v>
@@ -1743,7 +1759,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="B57" t="s">
         <v>210</v>
@@ -1751,15 +1767,15 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>21</v>
+        <v>235</v>
       </c>
       <c r="B58" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="B59" t="s">
         <v>209</v>
@@ -1767,7 +1783,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>236</v>
+        <v>110</v>
       </c>
       <c r="B60" t="s">
         <v>210</v>
@@ -1775,15 +1791,15 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>284</v>
+        <v>236</v>
       </c>
       <c r="B61" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>22</v>
+        <v>283</v>
       </c>
       <c r="B62" t="s">
         <v>210</v>
@@ -1791,7 +1807,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>213</v>
+        <v>22</v>
       </c>
       <c r="B63" t="s">
         <v>210</v>
@@ -1799,7 +1815,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>213</v>
       </c>
       <c r="B64" t="s">
         <v>210</v>
@@ -1807,23 +1823,23 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B65" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B66" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="B67" t="s">
         <v>210</v>
@@ -1831,15 +1847,15 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="B68" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>26</v>
+        <v>284</v>
       </c>
       <c r="B69" t="s">
         <v>209</v>
@@ -1847,15 +1863,15 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>238</v>
+        <v>26</v>
       </c>
       <c r="B70" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>27</v>
+        <v>238</v>
       </c>
       <c r="B71" t="s">
         <v>210</v>
@@ -1863,7 +1879,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>286</v>
+        <v>27</v>
       </c>
       <c r="B72" t="s">
         <v>210</v>
@@ -1871,7 +1887,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>285</v>
       </c>
       <c r="B73" t="s">
         <v>210</v>
@@ -1879,15 +1895,15 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>214</v>
+        <v>135</v>
       </c>
       <c r="B74" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>267</v>
+        <v>214</v>
       </c>
       <c r="B75" t="s">
         <v>209</v>
@@ -1895,7 +1911,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>161</v>
+        <v>267</v>
       </c>
       <c r="B76" t="s">
         <v>209</v>
@@ -1903,31 +1919,31 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>289</v>
+        <v>161</v>
       </c>
       <c r="B77" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>260</v>
+        <v>288</v>
       </c>
       <c r="B78" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B79" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>28</v>
+        <v>261</v>
       </c>
       <c r="B80" t="s">
         <v>210</v>
@@ -1935,31 +1951,31 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B81" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>239</v>
+        <v>29</v>
       </c>
       <c r="B82" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>30</v>
+        <v>239</v>
       </c>
       <c r="B83" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="B84" t="s">
         <v>209</v>
@@ -1967,7 +1983,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="B85" t="s">
         <v>209</v>
@@ -1975,63 +1991,63 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>240</v>
+        <v>31</v>
       </c>
       <c r="B86" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>290</v>
+        <v>240</v>
       </c>
       <c r="B87" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>241</v>
+        <v>289</v>
       </c>
       <c r="B88" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>32</v>
+        <v>241</v>
       </c>
       <c r="B89" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>262</v>
+        <v>32</v>
       </c>
       <c r="B90" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B91" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="B92" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
       <c r="B93" t="s">
         <v>209</v>
@@ -2039,15 +2055,15 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>136</v>
+        <v>268</v>
       </c>
       <c r="B94" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="B95" t="s">
         <v>209</v>
@@ -2055,23 +2071,23 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>137</v>
+        <v>33</v>
       </c>
       <c r="B96" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>201</v>
+        <v>137</v>
       </c>
       <c r="B97" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="B98" t="s">
         <v>210</v>
@@ -2079,15 +2095,15 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>186</v>
+        <v>34</v>
       </c>
       <c r="B99" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="B100" t="s">
         <v>210</v>
@@ -2095,15 +2111,15 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="B101" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
       <c r="B102" t="s">
         <v>210</v>
@@ -2111,15 +2127,15 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>291</v>
+        <v>224</v>
       </c>
       <c r="B103" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="B104" t="s">
         <v>210</v>
@@ -2127,7 +2143,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>35</v>
+        <v>269</v>
       </c>
       <c r="B105" t="s">
         <v>210</v>
@@ -2135,23 +2151,23 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>287</v>
+        <v>35</v>
       </c>
       <c r="B106" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="B107" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>36</v>
+        <v>257</v>
       </c>
       <c r="B108" t="s">
         <v>209</v>
@@ -2159,7 +2175,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>292</v>
+        <v>36</v>
       </c>
       <c r="B109" t="s">
         <v>209</v>
@@ -2167,7 +2183,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>138</v>
+        <v>291</v>
       </c>
       <c r="B110" t="s">
         <v>209</v>
@@ -2175,7 +2191,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>225</v>
+        <v>138</v>
       </c>
       <c r="B111" t="s">
         <v>209</v>
@@ -2183,7 +2199,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="B112" t="s">
         <v>209</v>
@@ -2191,15 +2207,15 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>125</v>
+        <v>196</v>
       </c>
       <c r="B113" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="B114" t="s">
         <v>209</v>
@@ -2207,7 +2223,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>226</v>
+        <v>37</v>
       </c>
       <c r="B115" t="s">
         <v>210</v>
@@ -2215,15 +2231,15 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>38</v>
+        <v>226</v>
       </c>
       <c r="B116" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>187</v>
+        <v>38</v>
       </c>
       <c r="B117" t="s">
         <v>210</v>
@@ -2231,31 +2247,31 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>39</v>
+        <v>187</v>
       </c>
       <c r="B118" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="B119" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>139</v>
+        <v>188</v>
       </c>
       <c r="B120" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="B121" t="s">
         <v>209</v>
@@ -2263,7 +2279,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>203</v>
+        <v>40</v>
       </c>
       <c r="B122" t="s">
         <v>210</v>
@@ -2271,7 +2287,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>167</v>
+        <v>203</v>
       </c>
       <c r="B123" t="s">
         <v>210</v>
@@ -2279,15 +2295,15 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="B124" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>243</v>
+        <v>41</v>
       </c>
       <c r="B125" t="s">
         <v>210</v>
@@ -2295,31 +2311,31 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>42</v>
+        <v>243</v>
       </c>
       <c r="B126" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>177</v>
+        <v>42</v>
       </c>
       <c r="B127" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>227</v>
+        <v>177</v>
       </c>
       <c r="B128" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>258</v>
+        <v>227</v>
       </c>
       <c r="B129" t="s">
         <v>209</v>
@@ -2327,15 +2343,15 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>100</v>
+        <v>258</v>
       </c>
       <c r="B130" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="B131" t="s">
         <v>209</v>
@@ -2343,7 +2359,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>204</v>
+        <v>140</v>
       </c>
       <c r="B132" t="s">
         <v>209</v>
@@ -2351,7 +2367,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>293</v>
+        <v>204</v>
       </c>
       <c r="B133" t="s">
         <v>209</v>
@@ -2359,15 +2375,15 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>43</v>
+        <v>292</v>
       </c>
       <c r="B134" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B135" t="s">
         <v>210</v>
@@ -2375,15 +2391,15 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>162</v>
+        <v>44</v>
       </c>
       <c r="B136" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>244</v>
+        <v>162</v>
       </c>
       <c r="B137" t="s">
         <v>210</v>
@@ -2391,23 +2407,23 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="B138" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>280</v>
+        <v>228</v>
       </c>
       <c r="B139" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
       <c r="B140" t="s">
         <v>209</v>
@@ -2415,15 +2431,15 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B141" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>178</v>
+        <v>46</v>
       </c>
       <c r="B142" t="s">
         <v>210</v>
@@ -2431,7 +2447,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>263</v>
+        <v>178</v>
       </c>
       <c r="B143" t="s">
         <v>210</v>
@@ -2439,31 +2455,31 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>111</v>
+        <v>263</v>
       </c>
       <c r="B144" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="B145" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B146" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>112</v>
+        <v>48</v>
       </c>
       <c r="B147" t="s">
         <v>210</v>
@@ -2471,7 +2487,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>215</v>
+        <v>112</v>
       </c>
       <c r="B148" t="s">
         <v>210</v>
@@ -2479,7 +2495,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>49</v>
+        <v>215</v>
       </c>
       <c r="B149" t="s">
         <v>210</v>
@@ -2487,7 +2503,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B150" t="s">
         <v>210</v>
@@ -2495,15 +2511,15 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B151" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B152" t="s">
         <v>210</v>
@@ -2511,7 +2527,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>245</v>
+        <v>52</v>
       </c>
       <c r="B153" t="s">
         <v>210</v>
@@ -2519,7 +2535,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B154" t="s">
         <v>210</v>
@@ -2527,7 +2543,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="B155" t="s">
         <v>210</v>
@@ -2535,15 +2551,15 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>53</v>
+        <v>246</v>
       </c>
       <c r="B156" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>197</v>
+        <v>53</v>
       </c>
       <c r="B157" t="s">
         <v>210</v>
@@ -2551,7 +2567,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>141</v>
+        <v>197</v>
       </c>
       <c r="B158" t="s">
         <v>210</v>
@@ -2559,23 +2575,23 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>288</v>
+        <v>141</v>
       </c>
       <c r="B159" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>198</v>
+        <v>287</v>
       </c>
       <c r="B160" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>142</v>
+        <v>198</v>
       </c>
       <c r="B161" t="s">
         <v>209</v>
@@ -2583,7 +2599,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>54</v>
+        <v>142</v>
       </c>
       <c r="B162" t="s">
         <v>209</v>
@@ -2591,7 +2607,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B163" t="s">
         <v>209</v>
@@ -2599,7 +2615,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B164" t="s">
         <v>209</v>
@@ -2607,23 +2623,23 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
       <c r="B165" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>264</v>
+        <v>143</v>
       </c>
       <c r="B166" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>57</v>
+        <v>264</v>
       </c>
       <c r="B167" t="s">
         <v>210</v>
@@ -2631,7 +2647,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>105</v>
+        <v>57</v>
       </c>
       <c r="B168" t="s">
         <v>210</v>
@@ -2639,39 +2655,39 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B169" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B170" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B171" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B172" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="B173" t="s">
         <v>210</v>
@@ -2679,7 +2695,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="B174" t="s">
         <v>209</v>
@@ -2687,7 +2703,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="B175" t="s">
         <v>210</v>
@@ -2695,31 +2711,31 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>179</v>
+        <v>61</v>
       </c>
       <c r="B176" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>62</v>
+        <v>179</v>
       </c>
       <c r="B177" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>270</v>
+        <v>62</v>
       </c>
       <c r="B178" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>113</v>
+        <v>270</v>
       </c>
       <c r="B179" t="s">
         <v>209</v>
@@ -2727,23 +2743,23 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>114</v>
+        <v>296</v>
       </c>
       <c r="B180" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="B181" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>205</v>
+        <v>114</v>
       </c>
       <c r="B182" t="s">
         <v>209</v>
@@ -2751,7 +2767,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="B183" t="s">
         <v>210</v>
@@ -2759,23 +2775,23 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>118</v>
+        <v>205</v>
       </c>
       <c r="B184" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>216</v>
+        <v>107</v>
       </c>
       <c r="B185" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>271</v>
+        <v>118</v>
       </c>
       <c r="B186" t="s">
         <v>210</v>
@@ -2783,7 +2799,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="B187" t="s">
         <v>209</v>
@@ -2791,15 +2807,15 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>206</v>
+        <v>271</v>
       </c>
       <c r="B188" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>180</v>
+        <v>229</v>
       </c>
       <c r="B189" t="s">
         <v>209</v>
@@ -2807,63 +2823,63 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>63</v>
+        <v>206</v>
       </c>
       <c r="B190" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>230</v>
+        <v>180</v>
       </c>
       <c r="B191" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="B192" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B193" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="B194" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B195" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B196" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>217</v>
+        <v>247</v>
       </c>
       <c r="B197" t="s">
         <v>210</v>
@@ -2871,15 +2887,15 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>218</v>
+        <v>65</v>
       </c>
       <c r="B198" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
       <c r="B199" t="s">
         <v>210</v>
@@ -2887,7 +2903,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>66</v>
+        <v>218</v>
       </c>
       <c r="B200" t="s">
         <v>210</v>
@@ -2895,47 +2911,47 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="B201" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>189</v>
+        <v>66</v>
       </c>
       <c r="B202" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>115</v>
+        <v>232</v>
       </c>
       <c r="B203" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>67</v>
+        <v>189</v>
       </c>
       <c r="B204" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B205" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>272</v>
+        <v>67</v>
       </c>
       <c r="B206" t="s">
         <v>209</v>
@@ -2943,7 +2959,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B207" t="s">
         <v>209</v>
@@ -2951,23 +2967,23 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>68</v>
+        <v>272</v>
       </c>
       <c r="B208" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>207</v>
+        <v>122</v>
       </c>
       <c r="B209" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B210" t="s">
         <v>210</v>
@@ -2975,7 +2991,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>102</v>
+        <v>207</v>
       </c>
       <c r="B211" t="s">
         <v>210</v>
@@ -2983,7 +2999,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>70</v>
+        <v>297</v>
       </c>
       <c r="B212" t="s">
         <v>210</v>
@@ -2991,7 +3007,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>147</v>
+        <v>69</v>
       </c>
       <c r="B213" t="s">
         <v>210</v>
@@ -2999,23 +3015,23 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="B214" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="B215" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>149</v>
+        <v>70</v>
       </c>
       <c r="B216" t="s">
         <v>209</v>
@@ -3023,23 +3039,23 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>254</v>
+        <v>299</v>
       </c>
       <c r="B217" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="B218" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>190</v>
+        <v>281</v>
       </c>
       <c r="B219" t="s">
         <v>209</v>
@@ -3047,7 +3063,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>71</v>
+        <v>148</v>
       </c>
       <c r="B220" t="s">
         <v>210</v>
@@ -3055,7 +3071,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>72</v>
+        <v>149</v>
       </c>
       <c r="B221" t="s">
         <v>209</v>
@@ -3063,15 +3079,15 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>173</v>
+        <v>254</v>
       </c>
       <c r="B222" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="223" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A223" s="2" t="s">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="B223" t="s">
         <v>210</v>
@@ -3079,39 +3095,39 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="B224" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B225" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B226" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="B227" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B228" t="s">
         <v>210</v>
@@ -3119,23 +3135,23 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="B229" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>249</v>
+        <v>74</v>
       </c>
       <c r="B230" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>275</v>
+        <v>75</v>
       </c>
       <c r="B231" t="s">
         <v>210</v>
@@ -3143,23 +3159,23 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>77</v>
+        <v>151</v>
       </c>
       <c r="B232" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>277</v>
+        <v>76</v>
       </c>
       <c r="B233" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="B234" t="s">
         <v>210</v>
@@ -3167,23 +3183,23 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>101</v>
+        <v>249</v>
       </c>
       <c r="B235" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>79</v>
+        <v>275</v>
       </c>
       <c r="B236" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B237" t="s">
         <v>210</v>
@@ -3191,23 +3207,23 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>81</v>
+        <v>277</v>
       </c>
       <c r="B238" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>219</v>
+        <v>78</v>
       </c>
       <c r="B239" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>250</v>
+        <v>101</v>
       </c>
       <c r="B240" t="s">
         <v>210</v>
@@ -3215,15 +3231,15 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>265</v>
+        <v>79</v>
       </c>
       <c r="B241" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>159</v>
+        <v>80</v>
       </c>
       <c r="B242" t="s">
         <v>210</v>
@@ -3231,15 +3247,15 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="B243" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>152</v>
+        <v>219</v>
       </c>
       <c r="B244" t="s">
         <v>210</v>
@@ -3247,15 +3263,15 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>82</v>
+        <v>250</v>
       </c>
       <c r="B245" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>83</v>
+        <v>265</v>
       </c>
       <c r="B246" t="s">
         <v>210</v>
@@ -3263,15 +3279,15 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>274</v>
+        <v>159</v>
       </c>
       <c r="B247" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="B248" t="s">
         <v>210</v>
@@ -3279,23 +3295,23 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="B249" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>183</v>
+        <v>82</v>
       </c>
       <c r="B250" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>220</v>
+        <v>83</v>
       </c>
       <c r="B251" t="s">
         <v>209</v>
@@ -3303,7 +3319,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>84</v>
+        <v>274</v>
       </c>
       <c r="B252" t="s">
         <v>209</v>
@@ -3311,15 +3327,15 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>199</v>
+        <v>153</v>
       </c>
       <c r="B253" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B254" t="s">
         <v>209</v>
@@ -3327,23 +3343,23 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>108</v>
+        <v>183</v>
       </c>
       <c r="B255" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>85</v>
+        <v>220</v>
       </c>
       <c r="B256" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B257" t="s">
         <v>209</v>
@@ -3351,31 +3367,31 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>87</v>
+        <v>199</v>
       </c>
       <c r="B258" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>281</v>
+        <v>191</v>
       </c>
       <c r="B259" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="B260" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>221</v>
+        <v>85</v>
       </c>
       <c r="B261" t="s">
         <v>209</v>
@@ -3383,7 +3399,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>276</v>
+        <v>86</v>
       </c>
       <c r="B262" t="s">
         <v>209</v>
@@ -3391,31 +3407,31 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B263" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>90</v>
+        <v>280</v>
       </c>
       <c r="B264" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B265" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B266" t="s">
         <v>210</v>
@@ -3423,7 +3439,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>168</v>
+        <v>276</v>
       </c>
       <c r="B267" t="s">
         <v>209</v>
@@ -3431,7 +3447,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="B268" t="s">
         <v>210</v>
@@ -3439,39 +3455,39 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>192</v>
+        <v>90</v>
       </c>
       <c r="B269" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>208</v>
+        <v>91</v>
       </c>
       <c r="B270" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>116</v>
+        <v>222</v>
       </c>
       <c r="B271" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>92</v>
+        <v>168</v>
       </c>
       <c r="B272" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B273" t="s">
         <v>210</v>
@@ -3479,15 +3495,15 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>156</v>
+        <v>192</v>
       </c>
       <c r="B274" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>93</v>
+        <v>208</v>
       </c>
       <c r="B275" t="s">
         <v>210</v>
@@ -3495,39 +3511,39 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>251</v>
+        <v>116</v>
       </c>
       <c r="B276" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="B277" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>255</v>
+        <v>155</v>
       </c>
       <c r="B278" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B279" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
       <c r="B280" t="s">
         <v>210</v>
@@ -3535,15 +3551,15 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B281" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="B282" t="s">
         <v>210</v>
@@ -3551,31 +3567,31 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>193</v>
+        <v>255</v>
       </c>
       <c r="B283" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>294</v>
+        <v>163</v>
       </c>
       <c r="B284" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
       <c r="B285" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>223</v>
+        <v>252</v>
       </c>
       <c r="B286" t="s">
         <v>209</v>
@@ -3583,49 +3599,97 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B287" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>97</v>
+        <v>193</v>
       </c>
       <c r="B288" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>98</v>
+        <v>293</v>
       </c>
       <c r="B289" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B290" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
       <c r="B291" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
+        <v>96</v>
+      </c>
+      <c r="B292" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A293" t="s">
+        <v>97</v>
+      </c>
+      <c r="B293" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A294" t="s">
+        <v>300</v>
+      </c>
+      <c r="B294" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A295" t="s">
+        <v>98</v>
+      </c>
+      <c r="B295" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A296" t="s">
+        <v>99</v>
+      </c>
+      <c r="B296" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A297" t="s">
+        <v>184</v>
+      </c>
+      <c r="B297" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A298" t="s">
         <v>158</v>
       </c>
-      <c r="B292" t="s">
+      <c r="B298" t="s">
         <v>210</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrections to care data (v66b)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CD2481-A03F-488B-B04F-43A3185762FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C85B744-28D3-49E5-97BC-9371E4A97BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6870" yWindow="620" windowWidth="28800" windowHeight="19890" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="20325" yWindow="2790" windowWidth="30060" windowHeight="15225" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1301,15 +1301,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
   <dimension ref="A1:B298"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="A289" sqref="A289"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1317,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -1325,7 +1327,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1333,7 +1335,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1341,7 +1343,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>200</v>
       </c>
@@ -1349,7 +1351,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>160</v>
       </c>
@@ -1357,7 +1359,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -1365,7 +1367,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1373,7 +1375,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -1381,7 +1383,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1389,7 +1391,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1397,7 +1399,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>233</v>
       </c>
@@ -1405,7 +1407,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>129</v>
       </c>
@@ -1413,7 +1415,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>172</v>
       </c>
@@ -1421,7 +1423,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>278</v>
       </c>
@@ -1429,7 +1431,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1437,7 +1439,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>130</v>
       </c>
@@ -1445,7 +1447,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>185</v>
       </c>
@@ -1453,7 +1455,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1461,7 +1463,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1469,7 +1471,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1477,7 +1479,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1485,7 +1487,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>234</v>
       </c>
@@ -1493,7 +1495,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1501,7 +1503,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1509,7 +1511,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>266</v>
       </c>
@@ -1517,7 +1519,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>131</v>
       </c>
@@ -1525,7 +1527,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>194</v>
       </c>
@@ -1533,7 +1535,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1541,7 +1543,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -1549,7 +1551,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -1557,7 +1559,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>165</v>
       </c>
@@ -1565,7 +1567,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>273</v>
       </c>
@@ -1573,7 +1575,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -1581,7 +1583,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>174</v>
       </c>
@@ -1589,7 +1591,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1597,7 +1599,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1605,7 +1607,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>132</v>
       </c>
@@ -1613,7 +1615,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>175</v>
       </c>
@@ -1621,7 +1623,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>133</v>
       </c>
@@ -1629,7 +1631,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -1637,7 +1639,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -1645,7 +1647,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>120</v>
       </c>
@@ -1653,7 +1655,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>117</v>
       </c>
@@ -1661,7 +1663,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -1669,7 +1671,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>259</v>
       </c>
@@ -1677,7 +1679,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>169</v>
       </c>
@@ -1685,7 +1687,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>170</v>
       </c>
@@ -1693,7 +1695,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>109</v>
       </c>
@@ -1701,7 +1703,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>211</v>
       </c>
@@ -1709,7 +1711,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>195</v>
       </c>
@@ -1717,7 +1719,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>294</v>
       </c>
@@ -1725,7 +1727,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>295</v>
       </c>
@@ -1733,7 +1735,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>282</v>
       </c>
@@ -1741,7 +1743,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>176</v>
       </c>
@@ -1749,7 +1751,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -1757,7 +1759,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>212</v>
       </c>
@@ -1765,7 +1767,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>235</v>
       </c>
@@ -1773,7 +1775,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>21</v>
       </c>
@@ -1781,7 +1783,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>110</v>
       </c>
@@ -1789,7 +1791,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>236</v>
       </c>
@@ -1797,7 +1799,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>283</v>
       </c>
@@ -1805,7 +1807,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -1813,7 +1815,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>213</v>
       </c>
@@ -1821,7 +1823,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>23</v>
       </c>
@@ -1829,7 +1831,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>24</v>
       </c>
@@ -1837,7 +1839,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>25</v>
       </c>
@@ -1845,7 +1847,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>237</v>
       </c>
@@ -1853,7 +1855,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>284</v>
       </c>
@@ -1861,7 +1863,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>26</v>
       </c>
@@ -1869,7 +1871,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>238</v>
       </c>
@@ -1877,7 +1879,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>27</v>
       </c>
@@ -1885,7 +1887,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>285</v>
       </c>
@@ -1893,7 +1895,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>135</v>
       </c>
@@ -1901,7 +1903,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>214</v>
       </c>
@@ -1909,7 +1911,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>267</v>
       </c>
@@ -1917,7 +1919,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>161</v>
       </c>
@@ -1925,7 +1927,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>288</v>
       </c>
@@ -1933,7 +1935,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>260</v>
       </c>
@@ -1941,7 +1943,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>261</v>
       </c>
@@ -1949,7 +1951,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>28</v>
       </c>
@@ -1957,7 +1959,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>29</v>
       </c>
@@ -1965,7 +1967,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>239</v>
       </c>
@@ -1973,7 +1975,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>30</v>
       </c>
@@ -1981,7 +1983,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>121</v>
       </c>
@@ -1989,7 +1991,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>31</v>
       </c>
@@ -1997,7 +1999,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>240</v>
       </c>
@@ -2005,7 +2007,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>289</v>
       </c>
@@ -2013,7 +2015,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>241</v>
       </c>
@@ -2021,7 +2023,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>32</v>
       </c>
@@ -2029,7 +2031,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>262</v>
       </c>
@@ -2037,7 +2039,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>256</v>
       </c>
@@ -2045,7 +2047,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>242</v>
       </c>
@@ -2053,7 +2055,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>268</v>
       </c>
@@ -2061,7 +2063,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>136</v>
       </c>
@@ -2069,7 +2071,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>33</v>
       </c>
@@ -2077,7 +2079,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>137</v>
       </c>
@@ -2085,7 +2087,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>201</v>
       </c>
@@ -2093,7 +2095,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>34</v>
       </c>
@@ -2101,7 +2103,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>186</v>
       </c>
@@ -2109,7 +2111,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>166</v>
       </c>
@@ -2117,7 +2119,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>202</v>
       </c>
@@ -2125,7 +2127,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>224</v>
       </c>
@@ -2133,7 +2135,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>290</v>
       </c>
@@ -2141,7 +2143,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>269</v>
       </c>
@@ -2149,7 +2151,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>35</v>
       </c>
@@ -2157,7 +2159,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>286</v>
       </c>
@@ -2165,7 +2167,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>257</v>
       </c>
@@ -2173,7 +2175,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>36</v>
       </c>
@@ -2181,7 +2183,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>291</v>
       </c>
@@ -2189,7 +2191,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>138</v>
       </c>
@@ -2197,7 +2199,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>225</v>
       </c>
@@ -2205,7 +2207,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>196</v>
       </c>
@@ -2213,7 +2215,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>125</v>
       </c>
@@ -2221,7 +2223,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>37</v>
       </c>
@@ -2229,7 +2231,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>226</v>
       </c>
@@ -2237,7 +2239,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>38</v>
       </c>
@@ -2245,7 +2247,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>187</v>
       </c>
@@ -2253,7 +2255,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>39</v>
       </c>
@@ -2261,7 +2263,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>188</v>
       </c>
@@ -2269,7 +2271,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>139</v>
       </c>
@@ -2277,7 +2279,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>40</v>
       </c>
@@ -2285,7 +2287,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>203</v>
       </c>
@@ -2293,7 +2295,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>167</v>
       </c>
@@ -2301,7 +2303,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>41</v>
       </c>
@@ -2309,7 +2311,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>243</v>
       </c>
@@ -2317,7 +2319,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>42</v>
       </c>
@@ -2325,7 +2327,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>177</v>
       </c>
@@ -2333,7 +2335,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>227</v>
       </c>
@@ -2341,7 +2343,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>258</v>
       </c>
@@ -2349,7 +2351,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>100</v>
       </c>
@@ -2357,7 +2359,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>140</v>
       </c>
@@ -2365,7 +2367,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>204</v>
       </c>
@@ -2373,7 +2375,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>292</v>
       </c>
@@ -2381,7 +2383,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>43</v>
       </c>
@@ -2389,7 +2391,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>44</v>
       </c>
@@ -2397,7 +2399,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>162</v>
       </c>
@@ -2405,7 +2407,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>244</v>
       </c>
@@ -2413,7 +2415,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>228</v>
       </c>
@@ -2421,7 +2423,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>279</v>
       </c>
@@ -2429,7 +2431,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>45</v>
       </c>
@@ -2437,7 +2439,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>46</v>
       </c>
@@ -2445,7 +2447,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>178</v>
       </c>
@@ -2453,7 +2455,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>263</v>
       </c>
@@ -2461,7 +2463,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>111</v>
       </c>
@@ -2469,7 +2471,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>47</v>
       </c>
@@ -2477,7 +2479,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>48</v>
       </c>
@@ -2485,7 +2487,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>112</v>
       </c>
@@ -2493,7 +2495,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>215</v>
       </c>
@@ -2501,7 +2503,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>49</v>
       </c>
@@ -2509,7 +2511,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>50</v>
       </c>
@@ -2517,7 +2519,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>51</v>
       </c>
@@ -2525,7 +2527,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>52</v>
       </c>
@@ -2533,7 +2535,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>245</v>
       </c>
@@ -2541,7 +2543,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>253</v>
       </c>
@@ -2549,7 +2551,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>246</v>
       </c>
@@ -2557,7 +2559,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>53</v>
       </c>
@@ -2565,7 +2567,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>197</v>
       </c>
@@ -2573,7 +2575,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>141</v>
       </c>
@@ -2581,7 +2583,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>287</v>
       </c>
@@ -2589,7 +2591,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>198</v>
       </c>
@@ -2597,7 +2599,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>142</v>
       </c>
@@ -2605,7 +2607,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>54</v>
       </c>
@@ -2613,7 +2615,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>55</v>
       </c>
@@ -2621,7 +2623,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>56</v>
       </c>
@@ -2629,7 +2631,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>143</v>
       </c>
@@ -2637,7 +2639,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>264</v>
       </c>
@@ -2645,7 +2647,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>57</v>
       </c>
@@ -2653,7 +2655,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>105</v>
       </c>
@@ -2661,7 +2663,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>106</v>
       </c>
@@ -2669,7 +2671,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>58</v>
       </c>
@@ -2677,7 +2679,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>59</v>
       </c>
@@ -2685,7 +2687,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>60</v>
       </c>
@@ -2693,7 +2695,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>144</v>
       </c>
@@ -2701,7 +2703,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>126</v>
       </c>
@@ -2709,7 +2711,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>61</v>
       </c>
@@ -2717,7 +2719,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>179</v>
       </c>
@@ -2725,7 +2727,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>62</v>
       </c>
@@ -2733,7 +2735,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>270</v>
       </c>
@@ -2741,7 +2743,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>296</v>
       </c>
@@ -2749,7 +2751,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>113</v>
       </c>
@@ -2757,7 +2759,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>114</v>
       </c>
@@ -2765,7 +2767,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>145</v>
       </c>
@@ -2773,7 +2775,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>205</v>
       </c>
@@ -2781,7 +2783,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>107</v>
       </c>
@@ -2789,7 +2791,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>118</v>
       </c>
@@ -2797,7 +2799,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>216</v>
       </c>
@@ -2805,7 +2807,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>271</v>
       </c>
@@ -2813,7 +2815,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>229</v>
       </c>
@@ -2821,7 +2823,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>206</v>
       </c>
@@ -2829,7 +2831,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>180</v>
       </c>
@@ -2837,7 +2839,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>63</v>
       </c>
@@ -2845,7 +2847,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>230</v>
       </c>
@@ -2853,7 +2855,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>146</v>
       </c>
@@ -2861,7 +2863,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>231</v>
       </c>
@@ -2869,7 +2871,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>64</v>
       </c>
@@ -2877,7 +2879,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>247</v>
       </c>
@@ -2885,7 +2887,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>65</v>
       </c>
@@ -2893,7 +2895,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>217</v>
       </c>
@@ -2901,7 +2903,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>218</v>
       </c>
@@ -2909,7 +2911,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>248</v>
       </c>
@@ -2917,7 +2919,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>66</v>
       </c>
@@ -2925,7 +2927,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>232</v>
       </c>
@@ -2933,7 +2935,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>189</v>
       </c>
@@ -2941,7 +2943,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>115</v>
       </c>
@@ -2949,7 +2951,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>67</v>
       </c>
@@ -2957,7 +2959,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>119</v>
       </c>
@@ -2965,7 +2967,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>272</v>
       </c>
@@ -2973,7 +2975,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>122</v>
       </c>
@@ -2981,7 +2983,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>68</v>
       </c>
@@ -2989,7 +2991,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>207</v>
       </c>
@@ -2997,15 +2999,15 @@
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>297</v>
       </c>
       <c r="B212" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>69</v>
       </c>
@@ -3013,7 +3015,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>298</v>
       </c>
@@ -3021,7 +3023,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>102</v>
       </c>
@@ -3029,7 +3031,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>70</v>
       </c>
@@ -3037,7 +3039,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>299</v>
       </c>
@@ -3045,7 +3047,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>147</v>
       </c>
@@ -3053,7 +3055,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>281</v>
       </c>
@@ -3061,7 +3063,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>148</v>
       </c>
@@ -3069,7 +3071,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>149</v>
       </c>
@@ -3077,7 +3079,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>254</v>
       </c>
@@ -3085,7 +3087,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="223" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>171</v>
       </c>
@@ -3093,7 +3095,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>190</v>
       </c>
@@ -3101,7 +3103,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>71</v>
       </c>
@@ -3109,7 +3111,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>72</v>
       </c>
@@ -3117,7 +3119,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>173</v>
       </c>
@@ -3125,7 +3127,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>73</v>
       </c>
@@ -3133,7 +3135,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>150</v>
       </c>
@@ -3141,7 +3143,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>74</v>
       </c>
@@ -3149,7 +3151,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>75</v>
       </c>
@@ -3157,7 +3159,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>151</v>
       </c>
@@ -3165,7 +3167,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>76</v>
       </c>
@@ -3173,7 +3175,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>181</v>
       </c>
@@ -3181,7 +3183,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>249</v>
       </c>
@@ -3189,7 +3191,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>275</v>
       </c>
@@ -3197,7 +3199,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>77</v>
       </c>
@@ -3205,7 +3207,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>277</v>
       </c>
@@ -3213,7 +3215,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>78</v>
       </c>
@@ -3221,7 +3223,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>101</v>
       </c>
@@ -3229,7 +3231,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>79</v>
       </c>
@@ -3237,7 +3239,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>80</v>
       </c>
@@ -3245,7 +3247,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>81</v>
       </c>
@@ -3253,7 +3255,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>219</v>
       </c>
@@ -3261,7 +3263,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>250</v>
       </c>
@@ -3269,7 +3271,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>265</v>
       </c>
@@ -3277,7 +3279,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>159</v>
       </c>
@@ -3285,7 +3287,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>127</v>
       </c>
@@ -3293,7 +3295,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>152</v>
       </c>
@@ -3301,15 +3303,15 @@
         <v>210</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>82</v>
       </c>
       <c r="B250" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>83</v>
       </c>
@@ -3317,7 +3319,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>274</v>
       </c>
@@ -3325,7 +3327,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>153</v>
       </c>
@@ -3333,7 +3335,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>182</v>
       </c>
@@ -3341,7 +3343,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>183</v>
       </c>
@@ -3349,7 +3351,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>220</v>
       </c>
@@ -3357,7 +3359,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>84</v>
       </c>
@@ -3365,7 +3367,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>199</v>
       </c>
@@ -3373,7 +3375,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>191</v>
       </c>
@@ -3381,7 +3383,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>108</v>
       </c>
@@ -3389,7 +3391,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>85</v>
       </c>
@@ -3397,7 +3399,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>86</v>
       </c>
@@ -3405,7 +3407,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>87</v>
       </c>
@@ -3413,7 +3415,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>280</v>
       </c>
@@ -3421,7 +3423,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>88</v>
       </c>
@@ -3429,7 +3431,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>221</v>
       </c>
@@ -3437,7 +3439,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>276</v>
       </c>
@@ -3445,7 +3447,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>89</v>
       </c>
@@ -3453,7 +3455,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>90</v>
       </c>
@@ -3461,7 +3463,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>91</v>
       </c>
@@ -3469,7 +3471,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>222</v>
       </c>
@@ -3477,7 +3479,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>168</v>
       </c>
@@ -3485,7 +3487,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>154</v>
       </c>
@@ -3493,7 +3495,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>192</v>
       </c>
@@ -3501,7 +3503,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>208</v>
       </c>
@@ -3509,7 +3511,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>116</v>
       </c>
@@ -3517,7 +3519,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>92</v>
       </c>
@@ -3525,7 +3527,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>155</v>
       </c>
@@ -3533,7 +3535,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>156</v>
       </c>
@@ -3541,7 +3543,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>93</v>
       </c>
@@ -3549,7 +3551,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>251</v>
       </c>
@@ -3557,7 +3559,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>128</v>
       </c>
@@ -3565,7 +3567,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>255</v>
       </c>
@@ -3573,7 +3575,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>163</v>
       </c>
@@ -3581,7 +3583,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>157</v>
       </c>
@@ -3589,7 +3591,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>252</v>
       </c>
@@ -3597,7 +3599,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>94</v>
       </c>
@@ -3605,7 +3607,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>193</v>
       </c>
@@ -3613,15 +3615,15 @@
         <v>209</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>293</v>
       </c>
       <c r="B289" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>95</v>
       </c>
@@ -3629,7 +3631,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>223</v>
       </c>
@@ -3637,7 +3639,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>96</v>
       </c>
@@ -3645,7 +3647,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>97</v>
       </c>
@@ -3653,7 +3655,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>300</v>
       </c>
@@ -3661,7 +3663,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>98</v>
       </c>
@@ -3669,7 +3671,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>99</v>
       </c>
@@ -3677,7 +3679,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>184</v>
       </c>
@@ -3685,7 +3687,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>158</v>
       </c>

</xml_diff>

<commit_message>
Fixed status for Zorggroep Ena
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E7C28F-036C-46A7-9CFC-FBE8260F5ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4EAA13-5C40-4E2E-B91E-309C8E00CF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4510" yWindow="3520" windowWidth="32790" windowHeight="15370" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="710" yWindow="2050" windowWidth="17860" windowHeight="18590" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3579,7 +3579,7 @@
         <v>91</v>
       </c>
       <c r="B283" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated data vor Visio
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_care.xlsx
+++ b/src/data/routekaart_status_care.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4EAA13-5C40-4E2E-B91E-309C8E00CF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7495FF-D3E3-41E8-894E-5E391C8DB02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="710" yWindow="2050" windowWidth="17860" windowHeight="18590" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="4940" yWindow="4940" windowWidth="28800" windowHeight="15370" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1310,7 +1310,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2323,7 +2325,7 @@
         <v>136</v>
       </c>
       <c r="B126" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>